<commit_message>
add gc log debug, slides about gitops
</commit_message>
<xml_diff>
--- a/kafka_benchmark/benchmark_stats.xlsx
+++ b/kafka_benchmark/benchmark_stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lijjin/Documents/work/git_ws/redistest/kafka_benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{96B56142-EB63-0842-AD39-AB7B83F21A2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDA4634-1F77-8A41-9A25-71099C1F2B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{35590E01-C7C5-464A-8FB5-DBB7ECFA3BB7}"/>
   </bookViews>
@@ -20,7 +20,7 @@
     <sheet name="600 executor" sheetId="3" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Kafka Producer'!$A$1:$AB$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Kafka Producer'!$A$1:$AD$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2502" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2601" uniqueCount="245">
   <si>
     <t>Partition</t>
   </si>
@@ -731,13 +731,61 @@
   <si>
     <t>k8s_2ng_2j_3b_3p_2r_28800t_600e</t>
   </si>
+  <si>
+    <t>MariaDB</t>
+  </si>
+  <si>
+    <t>Hikari ConnectionPool Size</t>
+  </si>
+  <si>
+    <t>8.7K</t>
+  </si>
+  <si>
+    <t>7K</t>
+  </si>
+  <si>
+    <t>mariadb_k8s_2ng_2j_3b_3p_2r_28800t_600e</t>
+  </si>
+  <si>
+    <t>mariadb_k8s_2ng_2j_3b_3p_2r_24000t_600e</t>
+  </si>
+  <si>
+    <t>mariadb_k8s_2ng_2j_3b_3p_2r_19600t_600e</t>
+  </si>
+  <si>
+    <t>6.9K</t>
+  </si>
+  <si>
+    <t>mariadb_k8s_2ng_2j_3b_3p_2r_14400t_600e</t>
+  </si>
+  <si>
+    <t>7.8K</t>
+  </si>
+  <si>
+    <t>mariadb_k8s_2ng_2j_3b_3p_2r_9600t_600e</t>
+  </si>
+  <si>
+    <t>9.9K</t>
+  </si>
+  <si>
+    <t>mariadb_k8s_2ng_2j_3b_3p_2r_4800t_600e</t>
+  </si>
+  <si>
+    <t>mariadb_k8s_2ng_2j_3b_3p_2r_24000t_600e_6cpu</t>
+  </si>
+  <si>
+    <t>mariadb_k8s_2ng_2j_3b_3p_2r_9600t_600e_6cpu</t>
+  </si>
+  <si>
+    <t>mariadb_k8s_2ng_2j_3b_3p_2r_4800t_600e_6cpu</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="173" formatCode="0.0000000%"/>
+    <numFmt numFmtId="164" formatCode="0.0000000%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -808,7 +856,7 @@
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="173" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -1127,36 +1175,40 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60B9A07-2A84-A84C-9DF8-25F7D96E359D}">
-  <dimension ref="A1:AB44"/>
+  <dimension ref="A1:AD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="N40" sqref="N40"/>
+    <sheetView tabSelected="1" topLeftCell="M38" workbookViewId="0">
+      <selection activeCell="P53" sqref="P53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
-    <col min="5" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="8" width="23.5" customWidth="1"/>
+    <col min="5" max="5" width="13.1640625" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="12.83203125" customWidth="1"/>
+    <col min="8" max="8" width="14.5" customWidth="1"/>
     <col min="9" max="9" width="15.83203125" customWidth="1"/>
-    <col min="10" max="10" width="13.5" customWidth="1"/>
+    <col min="10" max="10" width="11.83203125" customWidth="1"/>
     <col min="11" max="11" width="9.1640625" customWidth="1"/>
     <col min="12" max="12" width="13.5" customWidth="1"/>
     <col min="13" max="13" width="16.33203125" customWidth="1"/>
-    <col min="14" max="14" width="15" customWidth="1"/>
-    <col min="15" max="16" width="21.1640625" customWidth="1"/>
-    <col min="17" max="17" width="24.5" customWidth="1"/>
-    <col min="18" max="19" width="21.1640625" customWidth="1"/>
-    <col min="20" max="20" width="14.6640625" customWidth="1"/>
-    <col min="21" max="22" width="11.33203125" customWidth="1"/>
-    <col min="23" max="23" width="18" customWidth="1"/>
-    <col min="24" max="24" width="20" customWidth="1"/>
-    <col min="25" max="26" width="17.33203125" customWidth="1"/>
-    <col min="27" max="27" width="37.6640625" customWidth="1"/>
-    <col min="28" max="28" width="31.6640625" customWidth="1"/>
+    <col min="14" max="14" width="9.1640625" customWidth="1"/>
+    <col min="15" max="15" width="13.33203125" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="18" width="21.1640625" customWidth="1"/>
+    <col min="19" max="19" width="24.5" customWidth="1"/>
+    <col min="20" max="21" width="21.1640625" customWidth="1"/>
+    <col min="22" max="22" width="14.6640625" customWidth="1"/>
+    <col min="23" max="24" width="11.33203125" customWidth="1"/>
+    <col min="25" max="25" width="18" customWidth="1"/>
+    <col min="26" max="26" width="20" customWidth="1"/>
+    <col min="27" max="28" width="17.33203125" customWidth="1"/>
+    <col min="29" max="29" width="37.6640625" customWidth="1"/>
+    <col min="30" max="30" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1197,52 +1249,58 @@
         <v>184</v>
       </c>
       <c r="N1" t="s">
+        <v>229</v>
+      </c>
+      <c r="O1" t="s">
+        <v>230</v>
+      </c>
+      <c r="P1" t="s">
         <v>129</v>
       </c>
-      <c r="O1" t="s">
+      <c r="Q1" t="s">
         <v>134</v>
       </c>
-      <c r="P1" t="s">
+      <c r="R1" t="s">
         <v>135</v>
       </c>
-      <c r="Q1" s="3" t="s">
+      <c r="S1" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="R1" s="3" t="s">
+      <c r="T1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="S1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="V1" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="W1" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="V1" s="3" t="s">
+      <c r="X1" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="W1" t="s">
+      <c r="Y1" t="s">
         <v>132</v>
       </c>
-      <c r="X1" t="s">
+      <c r="Z1" t="s">
         <v>131</v>
       </c>
-      <c r="Y1" t="s">
+      <c r="AA1" t="s">
         <v>5</v>
       </c>
-      <c r="Z1" t="s">
+      <c r="AB1" t="s">
         <v>6</v>
       </c>
-      <c r="AA1" t="s">
+      <c r="AC1" t="s">
         <v>7</v>
       </c>
-      <c r="AB1" t="s">
+      <c r="AD1" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1273,39 +1331,42 @@
       <c r="M2" t="s">
         <v>185</v>
       </c>
-      <c r="N2">
+      <c r="N2" t="s">
+        <v>167</v>
+      </c>
+      <c r="P2">
         <v>9334.57</v>
       </c>
-      <c r="O2">
+      <c r="Q2">
         <v>439.11</v>
       </c>
-      <c r="P2">
+      <c r="R2">
         <v>9176</v>
       </c>
-      <c r="Q2">
+      <c r="S2">
         <v>15</v>
       </c>
-      <c r="R2">
+      <c r="T2">
         <v>20</v>
       </c>
-      <c r="S2">
+      <c r="U2">
         <v>22</v>
       </c>
-      <c r="W2">
+      <c r="Y2">
         <v>6221133</v>
       </c>
-      <c r="Y2">
-        <f>X2/W2</f>
+      <c r="AA2">
+        <f>Z2/Y2</f>
         <v>0</v>
       </c>
-      <c r="Z2" t="s">
+      <c r="AB2" t="s">
         <v>127</v>
       </c>
-      <c r="AA2" s="1" t="s">
+      <c r="AC2" s="1" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1336,42 +1397,45 @@
       <c r="M3" t="s">
         <v>185</v>
       </c>
-      <c r="N3">
+      <c r="N3" t="s">
+        <v>167</v>
+      </c>
+      <c r="P3">
         <v>10080.200000000001</v>
       </c>
-      <c r="O3">
+      <c r="Q3">
         <v>561.70000000000005</v>
       </c>
-      <c r="P3">
+      <c r="R3">
         <v>6371</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>3</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>7</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>9</v>
       </c>
-      <c r="W3">
+      <c r="Y3">
         <v>7047871</v>
       </c>
-      <c r="X3">
+      <c r="Z3">
         <v>1603686474</v>
       </c>
-      <c r="Y3">
-        <f>X3/W3</f>
+      <c r="AA3">
+        <f>Z3/Y3</f>
         <v>227.54197317175641</v>
       </c>
-      <c r="Z3" t="s">
+      <c r="AB3" t="s">
         <v>145</v>
       </c>
-      <c r="AA3" s="1" t="s">
+      <c r="AC3" s="1" t="s">
         <v>144</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1402,36 +1466,39 @@
       <c r="M4" t="s">
         <v>185</v>
       </c>
-      <c r="N4">
+      <c r="N4" t="s">
+        <v>167</v>
+      </c>
+      <c r="P4">
         <v>13909.52</v>
       </c>
-      <c r="O4">
+      <c r="Q4">
         <v>163.09</v>
       </c>
-      <c r="P4">
+      <c r="R4">
         <v>14405</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>3</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>10</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>14</v>
       </c>
-      <c r="W4">
+      <c r="Y4">
         <v>8908295</v>
       </c>
-      <c r="Y4">
-        <f t="shared" ref="Y4:Y18" si="0">X4/W4</f>
+      <c r="AA4">
+        <f t="shared" ref="AA4:AA17" si="0">Z4/Y4</f>
         <v>0</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AC4" s="1" t="s">
         <v>139</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1462,39 +1529,42 @@
       <c r="M5" t="s">
         <v>185</v>
       </c>
-      <c r="N5">
+      <c r="N5" t="s">
+        <v>167</v>
+      </c>
+      <c r="P5">
         <v>17379.650000000001</v>
       </c>
-      <c r="O5">
+      <c r="Q5">
         <v>245.08</v>
       </c>
-      <c r="P5">
+      <c r="R5">
         <v>2781</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>6</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>14</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>15</v>
       </c>
-      <c r="W5">
+      <c r="Y5">
         <v>5530727</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="Z5" t="s">
+      <c r="AB5" t="s">
         <v>17</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AC5" s="1" t="s">
         <v>146</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1525,36 +1595,39 @@
       <c r="M6" t="s">
         <v>185</v>
       </c>
-      <c r="N6">
+      <c r="N6" t="s">
+        <v>167</v>
+      </c>
+      <c r="P6">
         <v>18007.71</v>
       </c>
-      <c r="O6">
+      <c r="Q6">
         <v>116.95</v>
       </c>
-      <c r="P6">
+      <c r="R6">
         <v>5638</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>3</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>11</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>17</v>
       </c>
-      <c r="W6">
+      <c r="Y6">
         <v>5608986</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AC6" s="1" t="s">
         <v>140</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1585,36 +1658,39 @@
       <c r="M7" t="s">
         <v>185</v>
       </c>
-      <c r="N7">
+      <c r="N7" t="s">
+        <v>167</v>
+      </c>
+      <c r="P7">
         <v>20483.23</v>
       </c>
-      <c r="O7">
+      <c r="Q7">
         <v>51.68</v>
       </c>
-      <c r="P7">
+      <c r="R7">
         <v>1218</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>8</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>24</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>46</v>
       </c>
-      <c r="W7">
+      <c r="Y7">
         <v>6581814</v>
       </c>
-      <c r="Y7">
+      <c r="AA7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AC7" s="1" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1645,36 +1721,39 @@
       <c r="M8" t="s">
         <v>185</v>
       </c>
-      <c r="N8">
+      <c r="N8" t="s">
+        <v>167</v>
+      </c>
+      <c r="P8">
         <v>19699.2</v>
       </c>
-      <c r="O8">
+      <c r="Q8">
         <v>30.03</v>
       </c>
-      <c r="P8">
+      <c r="R8">
         <v>2036</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>13</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>28</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>48.99</v>
       </c>
-      <c r="W8">
+      <c r="Y8">
         <v>5928927</v>
       </c>
-      <c r="Y8">
+      <c r="AA8">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AC8" s="1" t="s">
         <v>142</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1705,36 +1784,39 @@
       <c r="M9" t="s">
         <v>185</v>
       </c>
-      <c r="N9">
+      <c r="N9" t="s">
+        <v>167</v>
+      </c>
+      <c r="P9">
         <v>19646.96</v>
       </c>
-      <c r="O9">
+      <c r="Q9">
         <v>14.76</v>
       </c>
-      <c r="P9">
+      <c r="R9">
         <v>1069</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>5</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>18</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>32</v>
       </c>
-      <c r="W9">
+      <c r="Y9">
         <v>5909098</v>
       </c>
-      <c r="Y9">
+      <c r="AA9">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA9" s="1" t="s">
+      <c r="AC9" s="1" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1765,36 +1847,39 @@
       <c r="M10" t="s">
         <v>185</v>
       </c>
-      <c r="N10">
+      <c r="N10" t="s">
+        <v>167</v>
+      </c>
+      <c r="P10">
         <v>11055.79</v>
       </c>
-      <c r="O10">
+      <c r="Q10">
         <v>362.88</v>
       </c>
-      <c r="P10">
+      <c r="R10">
         <v>8045</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>12</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <v>32</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>148</v>
       </c>
-      <c r="W10">
+      <c r="Y10">
         <v>7606150</v>
       </c>
-      <c r="Y10">
+      <c r="AA10">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA10" s="1" t="s">
+      <c r="AC10" s="1" t="s">
         <v>147</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1825,36 +1910,39 @@
       <c r="M11" t="s">
         <v>185</v>
       </c>
-      <c r="N11">
+      <c r="N11" t="s">
+        <v>167</v>
+      </c>
+      <c r="P11">
         <v>11355.91</v>
       </c>
-      <c r="O11">
+      <c r="Q11">
         <v>558.54</v>
       </c>
-      <c r="P11">
+      <c r="R11">
         <v>17347</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>23</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <v>41</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>111</v>
       </c>
-      <c r="W11">
+      <c r="Y11">
         <v>7377526</v>
       </c>
-      <c r="Y11">
+      <c r="AA11">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AC11" s="1" t="s">
         <v>151</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1885,36 +1973,39 @@
       <c r="M12" t="s">
         <v>185</v>
       </c>
-      <c r="N12">
+      <c r="N12" t="s">
+        <v>167</v>
+      </c>
+      <c r="P12">
         <v>14650.31</v>
       </c>
-      <c r="O12">
+      <c r="Q12">
         <v>179.67</v>
       </c>
-      <c r="P12">
+      <c r="R12">
         <v>19621</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>7</v>
       </c>
-      <c r="R12">
+      <c r="T12">
         <v>18</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <v>31</v>
       </c>
-      <c r="W12">
+      <c r="Y12">
         <v>9497239</v>
       </c>
-      <c r="Y12">
+      <c r="AA12">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA12" s="1" t="s">
+      <c r="AC12" s="1" t="s">
         <v>150</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -1945,36 +2036,39 @@
       <c r="M13" t="s">
         <v>185</v>
       </c>
-      <c r="N13">
+      <c r="N13" t="s">
+        <v>167</v>
+      </c>
+      <c r="P13">
         <v>17087.25</v>
       </c>
-      <c r="O13">
+      <c r="Q13">
         <v>133.91999999999999</v>
       </c>
-      <c r="P13">
+      <c r="R13">
         <v>7574</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <v>76</v>
       </c>
-      <c r="R13">
+      <c r="T13">
         <v>186</v>
       </c>
-      <c r="S13">
+      <c r="U13">
         <v>237</v>
       </c>
-      <c r="W13">
+      <c r="Y13">
         <v>5896333</v>
       </c>
-      <c r="Y13">
+      <c r="AA13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA13" s="1" t="s">
+      <c r="AC13" s="1" t="s">
         <v>148</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2005,36 +2099,39 @@
       <c r="M14" t="s">
         <v>185</v>
       </c>
-      <c r="N14">
+      <c r="N14" t="s">
+        <v>167</v>
+      </c>
+      <c r="P14">
         <v>18978.52</v>
       </c>
-      <c r="O14">
+      <c r="Q14">
         <v>86.32</v>
       </c>
-      <c r="P14">
+      <c r="R14">
         <v>3711</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>23</v>
       </c>
-      <c r="R14">
+      <c r="T14">
         <v>54</v>
       </c>
-      <c r="S14">
+      <c r="U14">
         <v>87</v>
       </c>
-      <c r="W14">
+      <c r="Y14">
         <v>6842516</v>
       </c>
-      <c r="Y14">
+      <c r="AA14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA14" s="1" t="s">
+      <c r="AC14" s="1" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2065,36 +2162,39 @@
       <c r="M15" t="s">
         <v>185</v>
       </c>
-      <c r="N15">
+      <c r="N15" t="s">
+        <v>167</v>
+      </c>
+      <c r="P15">
         <v>19052.41</v>
       </c>
-      <c r="O15">
+      <c r="Q15">
         <v>52.48</v>
       </c>
-      <c r="P15">
+      <c r="R15">
         <v>3189</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <v>3</v>
       </c>
-      <c r="R15">
+      <c r="T15">
         <v>7</v>
       </c>
-      <c r="S15">
+      <c r="U15">
         <v>13</v>
       </c>
-      <c r="W15">
+      <c r="Y15">
         <v>6280209</v>
       </c>
-      <c r="Y15">
+      <c r="AA15">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA15" s="1" t="s">
+      <c r="AC15" s="1" t="s">
         <v>152</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2125,36 +2225,39 @@
       <c r="M16" t="s">
         <v>185</v>
       </c>
-      <c r="N16">
+      <c r="N16" t="s">
+        <v>167</v>
+      </c>
+      <c r="P16">
         <v>20711.09</v>
       </c>
-      <c r="O16">
+      <c r="Q16">
         <v>27.48</v>
       </c>
-      <c r="P16">
+      <c r="R16">
         <v>2006</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>4</v>
       </c>
-      <c r="R16">
+      <c r="T16">
         <v>8</v>
       </c>
-      <c r="S16">
+      <c r="U16">
         <v>16</v>
       </c>
-      <c r="W16">
+      <c r="Y16">
         <v>6370420</v>
       </c>
-      <c r="Y16">
+      <c r="AA16">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA16" s="1" t="s">
+      <c r="AC16" s="1" t="s">
         <v>153</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>1</v>
       </c>
@@ -2185,36 +2288,39 @@
       <c r="M17" t="s">
         <v>185</v>
       </c>
-      <c r="N17">
+      <c r="N17" t="s">
+        <v>167</v>
+      </c>
+      <c r="P17">
         <v>19420.349999999999</v>
       </c>
-      <c r="O17">
+      <c r="Q17">
         <v>14.95</v>
       </c>
-      <c r="P17">
+      <c r="R17">
         <v>971</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>8</v>
       </c>
-      <c r="R17">
+      <c r="T17">
         <v>21</v>
       </c>
-      <c r="S17">
+      <c r="U17">
         <v>40</v>
       </c>
-      <c r="W17">
+      <c r="Y17">
         <v>5839137</v>
       </c>
-      <c r="Y17">
+      <c r="AA17">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA17" s="1" t="s">
+      <c r="AC17" s="1" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>3</v>
       </c>
@@ -2245,45 +2351,48 @@
       <c r="M18" t="s">
         <v>185</v>
       </c>
-      <c r="N18">
+      <c r="N18" t="s">
+        <v>167</v>
+      </c>
+      <c r="P18">
         <v>26652.22</v>
       </c>
-      <c r="O18">
+      <c r="Q18">
         <v>230.82</v>
       </c>
-      <c r="P18">
+      <c r="R18">
         <v>82528</v>
       </c>
-      <c r="Q18">
+      <c r="S18">
         <v>12</v>
       </c>
-      <c r="R18">
+      <c r="T18">
         <v>17</v>
       </c>
-      <c r="S18">
+      <c r="U18">
         <v>19</v>
       </c>
-      <c r="T18">
+      <c r="V18">
         <v>19336001</v>
       </c>
-      <c r="W18">
+      <c r="Y18">
         <v>18978145</v>
       </c>
-      <c r="X18">
+      <c r="Z18">
         <v>4359632902</v>
       </c>
-      <c r="Y18">
-        <f>X18/W18</f>
+      <c r="AA18">
+        <f>Z18/Y18</f>
         <v>229.71860010554246</v>
       </c>
-      <c r="Z18" t="s">
+      <c r="AB18" t="s">
         <v>155</v>
       </c>
-      <c r="AA18" s="1" t="s">
+      <c r="AC18" s="1" t="s">
         <v>156</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A19">
         <v>3</v>
       </c>
@@ -2314,45 +2423,48 @@
       <c r="M19" t="s">
         <v>185</v>
       </c>
-      <c r="N19">
+      <c r="N19" t="s">
+        <v>167</v>
+      </c>
+      <c r="P19">
         <v>20440.21</v>
       </c>
-      <c r="O19">
+      <c r="Q19">
         <v>137.83000000000001</v>
       </c>
-      <c r="P19">
+      <c r="R19">
         <v>15340</v>
       </c>
-      <c r="Q19">
+      <c r="S19">
         <v>20</v>
       </c>
-      <c r="R19">
+      <c r="T19">
         <v>43</v>
       </c>
-      <c r="S19">
+      <c r="U19">
         <v>166</v>
       </c>
-      <c r="T19">
+      <c r="V19">
         <v>14869949</v>
       </c>
-      <c r="W19">
+      <c r="Y19">
         <v>14869949</v>
       </c>
-      <c r="X19">
+      <c r="Z19">
         <v>4064366090</v>
       </c>
-      <c r="Y19">
-        <f>X19/W19</f>
+      <c r="AA19">
+        <f>Z19/Y19</f>
         <v>273.32750704121446</v>
       </c>
-      <c r="Z19" t="s">
+      <c r="AB19" t="s">
         <v>24</v>
       </c>
-      <c r="AA19" s="1" t="s">
+      <c r="AC19" s="1" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>3</v>
       </c>
@@ -2383,45 +2495,48 @@
       <c r="M20" t="s">
         <v>185</v>
       </c>
-      <c r="N20">
+      <c r="N20" t="s">
+        <v>167</v>
+      </c>
+      <c r="P20">
         <v>35637.03</v>
       </c>
-      <c r="O20">
+      <c r="Q20">
         <v>33.6</v>
       </c>
-      <c r="P20">
+      <c r="R20">
         <v>26562</v>
       </c>
-      <c r="Q20">
+      <c r="S20">
         <v>3</v>
       </c>
-      <c r="R20">
+      <c r="T20">
         <v>5</v>
       </c>
-      <c r="S20">
+      <c r="U20">
         <v>9</v>
       </c>
-      <c r="T20">
+      <c r="V20">
         <v>24242803</v>
       </c>
-      <c r="W20">
+      <c r="Y20">
         <v>24242803</v>
       </c>
-      <c r="X20">
+      <c r="Z20">
         <v>5607835436</v>
       </c>
-      <c r="Y20">
-        <f>X20/W20</f>
+      <c r="AA20">
+        <f>Z20/Y20</f>
         <v>231.31959765543613</v>
       </c>
-      <c r="Z20" t="s">
+      <c r="AB20" t="s">
         <v>162</v>
       </c>
-      <c r="AA20" s="1" t="s">
+      <c r="AC20" s="1" t="s">
         <v>163</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>3</v>
       </c>
@@ -2452,45 +2567,48 @@
       <c r="M21" t="s">
         <v>185</v>
       </c>
-      <c r="N21">
+      <c r="N21" t="s">
+        <v>167</v>
+      </c>
+      <c r="P21">
         <v>34071.14</v>
       </c>
-      <c r="O21">
+      <c r="Q21">
         <v>47.77</v>
       </c>
-      <c r="P21">
+      <c r="R21">
         <v>25615</v>
       </c>
-      <c r="Q21">
+      <c r="S21">
         <v>7</v>
       </c>
-      <c r="R21">
+      <c r="T21">
         <v>17</v>
       </c>
-      <c r="S21">
+      <c r="U21">
         <v>68</v>
       </c>
-      <c r="T21">
+      <c r="V21">
         <v>23089978</v>
       </c>
-      <c r="W21">
+      <c r="Y21">
         <v>23089978</v>
       </c>
-      <c r="X21">
+      <c r="Z21">
         <v>5063269190</v>
       </c>
-      <c r="Y21">
-        <f>X21/W21</f>
+      <c r="AA21">
+        <f>Z21/Y21</f>
         <v>219.28427952594845</v>
       </c>
-      <c r="Z21" t="s">
+      <c r="AB21" t="s">
         <v>155</v>
       </c>
-      <c r="AA21" s="1" t="s">
+      <c r="AC21" s="1" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -2527,49 +2645,52 @@
       <c r="M22" t="s">
         <v>186</v>
       </c>
-      <c r="N22">
+      <c r="N22" t="s">
+        <v>167</v>
+      </c>
+      <c r="P22">
         <v>14533.74</v>
       </c>
-      <c r="O22">
+      <c r="Q22">
         <v>313.93</v>
       </c>
-      <c r="P22">
+      <c r="R22">
         <v>12285</v>
       </c>
-      <c r="Q22">
+      <c r="S22">
         <v>21</v>
       </c>
-      <c r="R22">
+      <c r="T22">
         <v>61</v>
       </c>
-      <c r="S22">
+      <c r="U22">
         <v>83</v>
       </c>
-      <c r="T22">
+      <c r="V22">
         <v>8869478</v>
       </c>
-      <c r="U22">
+      <c r="W22">
         <v>1</v>
       </c>
-      <c r="V22" s="5">
-        <f>U22/T22</f>
+      <c r="X22" s="5">
+        <f>W22/V22</f>
         <v>1.1274620671024834E-7</v>
       </c>
-      <c r="W22">
+      <c r="Y22">
         <v>8868946</v>
       </c>
-      <c r="X22">
+      <c r="Z22">
         <v>1896080941</v>
       </c>
-      <c r="Y22">
-        <f>X22/W22</f>
+      <c r="AA22">
+        <f>Z22/Y22</f>
         <v>213.78875697292554</v>
       </c>
-      <c r="AA22" s="1" t="s">
+      <c r="AC22" s="1" t="s">
         <v>187</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -2606,49 +2727,52 @@
       <c r="M23" t="s">
         <v>186</v>
       </c>
-      <c r="N23">
+      <c r="N23" t="s">
+        <v>167</v>
+      </c>
+      <c r="P23">
         <v>6827.13</v>
       </c>
-      <c r="O23">
+      <c r="Q23">
         <v>793.3</v>
       </c>
-      <c r="P23">
+      <c r="R23">
         <v>115733</v>
       </c>
-      <c r="Q23">
+      <c r="S23">
         <v>6</v>
       </c>
-      <c r="R23">
+      <c r="T23">
         <v>18</v>
       </c>
-      <c r="S23">
+      <c r="U23">
         <v>26</v>
       </c>
-      <c r="T23">
+      <c r="V23">
         <v>4691491</v>
       </c>
-      <c r="U23">
+      <c r="W23">
         <v>7</v>
       </c>
-      <c r="V23" s="5">
-        <f t="shared" ref="V23:V44" si="1">U23/T23</f>
+      <c r="X23" s="5">
+        <f t="shared" ref="X23:X50" si="1">W23/V23</f>
         <v>1.4920629710256292E-6</v>
       </c>
-      <c r="W23">
+      <c r="Y23">
         <v>4691484</v>
       </c>
-      <c r="X23">
+      <c r="Z23">
         <v>1007059300</v>
       </c>
-      <c r="Y23">
-        <f t="shared" ref="Y22:Y31" si="2">X23/W23</f>
+      <c r="AA23">
+        <f t="shared" ref="AA23:AA30" si="2">Z23/Y23</f>
         <v>214.65687616114644</v>
       </c>
-      <c r="AA23" s="1" t="s">
+      <c r="AC23" s="1" t="s">
         <v>189</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -2685,52 +2809,55 @@
       <c r="M24" t="s">
         <v>186</v>
       </c>
-      <c r="N24">
+      <c r="N24" t="s">
+        <v>167</v>
+      </c>
+      <c r="P24">
         <v>7300.05</v>
       </c>
-      <c r="O24">
+      <c r="Q24">
         <v>964.97</v>
       </c>
-      <c r="P24">
+      <c r="R24">
         <v>203594</v>
       </c>
-      <c r="Q24">
+      <c r="S24">
         <v>44</v>
       </c>
-      <c r="R24">
+      <c r="T24">
         <v>112</v>
       </c>
-      <c r="S24">
+      <c r="U24">
         <v>351.99</v>
       </c>
-      <c r="T24">
+      <c r="V24">
         <v>5196681</v>
       </c>
-      <c r="U24">
+      <c r="W24">
         <v>46</v>
       </c>
-      <c r="V24" s="5">
+      <c r="X24" s="5">
         <f t="shared" si="1"/>
         <v>8.8518036800796502E-6</v>
       </c>
-      <c r="W24">
+      <c r="Y24">
         <v>5196637</v>
       </c>
-      <c r="X24">
+      <c r="Z24">
         <v>1116916192</v>
       </c>
-      <c r="Y24">
+      <c r="AA24">
         <f t="shared" si="2"/>
         <v>214.93057760239941</v>
       </c>
-      <c r="Z24" t="s">
+      <c r="AB24" t="s">
         <v>13</v>
       </c>
-      <c r="AA24" s="1" t="s">
+      <c r="AC24" s="1" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>2</v>
       </c>
@@ -2767,52 +2894,55 @@
       <c r="M25" t="s">
         <v>186</v>
       </c>
-      <c r="N25">
+      <c r="N25" t="s">
+        <v>167</v>
+      </c>
+      <c r="P25">
         <v>20680</v>
       </c>
-      <c r="O25">
+      <c r="Q25">
         <v>210.51</v>
       </c>
-      <c r="P25">
+      <c r="R25">
         <v>60229</v>
       </c>
-      <c r="Q25">
+      <c r="S25">
         <v>26</v>
       </c>
-      <c r="R25">
+      <c r="T25">
         <v>55</v>
       </c>
-      <c r="S25">
+      <c r="U25">
         <v>276</v>
       </c>
-      <c r="T25">
+      <c r="V25">
         <v>13000421</v>
       </c>
-      <c r="U25">
+      <c r="W25">
         <v>3</v>
       </c>
-      <c r="V25" s="5">
+      <c r="X25" s="5">
         <f t="shared" si="1"/>
         <v>2.3076175763846416E-7</v>
       </c>
-      <c r="W25">
+      <c r="Y25">
         <v>13000418</v>
       </c>
-      <c r="X25">
+      <c r="Z25">
         <v>2960238429</v>
       </c>
-      <c r="Y25">
+      <c r="AA25">
         <f t="shared" si="2"/>
         <v>227.70332684687523</v>
       </c>
-      <c r="Z25" t="s">
+      <c r="AB25" t="s">
         <v>158</v>
       </c>
-      <c r="AA25" s="1" t="s">
+      <c r="AC25" s="1" t="s">
         <v>191</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>2</v>
       </c>
@@ -2849,52 +2979,55 @@
       <c r="M26" t="s">
         <v>186</v>
       </c>
-      <c r="N26">
+      <c r="N26" t="s">
+        <v>167</v>
+      </c>
+      <c r="P26">
         <v>10154.18</v>
       </c>
-      <c r="O26">
+      <c r="Q26">
         <v>546.79</v>
       </c>
-      <c r="P26">
+      <c r="R26">
         <v>119842</v>
       </c>
-      <c r="Q26">
+      <c r="S26">
         <v>29</v>
       </c>
-      <c r="R26">
+      <c r="T26">
         <v>50</v>
       </c>
-      <c r="S26">
+      <c r="U26">
         <v>91</v>
       </c>
-      <c r="T26">
+      <c r="V26">
         <v>6481597</v>
       </c>
-      <c r="U26">
+      <c r="W26">
         <v>22</v>
       </c>
-      <c r="V26" s="5">
+      <c r="X26" s="5">
         <f t="shared" si="1"/>
         <v>3.3942252194945166E-6</v>
       </c>
-      <c r="W26">
+      <c r="Y26">
         <v>6481575</v>
       </c>
-      <c r="X26">
+      <c r="Z26">
         <v>1453396003</v>
       </c>
-      <c r="Y26">
+      <c r="AA26">
         <f t="shared" si="2"/>
         <v>224.23500507206967</v>
       </c>
-      <c r="Z26" t="s">
+      <c r="AB26" t="s">
         <v>145</v>
       </c>
-      <c r="AA26" s="1" t="s">
+      <c r="AC26" s="1" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>2</v>
       </c>
@@ -2931,52 +3064,55 @@
       <c r="M27" t="s">
         <v>186</v>
       </c>
-      <c r="N27">
+      <c r="N27" t="s">
+        <v>167</v>
+      </c>
+      <c r="P27">
         <v>8503.75</v>
       </c>
-      <c r="O27">
+      <c r="Q27">
         <v>623.32000000000005</v>
       </c>
-      <c r="P27">
+      <c r="R27">
         <v>213233</v>
       </c>
-      <c r="Q27">
+      <c r="S27">
         <v>15</v>
       </c>
-      <c r="R27">
+      <c r="T27">
         <v>33</v>
       </c>
-      <c r="S27">
+      <c r="U27">
         <v>261</v>
       </c>
-      <c r="T27">
+      <c r="V27">
         <v>5864453</v>
       </c>
-      <c r="U27">
+      <c r="W27">
         <v>44</v>
       </c>
-      <c r="V27" s="5">
+      <c r="X27" s="5">
         <f t="shared" si="1"/>
         <v>7.50283103982588E-6</v>
       </c>
-      <c r="W27">
+      <c r="Y27">
         <v>5864409</v>
       </c>
-      <c r="X27">
+      <c r="Z27">
         <v>1330856806</v>
       </c>
-      <c r="Y27">
+      <c r="AA27">
         <f t="shared" si="2"/>
         <v>226.93792435009223</v>
       </c>
-      <c r="Z27" t="s">
+      <c r="AB27" t="s">
         <v>195</v>
       </c>
-      <c r="AA27" s="1" t="s">
+      <c r="AC27" s="1" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>2</v>
       </c>
@@ -3016,52 +3152,55 @@
       <c r="M28" t="s">
         <v>186</v>
       </c>
-      <c r="N28">
+      <c r="N28" t="s">
+        <v>167</v>
+      </c>
+      <c r="P28">
         <v>7938.43</v>
       </c>
-      <c r="O28">
+      <c r="Q28">
         <v>591.41999999999996</v>
       </c>
-      <c r="P28">
+      <c r="R28">
         <v>6741</v>
       </c>
-      <c r="Q28">
+      <c r="S28">
         <v>217</v>
       </c>
-      <c r="R28">
+      <c r="T28">
         <v>482</v>
       </c>
-      <c r="S28">
+      <c r="U28">
         <v>601</v>
       </c>
-      <c r="T28">
+      <c r="V28">
         <v>4807900</v>
       </c>
-      <c r="U28">
+      <c r="W28">
         <v>0</v>
       </c>
-      <c r="V28" s="5">
+      <c r="X28" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W28">
+      <c r="Y28">
         <v>4807900</v>
       </c>
-      <c r="X28">
+      <c r="Z28">
         <v>1168595347</v>
       </c>
-      <c r="Y28">
+      <c r="AA28">
         <f t="shared" si="2"/>
         <v>243.0573320992533</v>
       </c>
-      <c r="Z28" t="s">
+      <c r="AB28" t="s">
         <v>199</v>
       </c>
-      <c r="AA28" s="1" t="s">
+      <c r="AC28" s="1" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>2</v>
       </c>
@@ -3101,52 +3240,55 @@
       <c r="M29" t="s">
         <v>186</v>
       </c>
-      <c r="N29">
+      <c r="N29" t="s">
+        <v>167</v>
+      </c>
+      <c r="P29">
         <v>3873.38</v>
       </c>
-      <c r="O29">
+      <c r="Q29">
         <v>1991.02</v>
       </c>
-      <c r="P29">
+      <c r="R29">
         <v>62988</v>
       </c>
-      <c r="Q29">
+      <c r="S29">
         <v>748</v>
       </c>
-      <c r="R29">
+      <c r="T29">
         <v>2504</v>
       </c>
-      <c r="S29">
+      <c r="U29">
         <v>3155.99</v>
       </c>
-      <c r="T29">
+      <c r="V29">
         <v>2367093</v>
       </c>
-      <c r="U29">
+      <c r="W29">
         <v>1</v>
       </c>
-      <c r="V29" s="5">
+      <c r="X29" s="5">
         <f t="shared" si="1"/>
         <v>4.2245910912667985E-7</v>
       </c>
-      <c r="W29">
+      <c r="Y29">
         <v>2367092</v>
       </c>
-      <c r="X29">
+      <c r="Z29">
         <v>550427270</v>
       </c>
-      <c r="Y29">
+      <c r="AA29">
         <f t="shared" si="2"/>
         <v>232.53311235896197</v>
       </c>
-      <c r="Z29" t="s">
+      <c r="AB29" t="s">
         <v>201</v>
       </c>
-      <c r="AA29" s="1" t="s">
+      <c r="AC29" s="1" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>2</v>
       </c>
@@ -3186,52 +3328,55 @@
       <c r="M30" t="s">
         <v>186</v>
       </c>
-      <c r="N30">
+      <c r="N30" t="s">
+        <v>167</v>
+      </c>
+      <c r="P30">
         <v>3826.16</v>
       </c>
-      <c r="O30">
+      <c r="Q30">
         <v>3125.63</v>
       </c>
-      <c r="P30">
+      <c r="R30">
         <v>14621</v>
       </c>
-      <c r="Q30">
+      <c r="S30">
         <v>1438</v>
       </c>
-      <c r="R30">
+      <c r="T30">
         <v>3912.95</v>
       </c>
-      <c r="S30">
+      <c r="U30">
         <v>4998.99</v>
       </c>
-      <c r="T30">
+      <c r="V30">
         <v>2357444</v>
       </c>
-      <c r="U30">
+      <c r="W30">
         <v>0</v>
       </c>
-      <c r="V30" s="5">
+      <c r="X30" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W30">
+      <c r="Y30">
         <v>2357444</v>
       </c>
-      <c r="X30">
+      <c r="Z30">
         <v>543342504</v>
       </c>
-      <c r="Y30">
+      <c r="AA30">
         <f t="shared" si="2"/>
         <v>230.47949558929076</v>
       </c>
-      <c r="Z30" t="s">
+      <c r="AB30" t="s">
         <v>203</v>
       </c>
-      <c r="AA30" s="1" t="s">
+      <c r="AC30" s="1" t="s">
         <v>204</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>2</v>
       </c>
@@ -3271,55 +3416,58 @@
       <c r="M31" t="s">
         <v>186</v>
       </c>
-      <c r="N31">
+      <c r="N31" t="s">
+        <v>167</v>
+      </c>
+      <c r="P31">
         <v>5840.74</v>
       </c>
-      <c r="O31">
+      <c r="Q31">
         <v>1646.29</v>
       </c>
-      <c r="P31">
+      <c r="R31">
         <v>62420</v>
       </c>
-      <c r="Q31">
+      <c r="S31">
         <v>86</v>
       </c>
-      <c r="R31">
+      <c r="T31">
         <v>1629.9</v>
       </c>
-      <c r="S31">
+      <c r="U31">
         <v>2862.99</v>
       </c>
-      <c r="T31">
+      <c r="V31">
         <v>3611966</v>
       </c>
-      <c r="U31">
+      <c r="W31">
         <v>3</v>
       </c>
-      <c r="V31" s="5">
+      <c r="X31" s="5">
         <f t="shared" si="1"/>
         <v>8.3057260228916886E-7</v>
       </c>
-      <c r="W31">
+      <c r="Y31">
         <v>3611344</v>
       </c>
-      <c r="X31">
+      <c r="Z31">
         <v>833435917</v>
       </c>
-      <c r="Y31">
-        <f>X31/W31</f>
+      <c r="AA31">
+        <f t="shared" ref="AA31:AA50" si="3">Z31/Y31</f>
         <v>230.78275484141085</v>
       </c>
-      <c r="Z31" t="s">
+      <c r="AB31" t="s">
         <v>205</v>
       </c>
-      <c r="AA31" s="1" t="s">
+      <c r="AC31" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="AB31" t="s">
+      <c r="AD31" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>2</v>
       </c>
@@ -3359,52 +3507,55 @@
       <c r="M32" t="s">
         <v>186</v>
       </c>
-      <c r="N32">
+      <c r="N32" t="s">
+        <v>167</v>
+      </c>
+      <c r="P32">
         <v>5968.45</v>
       </c>
-      <c r="O32">
+      <c r="Q32">
         <v>1056.67</v>
       </c>
-      <c r="P32">
+      <c r="R32">
         <v>61377</v>
       </c>
-      <c r="Q32">
+      <c r="S32">
         <v>39</v>
       </c>
-      <c r="R32">
+      <c r="T32">
         <v>299.95</v>
       </c>
-      <c r="S32">
+      <c r="U32">
         <v>410</v>
       </c>
-      <c r="T32">
+      <c r="V32">
         <v>3686456</v>
       </c>
-      <c r="U32">
+      <c r="W32">
         <v>13</v>
       </c>
-      <c r="V32" s="5">
+      <c r="X32" s="5">
         <f t="shared" si="1"/>
         <v>3.5264221246639049E-6</v>
       </c>
-      <c r="W32">
+      <c r="Y32">
         <v>3686443</v>
       </c>
-      <c r="X32">
+      <c r="Z32">
         <v>863169579</v>
       </c>
-      <c r="Y32">
-        <f>X32/W32</f>
+      <c r="AA32">
+        <f t="shared" si="3"/>
         <v>234.147002679819</v>
       </c>
-      <c r="Z32" t="s">
+      <c r="AB32" t="s">
         <v>11</v>
       </c>
-      <c r="AA32" s="1" t="s">
+      <c r="AC32" s="1" t="s">
         <v>208</v>
       </c>
     </row>
-    <row r="33" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>2</v>
       </c>
@@ -3444,52 +3595,55 @@
       <c r="M33" t="s">
         <v>186</v>
       </c>
-      <c r="N33">
+      <c r="N33" t="s">
+        <v>167</v>
+      </c>
+      <c r="P33">
         <v>15261.16</v>
       </c>
-      <c r="O33">
+      <c r="Q33">
         <v>288.79000000000002</v>
       </c>
-      <c r="P33">
+      <c r="R33">
         <v>3570</v>
       </c>
-      <c r="Q33">
+      <c r="S33">
         <v>69</v>
       </c>
-      <c r="R33">
+      <c r="T33">
         <v>118</v>
       </c>
-      <c r="S33">
+      <c r="U33">
         <v>135</v>
       </c>
-      <c r="T33">
+      <c r="V33">
         <v>9313564</v>
       </c>
-      <c r="U33">
+      <c r="W33">
         <v>1</v>
       </c>
-      <c r="V33" s="5">
+      <c r="X33" s="5">
         <f t="shared" si="1"/>
         <v>1.0737028274031294E-7</v>
       </c>
-      <c r="W33">
+      <c r="Y33">
         <v>9313563</v>
       </c>
-      <c r="X33">
+      <c r="Z33">
         <v>2200047234</v>
       </c>
-      <c r="Y33">
-        <f>X33/W33</f>
+      <c r="AA33">
+        <f t="shared" si="3"/>
         <v>236.21971891960143</v>
       </c>
-      <c r="Z33" t="s">
+      <c r="AB33" t="s">
         <v>195</v>
       </c>
-      <c r="AA33" s="1" t="s">
+      <c r="AC33" s="1" t="s">
         <v>209</v>
       </c>
     </row>
-    <row r="34" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>2</v>
       </c>
@@ -3529,55 +3683,58 @@
       <c r="M34" t="s">
         <v>186</v>
       </c>
-      <c r="N34">
+      <c r="N34" t="s">
+        <v>167</v>
+      </c>
+      <c r="P34">
         <v>22476.45</v>
       </c>
-      <c r="O34">
+      <c r="Q34">
         <v>192.85</v>
       </c>
-      <c r="P34">
+      <c r="R34">
         <v>60004</v>
       </c>
-      <c r="Q34">
+      <c r="S34">
         <v>12</v>
       </c>
-      <c r="R34">
+      <c r="T34">
         <v>34</v>
       </c>
-      <c r="S34">
+      <c r="U34">
         <v>46.99</v>
       </c>
-      <c r="T34">
+      <c r="V34">
         <v>14028183</v>
       </c>
-      <c r="U34">
+      <c r="W34">
         <v>1</v>
       </c>
-      <c r="V34" s="5">
+      <c r="X34" s="5">
         <f t="shared" si="1"/>
         <v>7.128506949189357E-8</v>
       </c>
-      <c r="W34">
+      <c r="Y34">
         <v>14028182</v>
       </c>
-      <c r="X34">
+      <c r="Z34">
         <v>3274689327</v>
       </c>
-      <c r="Y34">
-        <f>X34/W34</f>
+      <c r="AA34">
+        <f t="shared" si="3"/>
         <v>233.43647288009237</v>
       </c>
-      <c r="Z34" t="s">
+      <c r="AB34" t="s">
         <v>24</v>
       </c>
-      <c r="AA34" s="1" t="s">
+      <c r="AC34" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="AB34" t="s">
+      <c r="AD34" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="35" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>2</v>
       </c>
@@ -3617,55 +3774,58 @@
       <c r="M35" t="s">
         <v>186</v>
       </c>
-      <c r="N35">
+      <c r="N35" t="s">
+        <v>167</v>
+      </c>
+      <c r="P35">
         <v>10628.15</v>
       </c>
-      <c r="O35">
+      <c r="Q35">
         <v>506.24</v>
       </c>
-      <c r="P35">
+      <c r="R35">
         <v>34612</v>
       </c>
-      <c r="Q35">
+      <c r="S35">
         <v>20</v>
       </c>
-      <c r="R35">
+      <c r="T35">
         <v>62</v>
       </c>
-      <c r="S35">
+      <c r="U35">
         <v>102</v>
       </c>
-      <c r="T35">
+      <c r="V35">
         <v>6826079</v>
       </c>
-      <c r="U35">
+      <c r="W35">
         <v>0</v>
       </c>
-      <c r="V35" s="5">
+      <c r="X35" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W35">
+      <c r="Y35">
         <v>6826079</v>
       </c>
-      <c r="X35">
+      <c r="Z35">
         <v>1584049936</v>
       </c>
-      <c r="Y35">
-        <f>X35/W35</f>
+      <c r="AA35">
+        <f t="shared" si="3"/>
         <v>232.05854136759916</v>
       </c>
-      <c r="Z35" t="s">
+      <c r="AB35" t="s">
         <v>17</v>
       </c>
-      <c r="AA35" s="1" t="s">
+      <c r="AC35" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="AB35" t="s">
+      <c r="AD35" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="36" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>2</v>
       </c>
@@ -3705,55 +3865,58 @@
       <c r="M36" t="s">
         <v>186</v>
       </c>
-      <c r="N36">
+      <c r="N36" t="s">
+        <v>167</v>
+      </c>
+      <c r="P36">
         <v>13629.6</v>
       </c>
-      <c r="O36">
+      <c r="Q36">
         <v>429.63</v>
       </c>
-      <c r="P36">
+      <c r="R36">
         <v>61814</v>
       </c>
-      <c r="Q36">
+      <c r="S36">
         <v>16</v>
       </c>
-      <c r="R36">
+      <c r="T36">
         <v>60</v>
       </c>
-      <c r="S36">
+      <c r="U36">
         <v>132</v>
       </c>
-      <c r="T36">
+      <c r="V36">
         <v>9407177</v>
       </c>
-      <c r="U36">
+      <c r="W36">
         <v>26</v>
       </c>
-      <c r="V36" s="5">
+      <c r="X36" s="5">
         <f t="shared" si="1"/>
         <v>2.7638472200533697E-6</v>
       </c>
-      <c r="W36">
+      <c r="Y36">
         <v>9407151</v>
       </c>
-      <c r="X36">
+      <c r="Z36">
         <v>2182593331</v>
       </c>
-      <c r="Y36">
-        <f>X36/W36</f>
+      <c r="AA36">
+        <f t="shared" si="3"/>
         <v>232.01427626706536</v>
       </c>
-      <c r="Z36" t="s">
+      <c r="AB36" t="s">
         <v>216</v>
       </c>
-      <c r="AA36" s="1" t="s">
+      <c r="AC36" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="AB36" t="s">
+      <c r="AD36" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="37" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>2</v>
       </c>
@@ -3793,55 +3956,58 @@
       <c r="M37" t="s">
         <v>186</v>
       </c>
-      <c r="N37">
+      <c r="N37" t="s">
+        <v>167</v>
+      </c>
+      <c r="P37">
         <v>12102.34</v>
       </c>
-      <c r="O37">
+      <c r="Q37">
         <v>336.23</v>
       </c>
-      <c r="P37">
+      <c r="R37">
         <v>61162</v>
       </c>
-      <c r="Q37">
+      <c r="S37">
         <v>10</v>
       </c>
-      <c r="R37">
-        <v>37</v>
-      </c>
-      <c r="S37">
+      <c r="T37">
+        <v>37</v>
+      </c>
+      <c r="U37">
         <v>615</v>
       </c>
-      <c r="T37">
+      <c r="V37">
         <v>8734237</v>
       </c>
-      <c r="U37">
+      <c r="W37">
         <v>25</v>
       </c>
-      <c r="V37" s="5">
+      <c r="X37" s="5">
         <f t="shared" si="1"/>
         <v>2.8622992483487683E-6</v>
       </c>
-      <c r="W37">
+      <c r="Y37">
         <v>8734300</v>
       </c>
-      <c r="X37">
+      <c r="Z37">
         <v>2068104128</v>
       </c>
-      <c r="Y37">
-        <f>X37/W37</f>
+      <c r="AA37">
+        <f t="shared" si="3"/>
         <v>236.77960775334029</v>
       </c>
-      <c r="Z37" t="s">
+      <c r="AB37" t="s">
         <v>195</v>
       </c>
-      <c r="AA37" s="1" t="s">
+      <c r="AC37" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="AB37" t="s">
+      <c r="AD37" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="38" spans="1:28" ht="68" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:30" ht="68" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>2</v>
       </c>
@@ -3881,55 +4047,58 @@
       <c r="M38" t="s">
         <v>186</v>
       </c>
-      <c r="N38">
+      <c r="N38" t="s">
+        <v>167</v>
+      </c>
+      <c r="P38">
         <v>14571.72</v>
       </c>
-      <c r="O38">
+      <c r="Q38">
         <v>196.24</v>
       </c>
-      <c r="P38">
+      <c r="R38">
         <v>36362</v>
       </c>
-      <c r="Q38">
+      <c r="S38">
         <v>7</v>
       </c>
-      <c r="R38">
+      <c r="T38">
         <v>31</v>
       </c>
-      <c r="S38">
+      <c r="U38">
         <v>45</v>
       </c>
-      <c r="T38">
+      <c r="V38">
         <v>10326675</v>
       </c>
-      <c r="U38">
+      <c r="W38">
         <v>58133</v>
       </c>
-      <c r="V38" s="5">
+      <c r="X38" s="5">
         <f t="shared" si="1"/>
         <v>5.6294015256604856E-3</v>
       </c>
-      <c r="W38">
+      <c r="Y38">
         <v>10268542</v>
       </c>
-      <c r="X38">
+      <c r="Z38">
         <v>2387021242</v>
       </c>
-      <c r="Y38">
-        <f>X38/W38</f>
+      <c r="AA38">
+        <f t="shared" si="3"/>
         <v>232.45960741067233</v>
       </c>
-      <c r="Z38" t="s">
+      <c r="AB38" t="s">
         <v>145</v>
       </c>
-      <c r="AA38" s="1" t="s">
+      <c r="AC38" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="AB38" s="6" t="s">
+      <c r="AD38" s="6" t="s">
         <v>225</v>
       </c>
     </row>
-    <row r="39" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>2</v>
       </c>
@@ -3969,52 +4138,55 @@
       <c r="M39" t="s">
         <v>186</v>
       </c>
-      <c r="N39">
+      <c r="N39" t="s">
+        <v>167</v>
+      </c>
+      <c r="P39">
         <v>20503.560000000001</v>
       </c>
-      <c r="O39">
+      <c r="Q39">
         <v>129.66999999999999</v>
       </c>
-      <c r="P39">
+      <c r="R39">
         <v>47121</v>
       </c>
-      <c r="Q39">
+      <c r="S39">
         <v>6</v>
       </c>
-      <c r="R39">
+      <c r="T39">
         <v>20</v>
       </c>
-      <c r="S39">
+      <c r="U39">
         <v>31</v>
       </c>
-      <c r="T39">
+      <c r="V39">
         <v>14774683</v>
       </c>
-      <c r="U39">
+      <c r="W39">
         <v>0</v>
       </c>
-      <c r="V39" s="5">
+      <c r="X39" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W39">
+      <c r="Y39">
         <v>14774683</v>
       </c>
-      <c r="X39">
+      <c r="Z39">
         <v>3273247262</v>
       </c>
-      <c r="Y39">
-        <f>X39/W39</f>
+      <c r="AA39">
+        <f t="shared" si="3"/>
         <v>221.54433106957353</v>
       </c>
-      <c r="AA39" s="1" t="s">
+      <c r="AC39" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="AB39" t="s">
+      <c r="AD39" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="40" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>2</v>
       </c>
@@ -4054,55 +4226,58 @@
       <c r="M40" t="s">
         <v>186</v>
       </c>
-      <c r="N40">
+      <c r="N40" t="s">
+        <v>167</v>
+      </c>
+      <c r="P40">
         <v>18996.12</v>
       </c>
-      <c r="O40">
+      <c r="Q40">
         <v>158.12</v>
       </c>
-      <c r="P40">
+      <c r="R40">
         <v>75073</v>
       </c>
-      <c r="Q40">
+      <c r="S40">
         <v>4</v>
       </c>
-      <c r="R40">
+      <c r="T40">
         <v>12</v>
       </c>
-      <c r="S40">
+      <c r="U40">
         <v>21</v>
       </c>
-      <c r="T40">
+      <c r="V40">
         <v>13949234</v>
       </c>
-      <c r="U40">
+      <c r="W40">
         <v>6</v>
       </c>
-      <c r="V40" s="5">
+      <c r="X40" s="5">
         <f t="shared" si="1"/>
         <v>4.301311455525085E-7</v>
       </c>
-      <c r="W40">
+      <c r="Y40">
         <v>13949229</v>
       </c>
-      <c r="X40">
+      <c r="Z40">
         <v>3079892466</v>
       </c>
-      <c r="Y40">
-        <f>X40/W40</f>
+      <c r="AA40">
+        <f t="shared" si="3"/>
         <v>220.79302490481732</v>
       </c>
-      <c r="Z40" t="s">
+      <c r="AB40" t="s">
         <v>226</v>
       </c>
-      <c r="AA40" s="1" t="s">
+      <c r="AC40" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="AB40" t="s">
+      <c r="AD40" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="41" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A41">
         <v>2</v>
       </c>
@@ -4142,55 +4317,58 @@
       <c r="M41" t="s">
         <v>186</v>
       </c>
-      <c r="N41">
+      <c r="N41" t="s">
+        <v>167</v>
+      </c>
+      <c r="P41">
         <v>17653.580000000002</v>
       </c>
-      <c r="O41">
+      <c r="Q41">
         <v>221.66</v>
       </c>
-      <c r="P41">
+      <c r="R41">
         <v>31594</v>
       </c>
-      <c r="Q41">
+      <c r="S41">
         <v>8</v>
       </c>
-      <c r="R41">
+      <c r="T41">
         <v>31</v>
       </c>
-      <c r="S41">
+      <c r="U41">
         <v>46</v>
       </c>
-      <c r="T41">
+      <c r="V41">
         <v>12063344</v>
       </c>
-      <c r="U41">
+      <c r="W41">
         <v>2</v>
       </c>
-      <c r="V41" s="5">
+      <c r="X41" s="5">
         <f t="shared" si="1"/>
         <v>1.6579150855683133E-7</v>
       </c>
-      <c r="W41">
+      <c r="Y41">
         <v>12063342</v>
       </c>
-      <c r="X41">
+      <c r="Z41">
         <v>2662524936</v>
       </c>
-      <c r="Y41">
-        <f>X41/W41</f>
+      <c r="AA41">
+        <f t="shared" si="3"/>
         <v>220.71204944699403</v>
       </c>
-      <c r="Z41" t="s">
+      <c r="AB41" t="s">
         <v>158</v>
       </c>
-      <c r="AA41" s="1" t="s">
+      <c r="AC41" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="AB41" t="s">
+      <c r="AD41" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="42" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A42">
         <v>2</v>
       </c>
@@ -4230,55 +4408,58 @@
       <c r="M42" t="s">
         <v>186</v>
       </c>
-      <c r="N42">
+      <c r="N42" t="s">
+        <v>167</v>
+      </c>
+      <c r="P42">
         <v>15806.69</v>
       </c>
-      <c r="O42">
+      <c r="Q42">
         <v>273</v>
       </c>
-      <c r="P42">
+      <c r="R42">
         <v>16021</v>
       </c>
-      <c r="Q42">
+      <c r="S42">
         <v>7</v>
       </c>
-      <c r="R42">
+      <c r="T42">
         <v>24</v>
       </c>
-      <c r="S42">
+      <c r="U42">
         <v>34.99</v>
       </c>
-      <c r="T42">
+      <c r="V42">
         <v>10414046</v>
       </c>
-      <c r="U42">
+      <c r="W42">
         <v>1</v>
       </c>
-      <c r="V42" s="5">
+      <c r="X42" s="5">
         <f t="shared" si="1"/>
         <v>9.6024158141801949E-8</v>
       </c>
-      <c r="W42">
+      <c r="Y42">
         <v>10414045</v>
       </c>
-      <c r="X42">
+      <c r="Z42">
         <v>2275144885</v>
       </c>
-      <c r="Y42">
-        <f>X42/W42</f>
+      <c r="AA42">
+        <f t="shared" si="3"/>
         <v>218.46889321104337</v>
       </c>
-      <c r="Z42" t="s">
+      <c r="AB42" t="s">
         <v>17</v>
       </c>
-      <c r="AA42" s="1" t="s">
+      <c r="AC42" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="AB42" t="s">
+      <c r="AD42" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="43" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A43" s="3">
         <v>2</v>
       </c>
@@ -4318,55 +4499,58 @@
       <c r="M43" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="N43">
+      <c r="N43" t="s">
+        <v>167</v>
+      </c>
+      <c r="P43">
         <v>14157.48</v>
       </c>
-      <c r="O43">
+      <c r="Q43">
         <v>308.52999999999997</v>
       </c>
-      <c r="P43" s="3">
+      <c r="R43" s="3">
         <v>8172</v>
       </c>
-      <c r="Q43" s="3">
+      <c r="S43" s="3">
         <v>13</v>
       </c>
-      <c r="R43" s="3">
-        <v>35</v>
-      </c>
-      <c r="S43" s="3">
+      <c r="T43" s="3">
+        <v>35</v>
+      </c>
+      <c r="U43" s="3">
         <v>49</v>
       </c>
-      <c r="T43">
+      <c r="V43">
         <v>8998948</v>
       </c>
-      <c r="U43">
+      <c r="W43">
         <v>0</v>
       </c>
-      <c r="V43" s="5">
+      <c r="X43" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W43">
+      <c r="Y43">
         <v>8998948</v>
       </c>
-      <c r="X43">
+      <c r="Z43">
         <v>1956906490</v>
       </c>
-      <c r="Y43">
-        <f>X43/W43</f>
+      <c r="AA43">
+        <f t="shared" si="3"/>
         <v>217.45947304062653</v>
       </c>
-      <c r="Z43" t="s">
+      <c r="AB43" t="s">
         <v>195</v>
       </c>
-      <c r="AA43" s="1" t="s">
+      <c r="AC43" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="AB43" t="s">
+      <c r="AD43" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="44" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A44" s="3">
         <v>2</v>
       </c>
@@ -4406,56 +4590,878 @@
       <c r="M44" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="N44">
+      <c r="N44" t="s">
+        <v>167</v>
+      </c>
+      <c r="P44">
         <v>29457.69</v>
       </c>
-      <c r="O44">
+      <c r="Q44">
         <v>135.77000000000001</v>
       </c>
-      <c r="P44" s="3">
+      <c r="R44" s="3">
         <v>5436</v>
       </c>
-      <c r="Q44" s="3">
+      <c r="S44" s="3">
         <v>8</v>
       </c>
-      <c r="R44" s="3">
+      <c r="T44" s="3">
         <v>24</v>
       </c>
-      <c r="S44">
+      <c r="U44">
         <v>38</v>
       </c>
-      <c r="T44">
+      <c r="V44">
         <v>18308160</v>
       </c>
-      <c r="U44">
+      <c r="W44">
         <v>0</v>
       </c>
-      <c r="V44" s="5">
+      <c r="X44" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="W44">
+      <c r="Y44">
         <v>18308160</v>
       </c>
-      <c r="X44">
+      <c r="Z44">
         <v>3985857954</v>
       </c>
-      <c r="Y44">
-        <f>X44/W44</f>
+      <c r="AA44">
+        <f t="shared" si="3"/>
         <v>217.70936860940697</v>
       </c>
-      <c r="Z44" t="s">
+      <c r="AB44" t="s">
         <v>220</v>
       </c>
-      <c r="AA44" s="1" t="s">
+      <c r="AC44" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="AB44" t="s">
+      <c r="AD44" t="s">
         <v>223</v>
       </c>
     </row>
+    <row r="45" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>2</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45">
+        <v>3</v>
+      </c>
+      <c r="D45">
+        <v>28800</v>
+      </c>
+      <c r="E45">
+        <v>1</v>
+      </c>
+      <c r="F45">
+        <v>2</v>
+      </c>
+      <c r="G45">
+        <v>600</v>
+      </c>
+      <c r="H45" t="s">
+        <v>161</v>
+      </c>
+      <c r="I45" t="s">
+        <v>212</v>
+      </c>
+      <c r="J45">
+        <v>2</v>
+      </c>
+      <c r="K45">
+        <v>4</v>
+      </c>
+      <c r="L45">
+        <v>8</v>
+      </c>
+      <c r="M45" t="s">
+        <v>186</v>
+      </c>
+      <c r="N45" t="s">
+        <v>173</v>
+      </c>
+      <c r="O45">
+        <v>20</v>
+      </c>
+      <c r="P45">
+        <v>6464.38</v>
+      </c>
+      <c r="Q45">
+        <v>1112.6300000000001</v>
+      </c>
+      <c r="R45">
+        <v>61345</v>
+      </c>
+      <c r="S45" s="3">
+        <v>41</v>
+      </c>
+      <c r="T45">
+        <v>5786</v>
+      </c>
+      <c r="U45">
+        <v>9060.99</v>
+      </c>
+      <c r="V45">
+        <v>6238718</v>
+      </c>
+      <c r="W45">
+        <v>39</v>
+      </c>
+      <c r="X45" s="5">
+        <f t="shared" si="1"/>
+        <v>6.2512843183487377E-6</v>
+      </c>
+      <c r="Y45">
+        <v>6238679</v>
+      </c>
+      <c r="Z45">
+        <v>1499612804</v>
+      </c>
+      <c r="AA45">
+        <f t="shared" si="3"/>
+        <v>240.37345149510017</v>
+      </c>
+      <c r="AB45" t="s">
+        <v>232</v>
+      </c>
+      <c r="AC45" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="46" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>2</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46">
+        <v>3</v>
+      </c>
+      <c r="D46">
+        <v>24000</v>
+      </c>
+      <c r="E46">
+        <v>1</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <v>600</v>
+      </c>
+      <c r="H46" t="s">
+        <v>161</v>
+      </c>
+      <c r="I46" t="s">
+        <v>212</v>
+      </c>
+      <c r="J46">
+        <v>2</v>
+      </c>
+      <c r="K46">
+        <v>4</v>
+      </c>
+      <c r="L46">
+        <v>8</v>
+      </c>
+      <c r="M46" t="s">
+        <v>186</v>
+      </c>
+      <c r="N46" t="s">
+        <v>173</v>
+      </c>
+      <c r="O46">
+        <v>20</v>
+      </c>
+      <c r="P46">
+        <v>6436.02</v>
+      </c>
+      <c r="Q46">
+        <v>1840.1</v>
+      </c>
+      <c r="R46">
+        <v>32881</v>
+      </c>
+      <c r="S46">
+        <v>6369</v>
+      </c>
+      <c r="T46">
+        <v>13232.95</v>
+      </c>
+      <c r="U46">
+        <v>13329</v>
+      </c>
+      <c r="V46">
+        <v>6014128</v>
+      </c>
+      <c r="W46">
+        <v>0</v>
+      </c>
+      <c r="X46" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y46">
+        <v>6014128</v>
+      </c>
+      <c r="Z46">
+        <v>1450688200</v>
+      </c>
+      <c r="AA46">
+        <f t="shared" si="3"/>
+        <v>241.21338953876605</v>
+      </c>
+      <c r="AB46" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC46" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="47" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>2</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47">
+        <v>3</v>
+      </c>
+      <c r="D47">
+        <v>19600</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>2</v>
+      </c>
+      <c r="G47">
+        <v>600</v>
+      </c>
+      <c r="H47" t="s">
+        <v>161</v>
+      </c>
+      <c r="I47" t="s">
+        <v>212</v>
+      </c>
+      <c r="J47">
+        <v>2</v>
+      </c>
+      <c r="K47">
+        <v>4</v>
+      </c>
+      <c r="L47">
+        <v>8</v>
+      </c>
+      <c r="M47" t="s">
+        <v>186</v>
+      </c>
+      <c r="N47" t="s">
+        <v>173</v>
+      </c>
+      <c r="O47">
+        <v>20</v>
+      </c>
+      <c r="P47">
+        <v>5712.68</v>
+      </c>
+      <c r="Q47">
+        <v>2003.17</v>
+      </c>
+      <c r="R47">
+        <v>13631</v>
+      </c>
+      <c r="S47" s="3">
+        <v>15</v>
+      </c>
+      <c r="T47">
+        <v>357</v>
+      </c>
+      <c r="U47">
+        <v>568.99</v>
+      </c>
+      <c r="V47">
+        <v>5364431</v>
+      </c>
+      <c r="W47">
+        <v>0</v>
+      </c>
+      <c r="X47" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y47">
+        <v>5364431</v>
+      </c>
+      <c r="Z47">
+        <v>1297832908</v>
+      </c>
+      <c r="AA47">
+        <f t="shared" si="3"/>
+        <v>241.93300426457159</v>
+      </c>
+      <c r="AB47" t="s">
+        <v>236</v>
+      </c>
+      <c r="AC47" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="48" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="A48">
+        <v>2</v>
+      </c>
+      <c r="B48">
+        <v>3</v>
+      </c>
+      <c r="C48">
+        <v>3</v>
+      </c>
+      <c r="D48">
+        <v>14400</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>2</v>
+      </c>
+      <c r="G48">
+        <v>600</v>
+      </c>
+      <c r="H48" t="s">
+        <v>161</v>
+      </c>
+      <c r="I48" t="s">
+        <v>212</v>
+      </c>
+      <c r="J48">
+        <v>2</v>
+      </c>
+      <c r="K48">
+        <v>4</v>
+      </c>
+      <c r="L48">
+        <v>8</v>
+      </c>
+      <c r="M48" t="s">
+        <v>186</v>
+      </c>
+      <c r="N48" t="s">
+        <v>173</v>
+      </c>
+      <c r="O48">
+        <v>20</v>
+      </c>
+      <c r="P48">
+        <v>5672.26</v>
+      </c>
+      <c r="Q48">
+        <v>1692.19</v>
+      </c>
+      <c r="R48">
+        <v>10783</v>
+      </c>
+      <c r="S48" s="3">
+        <v>11</v>
+      </c>
+      <c r="T48">
+        <v>148</v>
+      </c>
+      <c r="U48">
+        <v>286</v>
+      </c>
+      <c r="V48">
+        <v>5290095</v>
+      </c>
+      <c r="W48">
+        <v>0</v>
+      </c>
+      <c r="X48" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y48">
+        <v>5290095</v>
+      </c>
+      <c r="Z48">
+        <v>1276042457</v>
+      </c>
+      <c r="AA48">
+        <f t="shared" si="3"/>
+        <v>241.21352395372861</v>
+      </c>
+      <c r="AB48" t="s">
+        <v>238</v>
+      </c>
+      <c r="AC48" s="1" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="49" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A49">
+        <v>2</v>
+      </c>
+      <c r="B49">
+        <v>3</v>
+      </c>
+      <c r="C49">
+        <v>3</v>
+      </c>
+      <c r="D49">
+        <v>9600</v>
+      </c>
+      <c r="E49">
+        <v>1</v>
+      </c>
+      <c r="F49">
+        <v>2</v>
+      </c>
+      <c r="G49">
+        <v>600</v>
+      </c>
+      <c r="H49" t="s">
+        <v>161</v>
+      </c>
+      <c r="I49" t="s">
+        <v>212</v>
+      </c>
+      <c r="J49">
+        <v>2</v>
+      </c>
+      <c r="K49">
+        <v>4</v>
+      </c>
+      <c r="L49">
+        <v>8</v>
+      </c>
+      <c r="M49" t="s">
+        <v>186</v>
+      </c>
+      <c r="N49" t="s">
+        <v>173</v>
+      </c>
+      <c r="O49">
+        <v>20</v>
+      </c>
+      <c r="P49">
+        <v>5625.35</v>
+      </c>
+      <c r="Q49">
+        <v>1151.0999999999999</v>
+      </c>
+      <c r="R49">
+        <v>7721</v>
+      </c>
+      <c r="S49" s="3">
+        <v>17</v>
+      </c>
+      <c r="T49">
+        <v>526.95000000000005</v>
+      </c>
+      <c r="U49">
+        <v>796.99</v>
+      </c>
+      <c r="V49">
+        <v>5127237</v>
+      </c>
+      <c r="W49">
+        <v>0</v>
+      </c>
+      <c r="X49" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y49">
+        <v>5127237</v>
+      </c>
+      <c r="Z49">
+        <v>1240026181</v>
+      </c>
+      <c r="AA49">
+        <f t="shared" si="3"/>
+        <v>241.8507630913102</v>
+      </c>
+      <c r="AB49" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC49" s="1" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A50">
+        <v>2</v>
+      </c>
+      <c r="B50">
+        <v>3</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>4800</v>
+      </c>
+      <c r="E50">
+        <v>1</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>600</v>
+      </c>
+      <c r="H50" t="s">
+        <v>161</v>
+      </c>
+      <c r="I50" t="s">
+        <v>212</v>
+      </c>
+      <c r="J50">
+        <v>2</v>
+      </c>
+      <c r="K50">
+        <v>4</v>
+      </c>
+      <c r="L50">
+        <v>8</v>
+      </c>
+      <c r="M50" t="s">
+        <v>186</v>
+      </c>
+      <c r="N50" t="s">
+        <v>173</v>
+      </c>
+      <c r="O50">
+        <v>20</v>
+      </c>
+      <c r="P50">
+        <v>9643.2099999999991</v>
+      </c>
+      <c r="Q50">
+        <v>488.84</v>
+      </c>
+      <c r="R50">
+        <v>3957</v>
+      </c>
+      <c r="S50" s="3">
+        <v>16</v>
+      </c>
+      <c r="T50">
+        <v>453</v>
+      </c>
+      <c r="U50">
+        <v>693</v>
+      </c>
+      <c r="V50">
+        <v>8769789</v>
+      </c>
+      <c r="W50">
+        <v>0</v>
+      </c>
+      <c r="X50" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="Y50">
+        <v>8769789</v>
+      </c>
+      <c r="Z50">
+        <v>2138097843</v>
+      </c>
+      <c r="AA50">
+        <f t="shared" si="3"/>
+        <v>243.80265511519147</v>
+      </c>
+      <c r="AB50" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC50" s="1" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="51" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A51">
+        <v>2</v>
+      </c>
+      <c r="B51">
+        <v>3</v>
+      </c>
+      <c r="C51">
+        <v>3</v>
+      </c>
+      <c r="D51">
+        <v>24000</v>
+      </c>
+      <c r="E51">
+        <v>1</v>
+      </c>
+      <c r="F51">
+        <v>2</v>
+      </c>
+      <c r="G51">
+        <v>600</v>
+      </c>
+      <c r="H51" t="s">
+        <v>161</v>
+      </c>
+      <c r="I51" t="s">
+        <v>212</v>
+      </c>
+      <c r="J51">
+        <v>2</v>
+      </c>
+      <c r="K51">
+        <v>6</v>
+      </c>
+      <c r="L51">
+        <v>8</v>
+      </c>
+      <c r="M51" t="s">
+        <v>186</v>
+      </c>
+      <c r="N51" t="s">
+        <v>173</v>
+      </c>
+      <c r="O51">
+        <v>20</v>
+      </c>
+      <c r="P51">
+        <v>7564.35</v>
+      </c>
+      <c r="Q51">
+        <v>1092.4100000000001</v>
+      </c>
+      <c r="R51">
+        <v>14025</v>
+      </c>
+      <c r="S51" s="3">
+        <v>9</v>
+      </c>
+      <c r="T51">
+        <v>57</v>
+      </c>
+      <c r="U51">
+        <v>96</v>
+      </c>
+      <c r="V51">
+        <v>7424634</v>
+      </c>
+      <c r="W51">
+        <v>0</v>
+      </c>
+      <c r="X51" s="5">
+        <f t="shared" ref="X51:X53" si="4">W51/V51</f>
+        <v>0</v>
+      </c>
+      <c r="Y51">
+        <v>7424634</v>
+      </c>
+      <c r="Z51">
+        <v>1741600627</v>
+      </c>
+      <c r="AA51">
+        <f t="shared" ref="AA51:AA53" si="5">Z51/Y51</f>
+        <v>234.57056967387214</v>
+      </c>
+      <c r="AB51" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC51" s="1" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="52" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A52">
+        <v>2</v>
+      </c>
+      <c r="B52">
+        <v>3</v>
+      </c>
+      <c r="C52">
+        <v>3</v>
+      </c>
+      <c r="D52">
+        <v>9600</v>
+      </c>
+      <c r="E52">
+        <v>1</v>
+      </c>
+      <c r="F52">
+        <v>2</v>
+      </c>
+      <c r="G52">
+        <v>600</v>
+      </c>
+      <c r="H52" t="s">
+        <v>161</v>
+      </c>
+      <c r="I52" t="s">
+        <v>212</v>
+      </c>
+      <c r="J52">
+        <v>2</v>
+      </c>
+      <c r="K52">
+        <v>6</v>
+      </c>
+      <c r="L52">
+        <v>8</v>
+      </c>
+      <c r="M52" t="s">
+        <v>186</v>
+      </c>
+      <c r="N52" t="s">
+        <v>173</v>
+      </c>
+      <c r="O52">
+        <v>20</v>
+      </c>
+      <c r="P52">
+        <v>5344.84</v>
+      </c>
+      <c r="Q52">
+        <v>1117.4000000000001</v>
+      </c>
+      <c r="R52">
+        <v>15348</v>
+      </c>
+      <c r="S52" s="3">
+        <v>19</v>
+      </c>
+      <c r="T52">
+        <v>313</v>
+      </c>
+      <c r="U52">
+        <v>525.98</v>
+      </c>
+      <c r="V52">
+        <v>4871968</v>
+      </c>
+      <c r="W52">
+        <v>0</v>
+      </c>
+      <c r="X52" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y52">
+        <v>4871968</v>
+      </c>
+      <c r="Z52">
+        <v>1173010698</v>
+      </c>
+      <c r="AA52">
+        <f t="shared" si="5"/>
+        <v>240.76732400541218</v>
+      </c>
+      <c r="AB52" t="s">
+        <v>127</v>
+      </c>
+      <c r="AC52" s="1" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="53" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A53">
+        <v>2</v>
+      </c>
+      <c r="B53">
+        <v>3</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>4800</v>
+      </c>
+      <c r="E53">
+        <v>1</v>
+      </c>
+      <c r="F53">
+        <v>2</v>
+      </c>
+      <c r="G53">
+        <v>600</v>
+      </c>
+      <c r="H53" t="s">
+        <v>161</v>
+      </c>
+      <c r="I53" t="s">
+        <v>212</v>
+      </c>
+      <c r="J53">
+        <v>2</v>
+      </c>
+      <c r="K53">
+        <v>6</v>
+      </c>
+      <c r="L53">
+        <v>8</v>
+      </c>
+      <c r="M53" t="s">
+        <v>186</v>
+      </c>
+      <c r="N53" t="s">
+        <v>173</v>
+      </c>
+      <c r="O53">
+        <v>20</v>
+      </c>
+      <c r="P53">
+        <v>9446.4599999999991</v>
+      </c>
+      <c r="Q53">
+        <v>496.35</v>
+      </c>
+      <c r="R53">
+        <v>4780</v>
+      </c>
+      <c r="S53" s="3">
+        <v>11</v>
+      </c>
+      <c r="T53">
+        <v>422</v>
+      </c>
+      <c r="U53">
+        <v>641</v>
+      </c>
+      <c r="V53">
+        <v>8571563</v>
+      </c>
+      <c r="W53">
+        <v>0</v>
+      </c>
+      <c r="X53" s="5">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="Y53">
+        <v>8571563</v>
+      </c>
+      <c r="Z53">
+        <v>2025504780</v>
+      </c>
+      <c r="AA53">
+        <f t="shared" si="5"/>
+        <v>236.30518494701607</v>
+      </c>
+      <c r="AB53" t="s">
+        <v>240</v>
+      </c>
+      <c r="AC53" s="1" t="s">
+        <v>244</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:AB35" xr:uid="{0BCD43CD-D15C-C44C-860E-27B2AEF78201}"/>
+  <autoFilter ref="A1:AD35" xr:uid="{0BCD43CD-D15C-C44C-860E-27B2AEF78201}"/>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -4466,7 +5472,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
webtest docker, actuator/prometheus, jmx exporter, benchmark
</commit_message>
<xml_diff>
--- a/kafka_benchmark/benchmark_stats.xlsx
+++ b/kafka_benchmark/benchmark_stats.xlsx
@@ -1,26 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lijjin/Documents/work/git_ws/redistest/kafka_benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DDA4634-1F77-8A41-9A25-71099C1F2B18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA39A38-21B9-7344-B8C0-310414CADCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-20" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{35590E01-C7C5-464A-8FB5-DBB7ECFA3BB7}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{35590E01-C7C5-464A-8FB5-DBB7ECFA3BB7}"/>
   </bookViews>
   <sheets>
-    <sheet name="Kafka Producer" sheetId="4" r:id="rId1"/>
-    <sheet name="Kafka Consumer" sheetId="5" r:id="rId2"/>
-    <sheet name="Kafka Producer Deprecated" sheetId="1" r:id="rId3"/>
-    <sheet name="4 executor" sheetId="2" r:id="rId4"/>
-    <sheet name="600 executor" sheetId="3" r:id="rId5"/>
+    <sheet name="Authz" sheetId="6" r:id="rId1"/>
+    <sheet name="Kafka Producer" sheetId="4" r:id="rId2"/>
+    <sheet name="Kafka Consumer" sheetId="5" r:id="rId3"/>
+    <sheet name="Kafka Producer Deprecated" sheetId="1" r:id="rId4"/>
+    <sheet name="4 executor" sheetId="2" r:id="rId5"/>
+    <sheet name="600 executor" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Kafka Producer'!$A$1:$AD$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Authz!$A$2:$U$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Kafka Producer'!$A$1:$AD$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2601" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2655" uniqueCount="260">
   <si>
     <t>Partition</t>
   </si>
@@ -676,9 +678,6 @@
     <t>CPU #</t>
   </si>
   <si>
-    <t>Memory (G)</t>
-  </si>
-  <si>
     <t>Ingress Nginx</t>
   </si>
   <si>
@@ -779,6 +778,54 @@
   <si>
     <t>mariadb_k8s_2ng_2j_3b_3p_2r_4800t_600e_6cpu</t>
   </si>
+  <si>
+    <t>Authz</t>
+  </si>
+  <si>
+    <t>Redis Replication</t>
+  </si>
+  <si>
+    <t>Replica Preference</t>
+  </si>
+  <si>
+    <t>Heap (G)</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_9600t_600e_4cpu</t>
+  </si>
+  <si>
+    <t>43679852 user-role mapping</t>
+  </si>
+  <si>
+    <t>Each user has 5 roles. 2 of them are associated with app1</t>
+  </si>
+  <si>
+    <t>80000 role-resource mapping. Role1-20 has 4 app1 resources mapped.</t>
+  </si>
+  <si>
+    <t>781000 app resources. 194 app1 resources belong to mapped role either though direct mapping or inheritance.</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_4800t_600e_4cpu</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_4800t_600e_4cpu.1</t>
+  </si>
+  <si>
+    <t>It seems that for 4800 concurrency, the response time is intermittently high</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_2400t_600e_4cpu</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_1200t_600e_4cpu</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_600t_600e_4cpu</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_300t_600e_4cpu</t>
+  </si>
 </sst>
 </file>
 
@@ -850,7 +897,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -860,6 +907,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1174,11 +1222,769 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1D1567-5C01-D845-B094-708B919E4B92}">
+  <dimension ref="A1:U53"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="T10" sqref="T10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="14.33203125" customWidth="1"/>
+    <col min="3" max="3" width="13.1640625" customWidth="1"/>
+    <col min="4" max="4" width="17.33203125" customWidth="1"/>
+    <col min="5" max="5" width="12.83203125" customWidth="1"/>
+    <col min="6" max="6" width="15.83203125" customWidth="1"/>
+    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="8" max="8" width="9.1640625" customWidth="1"/>
+    <col min="9" max="9" width="9" customWidth="1"/>
+    <col min="10" max="10" width="16.33203125" customWidth="1"/>
+    <col min="11" max="11" width="15" customWidth="1"/>
+    <col min="12" max="13" width="21.1640625" customWidth="1"/>
+    <col min="14" max="14" width="24.5" customWidth="1"/>
+    <col min="15" max="16" width="21.1640625" customWidth="1"/>
+    <col min="17" max="17" width="14.6640625" customWidth="1"/>
+    <col min="18" max="19" width="11.33203125" customWidth="1"/>
+    <col min="20" max="20" width="37.6640625" customWidth="1"/>
+    <col min="21" max="21" width="31.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+      <c r="A1" s="6" t="s">
+        <v>249</v>
+      </c>
+      <c r="B1" s="6" t="s">
+        <v>250</v>
+      </c>
+      <c r="C1" s="6" t="s">
+        <v>251</v>
+      </c>
+      <c r="D1" s="6" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>244</v>
+      </c>
+      <c r="B2" t="s">
+        <v>245</v>
+      </c>
+      <c r="C2" t="s">
+        <v>246</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F2" t="s">
+        <v>196</v>
+      </c>
+      <c r="G2" t="s">
+        <v>198</v>
+      </c>
+      <c r="H2" t="s">
+        <v>210</v>
+      </c>
+      <c r="I2" t="s">
+        <v>247</v>
+      </c>
+      <c r="J2" t="s">
+        <v>184</v>
+      </c>
+      <c r="K2" t="s">
+        <v>129</v>
+      </c>
+      <c r="L2" t="s">
+        <v>134</v>
+      </c>
+      <c r="M2" t="s">
+        <v>135</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="P2" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q2" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>188</v>
+      </c>
+      <c r="S2" s="3" t="s">
+        <v>194</v>
+      </c>
+      <c r="T2" t="s">
+        <v>7</v>
+      </c>
+      <c r="U2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3">
+        <v>3</v>
+      </c>
+      <c r="C3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D3">
+        <v>9600</v>
+      </c>
+      <c r="E3">
+        <v>600</v>
+      </c>
+      <c r="F3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>4</v>
+      </c>
+      <c r="I3">
+        <v>6</v>
+      </c>
+      <c r="J3" t="s">
+        <v>186</v>
+      </c>
+      <c r="K3">
+        <v>999.47</v>
+      </c>
+      <c r="L3">
+        <v>689.52</v>
+      </c>
+      <c r="M3">
+        <v>9334</v>
+      </c>
+      <c r="N3">
+        <v>35</v>
+      </c>
+      <c r="O3">
+        <v>304</v>
+      </c>
+      <c r="P3">
+        <v>535</v>
+      </c>
+      <c r="Q3">
+        <v>909782</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="S3" s="7">
+        <f>R3/Q3</f>
+        <v>0</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>1</v>
+      </c>
+      <c r="B4">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>173</v>
+      </c>
+      <c r="D4">
+        <v>4800</v>
+      </c>
+      <c r="E4">
+        <v>600</v>
+      </c>
+      <c r="F4" t="s">
+        <v>211</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>4</v>
+      </c>
+      <c r="I4">
+        <v>6</v>
+      </c>
+      <c r="J4" t="s">
+        <v>186</v>
+      </c>
+      <c r="K4">
+        <v>997.84</v>
+      </c>
+      <c r="L4">
+        <v>361.26</v>
+      </c>
+      <c r="M4">
+        <v>3952</v>
+      </c>
+      <c r="N4">
+        <v>65</v>
+      </c>
+      <c r="O4">
+        <v>116</v>
+      </c>
+      <c r="P4">
+        <v>236</v>
+      </c>
+      <c r="Q4">
+        <v>903334</v>
+      </c>
+      <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4" s="7">
+        <f>R4/Q4</f>
+        <v>0</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>1</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>173</v>
+      </c>
+      <c r="D5">
+        <v>4800</v>
+      </c>
+      <c r="E5">
+        <v>600</v>
+      </c>
+      <c r="F5" t="s">
+        <v>211</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+      <c r="H5">
+        <v>4</v>
+      </c>
+      <c r="I5">
+        <v>6</v>
+      </c>
+      <c r="J5" t="s">
+        <v>186</v>
+      </c>
+      <c r="K5">
+        <v>992.45</v>
+      </c>
+      <c r="L5">
+        <v>350.12</v>
+      </c>
+      <c r="M5">
+        <v>4931</v>
+      </c>
+      <c r="N5">
+        <v>892</v>
+      </c>
+      <c r="O5">
+        <v>1858</v>
+      </c>
+      <c r="P5">
+        <v>1927</v>
+      </c>
+      <c r="Q5">
+        <v>899083</v>
+      </c>
+      <c r="R5">
+        <v>0</v>
+      </c>
+      <c r="S5" s="7">
+        <f>R5/Q5</f>
+        <v>0</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="U5" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>1</v>
+      </c>
+      <c r="B6">
+        <v>3</v>
+      </c>
+      <c r="C6" t="s">
+        <v>173</v>
+      </c>
+      <c r="D6">
+        <v>2400</v>
+      </c>
+      <c r="E6">
+        <v>600</v>
+      </c>
+      <c r="F6" t="s">
+        <v>211</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+      <c r="H6">
+        <v>4</v>
+      </c>
+      <c r="I6">
+        <v>6</v>
+      </c>
+      <c r="J6" t="s">
+        <v>186</v>
+      </c>
+      <c r="K6">
+        <v>997.24</v>
+      </c>
+      <c r="L6">
+        <v>323.60000000000002</v>
+      </c>
+      <c r="M6">
+        <v>2039</v>
+      </c>
+      <c r="N6">
+        <v>63</v>
+      </c>
+      <c r="O6">
+        <v>102</v>
+      </c>
+      <c r="P6">
+        <v>135</v>
+      </c>
+      <c r="Q6">
+        <v>900303</v>
+      </c>
+      <c r="R6">
+        <v>0</v>
+      </c>
+      <c r="S6" s="7">
+        <f>R6/Q6</f>
+        <v>0</v>
+      </c>
+      <c r="T6" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>3</v>
+      </c>
+      <c r="C7" t="s">
+        <v>173</v>
+      </c>
+      <c r="D7">
+        <v>1200</v>
+      </c>
+      <c r="E7">
+        <v>600</v>
+      </c>
+      <c r="F7" t="s">
+        <v>211</v>
+      </c>
+      <c r="G7">
+        <v>1</v>
+      </c>
+      <c r="H7">
+        <v>4</v>
+      </c>
+      <c r="I7">
+        <v>6</v>
+      </c>
+      <c r="J7" t="s">
+        <v>186</v>
+      </c>
+      <c r="K7">
+        <v>997.36</v>
+      </c>
+      <c r="L7">
+        <v>175.85</v>
+      </c>
+      <c r="M7">
+        <v>844</v>
+      </c>
+      <c r="N7">
+        <v>73</v>
+      </c>
+      <c r="O7">
+        <v>512</v>
+      </c>
+      <c r="P7">
+        <v>567.99</v>
+      </c>
+      <c r="Q7">
+        <v>898286</v>
+      </c>
+      <c r="R7">
+        <v>0</v>
+      </c>
+      <c r="S7" s="7">
+        <f>R7/Q7</f>
+        <v>0</v>
+      </c>
+      <c r="T7" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1</v>
+      </c>
+      <c r="B8">
+        <v>3</v>
+      </c>
+      <c r="C8" t="s">
+        <v>173</v>
+      </c>
+      <c r="D8">
+        <v>600</v>
+      </c>
+      <c r="E8">
+        <v>600</v>
+      </c>
+      <c r="F8" t="s">
+        <v>211</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+      <c r="H8">
+        <v>4</v>
+      </c>
+      <c r="I8">
+        <v>6</v>
+      </c>
+      <c r="J8" t="s">
+        <v>186</v>
+      </c>
+      <c r="K8">
+        <v>994.77</v>
+      </c>
+      <c r="L8">
+        <v>95.03</v>
+      </c>
+      <c r="M8">
+        <v>520</v>
+      </c>
+      <c r="N8">
+        <v>64</v>
+      </c>
+      <c r="O8">
+        <v>274</v>
+      </c>
+      <c r="P8">
+        <v>329</v>
+      </c>
+      <c r="Q8">
+        <v>895808</v>
+      </c>
+      <c r="R8">
+        <v>0</v>
+      </c>
+      <c r="S8" s="7">
+        <f>R8/Q8</f>
+        <v>0</v>
+      </c>
+      <c r="T8" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A9">
+        <v>1</v>
+      </c>
+      <c r="B9">
+        <v>3</v>
+      </c>
+      <c r="C9" t="s">
+        <v>173</v>
+      </c>
+      <c r="D9">
+        <v>300</v>
+      </c>
+      <c r="E9">
+        <v>600</v>
+      </c>
+      <c r="F9" t="s">
+        <v>211</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+      <c r="H9">
+        <v>4</v>
+      </c>
+      <c r="I9">
+        <v>6</v>
+      </c>
+      <c r="J9" t="s">
+        <v>186</v>
+      </c>
+      <c r="K9">
+        <v>996.89</v>
+      </c>
+      <c r="L9">
+        <v>71.040000000000006</v>
+      </c>
+      <c r="M9">
+        <v>330</v>
+      </c>
+      <c r="N9">
+        <v>63</v>
+      </c>
+      <c r="O9">
+        <v>113</v>
+      </c>
+      <c r="P9">
+        <v>164</v>
+      </c>
+      <c r="Q9">
+        <v>897305</v>
+      </c>
+      <c r="R9">
+        <v>0</v>
+      </c>
+      <c r="S9" s="7">
+        <f>R9/Q9</f>
+        <v>0</v>
+      </c>
+      <c r="T9" s="1" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T11" s="1"/>
+    </row>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T12" s="1"/>
+    </row>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T13" s="1"/>
+    </row>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T14" s="1"/>
+    </row>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T15" s="1"/>
+    </row>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="T16" s="1"/>
+    </row>
+    <row r="17" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="T17" s="1"/>
+    </row>
+    <row r="18" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="T18" s="1"/>
+    </row>
+    <row r="19" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="T19" s="1"/>
+    </row>
+    <row r="20" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="T20" s="1"/>
+    </row>
+    <row r="21" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="T21" s="1"/>
+    </row>
+    <row r="22" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S22" s="5"/>
+      <c r="T22" s="1"/>
+    </row>
+    <row r="23" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S23" s="5"/>
+      <c r="T23" s="1"/>
+    </row>
+    <row r="24" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S24" s="5"/>
+      <c r="T24" s="1"/>
+    </row>
+    <row r="25" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S25" s="5"/>
+      <c r="T25" s="1"/>
+    </row>
+    <row r="26" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S26" s="5"/>
+      <c r="T26" s="1"/>
+    </row>
+    <row r="27" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S27" s="5"/>
+      <c r="T27" s="1"/>
+    </row>
+    <row r="28" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S28" s="5"/>
+      <c r="T28" s="1"/>
+    </row>
+    <row r="29" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S29" s="5"/>
+      <c r="T29" s="1"/>
+    </row>
+    <row r="30" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S30" s="5"/>
+      <c r="T30" s="1"/>
+    </row>
+    <row r="31" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S31" s="5"/>
+      <c r="T31" s="1"/>
+    </row>
+    <row r="32" spans="19:20" x14ac:dyDescent="0.2">
+      <c r="S32" s="5"/>
+      <c r="T32" s="1"/>
+    </row>
+    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S33" s="5"/>
+      <c r="T33" s="1"/>
+    </row>
+    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S34" s="5"/>
+      <c r="T34" s="1"/>
+    </row>
+    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S35" s="5"/>
+      <c r="T35" s="1"/>
+    </row>
+    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S36" s="5"/>
+      <c r="T36" s="1"/>
+    </row>
+    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S37" s="5"/>
+      <c r="T37" s="1"/>
+    </row>
+    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S38" s="5"/>
+      <c r="T38" s="1"/>
+      <c r="U38" s="6"/>
+    </row>
+    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S39" s="5"/>
+      <c r="T39" s="1"/>
+    </row>
+    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S40" s="5"/>
+      <c r="T40" s="1"/>
+    </row>
+    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S41" s="5"/>
+      <c r="T41" s="1"/>
+    </row>
+    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S42" s="5"/>
+      <c r="T42" s="1"/>
+    </row>
+    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A43" s="3"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="3"/>
+      <c r="D43" s="3"/>
+      <c r="E43" s="3"/>
+      <c r="F43" s="3"/>
+      <c r="G43" s="3"/>
+      <c r="H43" s="3"/>
+      <c r="I43" s="3"/>
+      <c r="J43" s="3"/>
+      <c r="M43" s="3"/>
+      <c r="N43" s="3"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="S43" s="5"/>
+      <c r="T43" s="1"/>
+    </row>
+    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="A44" s="3"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="3"/>
+      <c r="D44" s="3"/>
+      <c r="E44" s="3"/>
+      <c r="F44" s="3"/>
+      <c r="G44" s="3"/>
+      <c r="H44" s="3"/>
+      <c r="I44" s="3"/>
+      <c r="J44" s="3"/>
+      <c r="M44" s="3"/>
+      <c r="N44" s="3"/>
+      <c r="O44" s="3"/>
+      <c r="S44" s="5"/>
+      <c r="T44" s="1"/>
+    </row>
+    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="N45" s="3"/>
+      <c r="S45" s="5"/>
+      <c r="T45" s="1"/>
+    </row>
+    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="S46" s="5"/>
+      <c r="T46" s="1"/>
+    </row>
+    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="N47" s="3"/>
+      <c r="S47" s="5"/>
+      <c r="T47" s="1"/>
+    </row>
+    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="N48" s="3"/>
+      <c r="S48" s="5"/>
+      <c r="T48" s="1"/>
+    </row>
+    <row r="49" spans="14:20" x14ac:dyDescent="0.2">
+      <c r="N49" s="3"/>
+      <c r="S49" s="5"/>
+      <c r="T49" s="1"/>
+    </row>
+    <row r="50" spans="14:20" x14ac:dyDescent="0.2">
+      <c r="N50" s="3"/>
+      <c r="S50" s="5"/>
+      <c r="T50" s="1"/>
+    </row>
+    <row r="51" spans="14:20" x14ac:dyDescent="0.2">
+      <c r="N51" s="3"/>
+      <c r="S51" s="5"/>
+      <c r="T51" s="1"/>
+    </row>
+    <row r="52" spans="14:20" x14ac:dyDescent="0.2">
+      <c r="N52" s="3"/>
+      <c r="S52" s="5"/>
+      <c r="T52" s="1"/>
+    </row>
+    <row r="53" spans="14:20" x14ac:dyDescent="0.2">
+      <c r="N53" s="3"/>
+      <c r="S53" s="5"/>
+      <c r="T53" s="1"/>
+    </row>
+  </sheetData>
+  <autoFilter ref="A2:U35" xr:uid="{0BCD43CD-D15C-C44C-860E-27B2AEF78201}"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A60B9A07-2A84-A84C-9DF8-25F7D96E359D}">
   <dimension ref="A1:AD53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M38" workbookViewId="0">
-      <selection activeCell="P53" sqref="P53"/>
+    <sheetView topLeftCell="A23" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1191,7 +1997,7 @@
     <col min="9" max="9" width="15.83203125" customWidth="1"/>
     <col min="10" max="10" width="11.83203125" customWidth="1"/>
     <col min="11" max="11" width="9.1640625" customWidth="1"/>
-    <col min="12" max="12" width="13.5" customWidth="1"/>
+    <col min="12" max="12" width="10.1640625" customWidth="1"/>
     <col min="13" max="13" width="16.33203125" customWidth="1"/>
     <col min="14" max="14" width="9.1640625" customWidth="1"/>
     <col min="15" max="15" width="13.33203125" customWidth="1"/>
@@ -1243,16 +2049,16 @@
         <v>210</v>
       </c>
       <c r="L1" t="s">
-        <v>211</v>
+        <v>247</v>
       </c>
       <c r="M1" t="s">
         <v>184</v>
       </c>
       <c r="N1" t="s">
+        <v>228</v>
+      </c>
+      <c r="O1" t="s">
         <v>229</v>
-      </c>
-      <c r="O1" t="s">
-        <v>230</v>
       </c>
       <c r="P1" t="s">
         <v>129</v>
@@ -2640,7 +3446,7 @@
         <v>4</v>
       </c>
       <c r="L22">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M22" t="s">
         <v>186</v>
@@ -2722,7 +3528,7 @@
         <v>4</v>
       </c>
       <c r="L23">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M23" t="s">
         <v>186</v>
@@ -2804,7 +3610,7 @@
         <v>4</v>
       </c>
       <c r="L24">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M24" t="s">
         <v>186</v>
@@ -2889,7 +3695,7 @@
         <v>4</v>
       </c>
       <c r="L25">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M25" t="s">
         <v>186</v>
@@ -2974,7 +3780,7 @@
         <v>4</v>
       </c>
       <c r="L26">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M26" t="s">
         <v>186</v>
@@ -3059,7 +3865,7 @@
         <v>4</v>
       </c>
       <c r="L27">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M27" t="s">
         <v>186</v>
@@ -3147,7 +3953,7 @@
         <v>4</v>
       </c>
       <c r="L28">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M28" t="s">
         <v>186</v>
@@ -3235,7 +4041,7 @@
         <v>4</v>
       </c>
       <c r="L29">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M29" t="s">
         <v>186</v>
@@ -3323,7 +4129,7 @@
         <v>4</v>
       </c>
       <c r="L30">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M30" t="s">
         <v>186</v>
@@ -3411,7 +4217,7 @@
         <v>4</v>
       </c>
       <c r="L31">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M31" t="s">
         <v>186</v>
@@ -3502,7 +4308,7 @@
         <v>4</v>
       </c>
       <c r="L32">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M32" t="s">
         <v>186</v>
@@ -3590,7 +4396,7 @@
         <v>4</v>
       </c>
       <c r="L33">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M33" t="s">
         <v>186</v>
@@ -3669,7 +4475,7 @@
         <v>161</v>
       </c>
       <c r="I34" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J34">
         <v>1</v>
@@ -3678,7 +4484,7 @@
         <v>4</v>
       </c>
       <c r="L34">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M34" t="s">
         <v>186</v>
@@ -3728,10 +4534,10 @@
         <v>24</v>
       </c>
       <c r="AC34" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="AD34" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="35" spans="1:30" x14ac:dyDescent="0.2">
@@ -3760,7 +4566,7 @@
         <v>161</v>
       </c>
       <c r="I35" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J35">
         <v>1</v>
@@ -3769,7 +4575,7 @@
         <v>4</v>
       </c>
       <c r="L35">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M35" t="s">
         <v>186</v>
@@ -3819,10 +4625,10 @@
         <v>17</v>
       </c>
       <c r="AC35" s="1" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="AD35" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="36" spans="1:30" x14ac:dyDescent="0.2">
@@ -3851,7 +4657,7 @@
         <v>161</v>
       </c>
       <c r="I36" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J36">
         <v>1</v>
@@ -3860,7 +4666,7 @@
         <v>4</v>
       </c>
       <c r="L36">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M36" t="s">
         <v>186</v>
@@ -3907,13 +4713,13 @@
         <v>232.01427626706536</v>
       </c>
       <c r="AB36" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="AC36" s="1" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="AD36" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="37" spans="1:30" x14ac:dyDescent="0.2">
@@ -3942,7 +4748,7 @@
         <v>161</v>
       </c>
       <c r="I37" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J37">
         <v>1</v>
@@ -3951,7 +4757,7 @@
         <v>4</v>
       </c>
       <c r="L37">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M37" t="s">
         <v>186</v>
@@ -4001,10 +4807,10 @@
         <v>195</v>
       </c>
       <c r="AC37" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="AD37" t="s">
         <v>222</v>
-      </c>
-      <c r="AD37" t="s">
-        <v>223</v>
       </c>
     </row>
     <row r="38" spans="1:30" ht="68" x14ac:dyDescent="0.2">
@@ -4033,7 +4839,7 @@
         <v>161</v>
       </c>
       <c r="I38" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J38">
         <v>1</v>
@@ -4042,7 +4848,7 @@
         <v>4</v>
       </c>
       <c r="L38">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M38" t="s">
         <v>186</v>
@@ -4092,10 +4898,10 @@
         <v>145</v>
       </c>
       <c r="AC38" s="1" t="s">
+        <v>223</v>
+      </c>
+      <c r="AD38" s="6" t="s">
         <v>224</v>
-      </c>
-      <c r="AD38" s="6" t="s">
-        <v>225</v>
       </c>
     </row>
     <row r="39" spans="1:30" x14ac:dyDescent="0.2">
@@ -4124,7 +4930,7 @@
         <v>161</v>
       </c>
       <c r="I39" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J39">
         <v>2</v>
@@ -4133,7 +4939,7 @@
         <v>4</v>
       </c>
       <c r="L39">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M39" t="s">
         <v>186</v>
@@ -4180,10 +4986,10 @@
         <v>221.54433106957353</v>
       </c>
       <c r="AC39" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="AD39" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="40" spans="1:30" x14ac:dyDescent="0.2">
@@ -4212,7 +5018,7 @@
         <v>161</v>
       </c>
       <c r="I40" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J40">
         <v>2</v>
@@ -4221,7 +5027,7 @@
         <v>4</v>
       </c>
       <c r="L40">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M40" t="s">
         <v>186</v>
@@ -4268,13 +5074,13 @@
         <v>220.79302490481732</v>
       </c>
       <c r="AB40" t="s">
+        <v>225</v>
+      </c>
+      <c r="AC40" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="AC40" s="1" t="s">
-        <v>227</v>
-      </c>
       <c r="AD40" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="41" spans="1:30" x14ac:dyDescent="0.2">
@@ -4303,7 +5109,7 @@
         <v>161</v>
       </c>
       <c r="I41" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J41">
         <v>2</v>
@@ -4312,7 +5118,7 @@
         <v>4</v>
       </c>
       <c r="L41">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M41" t="s">
         <v>186</v>
@@ -4362,10 +5168,10 @@
         <v>158</v>
       </c>
       <c r="AC41" s="1" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="AD41" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="42" spans="1:30" x14ac:dyDescent="0.2">
@@ -4394,7 +5200,7 @@
         <v>161</v>
       </c>
       <c r="I42" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J42">
         <v>2</v>
@@ -4403,7 +5209,7 @@
         <v>4</v>
       </c>
       <c r="L42">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M42" t="s">
         <v>186</v>
@@ -4453,10 +5259,10 @@
         <v>17</v>
       </c>
       <c r="AC42" s="1" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="AD42" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="43" spans="1:30" x14ac:dyDescent="0.2">
@@ -4485,7 +5291,7 @@
         <v>161</v>
       </c>
       <c r="I43" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J43" s="3">
         <v>2</v>
@@ -4493,8 +5299,8 @@
       <c r="K43" s="3">
         <v>4</v>
       </c>
-      <c r="L43" s="3">
-        <v>8</v>
+      <c r="L43">
+        <v>2</v>
       </c>
       <c r="M43" s="3" t="s">
         <v>186</v>
@@ -4544,10 +5350,10 @@
         <v>195</v>
       </c>
       <c r="AC43" s="1" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="AD43" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="44" spans="1:30" x14ac:dyDescent="0.2">
@@ -4576,7 +5382,7 @@
         <v>161</v>
       </c>
       <c r="I44" s="3" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J44" s="3">
         <v>2</v>
@@ -4584,8 +5390,8 @@
       <c r="K44" s="3">
         <v>4</v>
       </c>
-      <c r="L44" s="3">
-        <v>8</v>
+      <c r="L44">
+        <v>2</v>
       </c>
       <c r="M44" s="3" t="s">
         <v>186</v>
@@ -4632,13 +5438,13 @@
         <v>217.70936860940697</v>
       </c>
       <c r="AB44" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="AC44" s="1" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="AD44" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="45" spans="1:30" x14ac:dyDescent="0.2">
@@ -4667,7 +5473,7 @@
         <v>161</v>
       </c>
       <c r="I45" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J45">
         <v>2</v>
@@ -4676,7 +5482,7 @@
         <v>4</v>
       </c>
       <c r="L45">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M45" t="s">
         <v>186</v>
@@ -4726,10 +5532,10 @@
         <v>240.37345149510017</v>
       </c>
       <c r="AB45" t="s">
+        <v>231</v>
+      </c>
+      <c r="AC45" s="1" t="s">
         <v>232</v>
-      </c>
-      <c r="AC45" s="1" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="46" spans="1:30" x14ac:dyDescent="0.2">
@@ -4758,7 +5564,7 @@
         <v>161</v>
       </c>
       <c r="I46" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J46">
         <v>2</v>
@@ -4767,7 +5573,7 @@
         <v>4</v>
       </c>
       <c r="L46">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M46" t="s">
         <v>186</v>
@@ -4817,10 +5623,10 @@
         <v>241.21338953876605</v>
       </c>
       <c r="AB46" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AC46" s="1" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="47" spans="1:30" x14ac:dyDescent="0.2">
@@ -4849,7 +5655,7 @@
         <v>161</v>
       </c>
       <c r="I47" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J47">
         <v>2</v>
@@ -4858,7 +5664,7 @@
         <v>4</v>
       </c>
       <c r="L47">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M47" t="s">
         <v>186</v>
@@ -4908,10 +5714,10 @@
         <v>241.93300426457159</v>
       </c>
       <c r="AB47" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="AC47" s="1" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
     </row>
     <row r="48" spans="1:30" x14ac:dyDescent="0.2">
@@ -4940,7 +5746,7 @@
         <v>161</v>
       </c>
       <c r="I48" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J48">
         <v>2</v>
@@ -4949,7 +5755,7 @@
         <v>4</v>
       </c>
       <c r="L48">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M48" t="s">
         <v>186</v>
@@ -4999,10 +5805,10 @@
         <v>241.21352395372861</v>
       </c>
       <c r="AB48" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="AC48" s="1" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="49" spans="1:29" x14ac:dyDescent="0.2">
@@ -5031,7 +5837,7 @@
         <v>161</v>
       </c>
       <c r="I49" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J49">
         <v>2</v>
@@ -5040,7 +5846,7 @@
         <v>4</v>
       </c>
       <c r="L49">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M49" t="s">
         <v>186</v>
@@ -5090,10 +5896,10 @@
         <v>241.8507630913102</v>
       </c>
       <c r="AB49" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="AC49" s="1" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="50" spans="1:29" x14ac:dyDescent="0.2">
@@ -5122,7 +5928,7 @@
         <v>161</v>
       </c>
       <c r="I50" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J50">
         <v>2</v>
@@ -5131,7 +5937,7 @@
         <v>4</v>
       </c>
       <c r="L50">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M50" t="s">
         <v>186</v>
@@ -5181,10 +5987,10 @@
         <v>243.80265511519147</v>
       </c>
       <c r="AB50" t="s">
+        <v>239</v>
+      </c>
+      <c r="AC50" s="1" t="s">
         <v>240</v>
-      </c>
-      <c r="AC50" s="1" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:29" x14ac:dyDescent="0.2">
@@ -5213,7 +6019,7 @@
         <v>161</v>
       </c>
       <c r="I51" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J51">
         <v>2</v>
@@ -5222,7 +6028,7 @@
         <v>6</v>
       </c>
       <c r="L51">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M51" t="s">
         <v>186</v>
@@ -5275,7 +6081,7 @@
         <v>127</v>
       </c>
       <c r="AC51" s="1" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
     </row>
     <row r="52" spans="1:29" x14ac:dyDescent="0.2">
@@ -5304,7 +6110,7 @@
         <v>161</v>
       </c>
       <c r="I52" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J52">
         <v>2</v>
@@ -5313,7 +6119,7 @@
         <v>6</v>
       </c>
       <c r="L52">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M52" t="s">
         <v>186</v>
@@ -5366,7 +6172,7 @@
         <v>127</v>
       </c>
       <c r="AC52" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="53" spans="1:29" x14ac:dyDescent="0.2">
@@ -5395,7 +6201,7 @@
         <v>161</v>
       </c>
       <c r="I53" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J53">
         <v>2</v>
@@ -5404,7 +6210,7 @@
         <v>6</v>
       </c>
       <c r="L53">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="M53" t="s">
         <v>186</v>
@@ -5454,10 +6260,10 @@
         <v>236.30518494701607</v>
       </c>
       <c r="AB53" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="AC53" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
   </sheetData>
@@ -5467,7 +6273,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{762E0C42-99D4-A543-A428-00648BDF84DF}">
   <dimension ref="A1:T4"/>
   <sheetViews>
@@ -5683,7 +6489,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E2990C7-E7E3-CA4E-8E79-0E886B76F9BB}">
   <dimension ref="A1:L22"/>
   <sheetViews>
@@ -6501,7 +7307,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{594E75D7-89FD-1144-9CC8-84E2776340D3}">
   <dimension ref="A1:J601"/>
   <sheetViews>
@@ -9942,7 +10748,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F8DF08BF-A93A-CD4D-8036-061C5DD0E181}">
   <dimension ref="A1:J675"/>
   <sheetViews>

</xml_diff>

<commit_message>
enhance jmeter report, response time, 99pct, 99.9pct, 99.99pct
</commit_message>
<xml_diff>
--- a/kafka_benchmark/benchmark_stats.xlsx
+++ b/kafka_benchmark/benchmark_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lijjin/Documents/work/git_ws/redistest/kafka_benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8AA39A38-21B9-7344-B8C0-310414CADCD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C9311E-B9AC-E942-8967-57B9FB4B9BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{35590E01-C7C5-464A-8FB5-DBB7ECFA3BB7}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="600 executor" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Authz!$A$2:$U$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Authz!$A$2:$W$36</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Kafka Producer'!$A$1:$AD$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2655" uniqueCount="260">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2674" uniqueCount="267">
   <si>
     <t>Partition</t>
   </si>
@@ -826,13 +826,35 @@
   <si>
     <t>k8s_1ng_1j_3r_300t_600e_4cpu</t>
   </si>
+  <si>
+    <t>k8s_1ng_1j_3r_19200t_600e_4cpu</t>
+  </si>
+  <si>
+    <t>502/Bad Gateway</t>
+  </si>
+  <si>
+    <t>k8s_2ng_1j_3r_19200t_600e_4cpu</t>
+  </si>
+  <si>
+    <t>k8s_2ng_1j_3r_9600t_600e_4cpu</t>
+  </si>
+  <si>
+    <t>Response Time 99.9% (ms)</t>
+  </si>
+  <si>
+    <t>Response Time 99.99% (ms)</t>
+  </si>
+  <si>
+    <t>k8s_2ng_1j_3r_4800t_600e_4cpu</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000%"/>
+    <numFmt numFmtId="171" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -897,7 +919,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -908,6 +930,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1223,10 +1246,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1D1567-5C01-D845-B094-708B919E4B92}">
-  <dimension ref="A1:U53"/>
+  <dimension ref="A1:W54"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="T10" sqref="T10"/>
+    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
+      <selection activeCell="V14" sqref="V14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1243,14 +1266,14 @@
     <col min="11" max="11" width="15" customWidth="1"/>
     <col min="12" max="13" width="21.1640625" customWidth="1"/>
     <col min="14" max="14" width="24.5" customWidth="1"/>
-    <col min="15" max="16" width="21.1640625" customWidth="1"/>
-    <col min="17" max="17" width="14.6640625" customWidth="1"/>
-    <col min="18" max="19" width="11.33203125" customWidth="1"/>
-    <col min="20" max="20" width="37.6640625" customWidth="1"/>
-    <col min="21" max="21" width="31.6640625" customWidth="1"/>
+    <col min="15" max="18" width="21.1640625" customWidth="1"/>
+    <col min="19" max="19" width="14.6640625" customWidth="1"/>
+    <col min="20" max="21" width="11.33203125" customWidth="1"/>
+    <col min="22" max="22" width="37.6640625" customWidth="1"/>
+    <col min="23" max="23" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="6" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" s="6" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>249</v>
       </c>
@@ -1264,7 +1287,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>244</v>
       </c>
@@ -1314,22 +1337,28 @@
         <v>138</v>
       </c>
       <c r="Q2" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="R2" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="S2" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="R2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="T2" t="s">
+      <c r="V2" t="s">
         <v>7</v>
       </c>
-      <c r="U2" t="s">
+      <c r="W2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1340,7 +1369,7 @@
         <v>173</v>
       </c>
       <c r="D3">
-        <v>9600</v>
+        <v>19200</v>
       </c>
       <c r="E3">
         <v>600</v>
@@ -1361,38 +1390,41 @@
         <v>186</v>
       </c>
       <c r="K3">
-        <v>999.47</v>
+        <v>994.96</v>
       </c>
       <c r="L3">
-        <v>689.52</v>
+        <v>1263.78</v>
       </c>
       <c r="M3">
-        <v>9334</v>
-      </c>
-      <c r="N3">
-        <v>35</v>
+        <v>11563</v>
+      </c>
+      <c r="N3" s="3">
+        <v>85</v>
       </c>
       <c r="O3">
-        <v>304</v>
+        <v>6388.95</v>
       </c>
       <c r="P3">
-        <v>535</v>
-      </c>
-      <c r="Q3">
-        <v>909782</v>
-      </c>
-      <c r="R3">
-        <v>0</v>
-      </c>
-      <c r="S3" s="7">
-        <f>R3/Q3</f>
-        <v>0</v>
-      </c>
-      <c r="T3" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.2">
+        <v>6853</v>
+      </c>
+      <c r="S3">
+        <v>915679</v>
+      </c>
+      <c r="T3">
+        <v>133</v>
+      </c>
+      <c r="U3" s="8">
+        <f t="shared" ref="U3:U13" si="0">T3/S3</f>
+        <v>1.4524740656933271E-4</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="W3" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1403,7 +1435,7 @@
         <v>173</v>
       </c>
       <c r="D4">
-        <v>4800</v>
+        <v>9600</v>
       </c>
       <c r="E4">
         <v>600</v>
@@ -1424,38 +1456,38 @@
         <v>186</v>
       </c>
       <c r="K4">
-        <v>997.84</v>
+        <v>999.47</v>
       </c>
       <c r="L4">
-        <v>361.26</v>
+        <v>689.52</v>
       </c>
       <c r="M4">
-        <v>3952</v>
+        <v>9334</v>
       </c>
       <c r="N4">
-        <v>65</v>
+        <v>35</v>
       </c>
       <c r="O4">
-        <v>116</v>
+        <v>304</v>
       </c>
       <c r="P4">
-        <v>236</v>
-      </c>
-      <c r="Q4">
-        <v>903334</v>
-      </c>
-      <c r="R4">
+        <v>535</v>
+      </c>
+      <c r="S4">
+        <v>909782</v>
+      </c>
+      <c r="T4">
         <v>0</v>
       </c>
-      <c r="S4" s="7">
-        <f>R4/Q4</f>
+      <c r="U4" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T4" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V4" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1487,41 +1519,38 @@
         <v>186</v>
       </c>
       <c r="K5">
-        <v>992.45</v>
+        <v>997.84</v>
       </c>
       <c r="L5">
-        <v>350.12</v>
+        <v>361.26</v>
       </c>
       <c r="M5">
-        <v>4931</v>
+        <v>3952</v>
       </c>
       <c r="N5">
-        <v>892</v>
+        <v>65</v>
       </c>
       <c r="O5">
-        <v>1858</v>
+        <v>116</v>
       </c>
       <c r="P5">
-        <v>1927</v>
-      </c>
-      <c r="Q5">
-        <v>899083</v>
-      </c>
-      <c r="R5">
+        <v>236</v>
+      </c>
+      <c r="S5">
+        <v>903334</v>
+      </c>
+      <c r="T5">
         <v>0</v>
       </c>
-      <c r="S5" s="7">
-        <f>R5/Q5</f>
+      <c r="U5" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T5" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="U5" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V5" s="1" t="s">
+        <v>253</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1532,7 +1561,7 @@
         <v>173</v>
       </c>
       <c r="D6">
-        <v>2400</v>
+        <v>4800</v>
       </c>
       <c r="E6">
         <v>600</v>
@@ -1553,38 +1582,41 @@
         <v>186</v>
       </c>
       <c r="K6">
-        <v>997.24</v>
+        <v>992.45</v>
       </c>
       <c r="L6">
-        <v>323.60000000000002</v>
+        <v>350.12</v>
       </c>
       <c r="M6">
-        <v>2039</v>
+        <v>4931</v>
       </c>
       <c r="N6">
-        <v>63</v>
+        <v>892</v>
       </c>
       <c r="O6">
-        <v>102</v>
+        <v>1858</v>
       </c>
       <c r="P6">
-        <v>135</v>
-      </c>
-      <c r="Q6">
-        <v>900303</v>
-      </c>
-      <c r="R6">
+        <v>1927</v>
+      </c>
+      <c r="S6">
+        <v>899083</v>
+      </c>
+      <c r="T6">
         <v>0</v>
       </c>
-      <c r="S6" s="7">
-        <f>R6/Q6</f>
+      <c r="U6" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T6" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V6" s="1" t="s">
+        <v>254</v>
+      </c>
+      <c r="W6" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1595,7 +1627,7 @@
         <v>173</v>
       </c>
       <c r="D7">
-        <v>1200</v>
+        <v>2400</v>
       </c>
       <c r="E7">
         <v>600</v>
@@ -1616,38 +1648,38 @@
         <v>186</v>
       </c>
       <c r="K7">
-        <v>997.36</v>
+        <v>997.24</v>
       </c>
       <c r="L7">
-        <v>175.85</v>
+        <v>323.60000000000002</v>
       </c>
       <c r="M7">
-        <v>844</v>
+        <v>2039</v>
       </c>
       <c r="N7">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="O7">
-        <v>512</v>
+        <v>102</v>
       </c>
       <c r="P7">
-        <v>567.99</v>
-      </c>
-      <c r="Q7">
-        <v>898286</v>
-      </c>
-      <c r="R7">
+        <v>135</v>
+      </c>
+      <c r="S7">
+        <v>900303</v>
+      </c>
+      <c r="T7">
         <v>0</v>
       </c>
-      <c r="S7" s="7">
-        <f>R7/Q7</f>
+      <c r="U7" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T7" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V7" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1658,7 +1690,7 @@
         <v>173</v>
       </c>
       <c r="D8">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="E8">
         <v>600</v>
@@ -1679,38 +1711,38 @@
         <v>186</v>
       </c>
       <c r="K8">
-        <v>994.77</v>
+        <v>997.36</v>
       </c>
       <c r="L8">
-        <v>95.03</v>
+        <v>175.85</v>
       </c>
       <c r="M8">
-        <v>520</v>
+        <v>844</v>
       </c>
       <c r="N8">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="O8">
-        <v>274</v>
+        <v>512</v>
       </c>
       <c r="P8">
-        <v>329</v>
-      </c>
-      <c r="Q8">
-        <v>895808</v>
-      </c>
-      <c r="R8">
+        <v>567.99</v>
+      </c>
+      <c r="S8">
+        <v>898286</v>
+      </c>
+      <c r="T8">
         <v>0</v>
       </c>
-      <c r="S8" s="7">
-        <f>R8/Q8</f>
+      <c r="U8" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T8" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="V8" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1721,7 +1753,7 @@
         <v>173</v>
       </c>
       <c r="D9">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E9">
         <v>600</v>
@@ -1742,177 +1774,405 @@
         <v>186</v>
       </c>
       <c r="K9">
+        <v>994.77</v>
+      </c>
+      <c r="L9">
+        <v>95.03</v>
+      </c>
+      <c r="M9">
+        <v>520</v>
+      </c>
+      <c r="N9">
+        <v>64</v>
+      </c>
+      <c r="O9">
+        <v>274</v>
+      </c>
+      <c r="P9">
+        <v>329</v>
+      </c>
+      <c r="S9">
+        <v>895808</v>
+      </c>
+      <c r="T9">
+        <v>0</v>
+      </c>
+      <c r="U9" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10">
+        <v>1</v>
+      </c>
+      <c r="B10">
+        <v>3</v>
+      </c>
+      <c r="C10" t="s">
+        <v>173</v>
+      </c>
+      <c r="D10">
+        <v>300</v>
+      </c>
+      <c r="E10">
+        <v>600</v>
+      </c>
+      <c r="F10" t="s">
+        <v>211</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+      <c r="H10">
+        <v>4</v>
+      </c>
+      <c r="I10">
+        <v>6</v>
+      </c>
+      <c r="J10" t="s">
+        <v>186</v>
+      </c>
+      <c r="K10">
         <v>996.89</v>
       </c>
-      <c r="L9">
+      <c r="L10">
         <v>71.040000000000006</v>
       </c>
-      <c r="M9">
+      <c r="M10">
         <v>330</v>
       </c>
-      <c r="N9">
+      <c r="N10">
         <v>63</v>
       </c>
-      <c r="O9">
+      <c r="O10">
         <v>113</v>
       </c>
-      <c r="P9">
+      <c r="P10">
         <v>164</v>
       </c>
-      <c r="Q9">
+      <c r="S10">
         <v>897305</v>
       </c>
-      <c r="R9">
+      <c r="T10">
         <v>0</v>
       </c>
-      <c r="S9" s="7">
-        <f>R9/Q9</f>
+      <c r="U10" s="7">
+        <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="T9" s="1" t="s">
+      <c r="V10" s="1" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="T10" s="1"/>
-    </row>
-    <row r="11" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="T11" s="1"/>
-    </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="T12" s="1"/>
-    </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="T13" s="1"/>
-    </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="T14" s="1"/>
-    </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="T15" s="1"/>
-    </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="T16" s="1"/>
-    </row>
-    <row r="17" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="T17" s="1"/>
-    </row>
-    <row r="18" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="T18" s="1"/>
-    </row>
-    <row r="19" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="T19" s="1"/>
-    </row>
-    <row r="20" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="T20" s="1"/>
-    </row>
-    <row r="21" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="T21" s="1"/>
-    </row>
-    <row r="22" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="S22" s="5"/>
-      <c r="T22" s="1"/>
-    </row>
-    <row r="23" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="S23" s="5"/>
-      <c r="T23" s="1"/>
-    </row>
-    <row r="24" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="S24" s="5"/>
-      <c r="T24" s="1"/>
-    </row>
-    <row r="25" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="S25" s="5"/>
-      <c r="T25" s="1"/>
-    </row>
-    <row r="26" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="S26" s="5"/>
-      <c r="T26" s="1"/>
-    </row>
-    <row r="27" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="S27" s="5"/>
-      <c r="T27" s="1"/>
-    </row>
-    <row r="28" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="S28" s="5"/>
-      <c r="T28" s="1"/>
-    </row>
-    <row r="29" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="S29" s="5"/>
-      <c r="T29" s="1"/>
-    </row>
-    <row r="30" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="S30" s="5"/>
-      <c r="T30" s="1"/>
-    </row>
-    <row r="31" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="S31" s="5"/>
-      <c r="T31" s="1"/>
-    </row>
-    <row r="32" spans="19:20" x14ac:dyDescent="0.2">
-      <c r="S32" s="5"/>
-      <c r="T32" s="1"/>
-    </row>
-    <row r="33" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="S33" s="5"/>
-      <c r="T33" s="1"/>
-    </row>
-    <row r="34" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="S34" s="5"/>
-      <c r="T34" s="1"/>
-    </row>
-    <row r="35" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="S35" s="5"/>
-      <c r="T35" s="1"/>
-    </row>
-    <row r="36" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="S36" s="5"/>
-      <c r="T36" s="1"/>
-    </row>
-    <row r="37" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="S37" s="5"/>
-      <c r="T37" s="1"/>
-    </row>
-    <row r="38" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="S38" s="5"/>
-      <c r="T38" s="1"/>
-      <c r="U38" s="6"/>
-    </row>
-    <row r="39" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="S39" s="5"/>
-      <c r="T39" s="1"/>
-    </row>
-    <row r="40" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="S40" s="5"/>
-      <c r="T40" s="1"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="S41" s="5"/>
-      <c r="T41" s="1"/>
-    </row>
-    <row r="42" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="S42" s="5"/>
-      <c r="T42" s="1"/>
-    </row>
-    <row r="43" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="A43" s="3"/>
-      <c r="B43" s="3"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="3"/>
-      <c r="E43" s="3"/>
-      <c r="F43" s="3"/>
-      <c r="G43" s="3"/>
-      <c r="H43" s="3"/>
-      <c r="I43" s="3"/>
-      <c r="J43" s="3"/>
-      <c r="M43" s="3"/>
-      <c r="N43" s="3"/>
-      <c r="O43" s="3"/>
-      <c r="P43" s="3"/>
-      <c r="S43" s="5"/>
-      <c r="T43" s="1"/>
-    </row>
-    <row r="44" spans="1:21" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11">
+        <v>1</v>
+      </c>
+      <c r="B11">
+        <v>3</v>
+      </c>
+      <c r="C11" t="s">
+        <v>173</v>
+      </c>
+      <c r="D11">
+        <v>19200</v>
+      </c>
+      <c r="E11">
+        <v>600</v>
+      </c>
+      <c r="F11" t="s">
+        <v>211</v>
+      </c>
+      <c r="G11">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>4</v>
+      </c>
+      <c r="I11">
+        <v>6</v>
+      </c>
+      <c r="J11" t="s">
+        <v>186</v>
+      </c>
+      <c r="K11">
+        <v>1015.9</v>
+      </c>
+      <c r="L11">
+        <v>2280.6799999999998</v>
+      </c>
+      <c r="M11">
+        <v>12474</v>
+      </c>
+      <c r="N11">
+        <v>255</v>
+      </c>
+      <c r="O11">
+        <v>4845</v>
+      </c>
+      <c r="P11">
+        <v>5355</v>
+      </c>
+      <c r="S11">
+        <v>933808</v>
+      </c>
+      <c r="T11">
+        <v>0</v>
+      </c>
+      <c r="U11" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V11" s="1" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12">
+        <v>1</v>
+      </c>
+      <c r="B12">
+        <v>3</v>
+      </c>
+      <c r="C12" t="s">
+        <v>173</v>
+      </c>
+      <c r="D12">
+        <v>9600</v>
+      </c>
+      <c r="E12">
+        <v>600</v>
+      </c>
+      <c r="F12" t="s">
+        <v>211</v>
+      </c>
+      <c r="G12">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>4</v>
+      </c>
+      <c r="I12">
+        <v>6</v>
+      </c>
+      <c r="J12" t="s">
+        <v>186</v>
+      </c>
+      <c r="K12">
+        <v>999.93</v>
+      </c>
+      <c r="L12">
+        <v>545.72</v>
+      </c>
+      <c r="M12">
+        <v>6965</v>
+      </c>
+      <c r="N12">
+        <v>61</v>
+      </c>
+      <c r="O12">
+        <v>242</v>
+      </c>
+      <c r="P12">
+        <v>375</v>
+      </c>
+      <c r="S12">
+        <v>914739</v>
+      </c>
+      <c r="T12">
+        <v>0</v>
+      </c>
+      <c r="U12" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V12" s="1" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A13">
+        <v>1</v>
+      </c>
+      <c r="B13">
+        <v>3</v>
+      </c>
+      <c r="C13" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13">
+        <v>4800</v>
+      </c>
+      <c r="E13">
+        <v>600</v>
+      </c>
+      <c r="F13" t="s">
+        <v>211</v>
+      </c>
+      <c r="G13">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>4</v>
+      </c>
+      <c r="I13">
+        <v>6</v>
+      </c>
+      <c r="J13" t="s">
+        <v>186</v>
+      </c>
+      <c r="K13">
+        <v>998.89</v>
+      </c>
+      <c r="L13">
+        <v>443.15</v>
+      </c>
+      <c r="M13">
+        <v>3530</v>
+      </c>
+      <c r="N13">
+        <v>65</v>
+      </c>
+      <c r="P13">
+        <v>112</v>
+      </c>
+      <c r="Q13">
+        <v>117</v>
+      </c>
+      <c r="R13">
+        <v>459.97</v>
+      </c>
+      <c r="S13">
+        <v>904625</v>
+      </c>
+      <c r="T13">
+        <v>0</v>
+      </c>
+      <c r="U13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="V13" s="1" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V14" s="1"/>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V15" s="1"/>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="V16" s="1"/>
+    </row>
+    <row r="17" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="V17" s="1"/>
+    </row>
+    <row r="18" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="V18" s="1"/>
+    </row>
+    <row r="19" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="V19" s="1"/>
+    </row>
+    <row r="20" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="V20" s="1"/>
+    </row>
+    <row r="21" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="V21" s="1"/>
+    </row>
+    <row r="22" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="V22" s="1"/>
+    </row>
+    <row r="23" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U23" s="5"/>
+      <c r="V23" s="1"/>
+    </row>
+    <row r="24" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U24" s="5"/>
+      <c r="V24" s="1"/>
+    </row>
+    <row r="25" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U25" s="5"/>
+      <c r="V25" s="1"/>
+    </row>
+    <row r="26" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U26" s="5"/>
+      <c r="V26" s="1"/>
+    </row>
+    <row r="27" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U27" s="5"/>
+      <c r="V27" s="1"/>
+    </row>
+    <row r="28" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U28" s="5"/>
+      <c r="V28" s="1"/>
+    </row>
+    <row r="29" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U29" s="5"/>
+      <c r="V29" s="1"/>
+    </row>
+    <row r="30" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U30" s="5"/>
+      <c r="V30" s="1"/>
+    </row>
+    <row r="31" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U31" s="5"/>
+      <c r="V31" s="1"/>
+    </row>
+    <row r="32" spans="21:22" x14ac:dyDescent="0.2">
+      <c r="U32" s="5"/>
+      <c r="V32" s="1"/>
+    </row>
+    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U33" s="5"/>
+      <c r="V33" s="1"/>
+    </row>
+    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U34" s="5"/>
+      <c r="V34" s="1"/>
+    </row>
+    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U35" s="5"/>
+      <c r="V35" s="1"/>
+    </row>
+    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U36" s="5"/>
+      <c r="V36" s="1"/>
+    </row>
+    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U37" s="5"/>
+      <c r="V37" s="1"/>
+    </row>
+    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U38" s="5"/>
+      <c r="V38" s="1"/>
+    </row>
+    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U39" s="5"/>
+      <c r="V39" s="1"/>
+      <c r="W39" s="6"/>
+    </row>
+    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U40" s="5"/>
+      <c r="V40" s="1"/>
+    </row>
+    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U41" s="5"/>
+      <c r="V41" s="1"/>
+    </row>
+    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U42" s="5"/>
+      <c r="V42" s="1"/>
+    </row>
+    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U43" s="5"/>
+      <c r="V43" s="1"/>
+    </row>
+    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A44" s="3"/>
       <c r="B44" s="3"/>
       <c r="C44" s="3"/>
@@ -1926,55 +2186,75 @@
       <c r="M44" s="3"/>
       <c r="N44" s="3"/>
       <c r="O44" s="3"/>
-      <c r="S44" s="5"/>
-      <c r="T44" s="1"/>
-    </row>
-    <row r="45" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="U44" s="5"/>
+      <c r="V44" s="1"/>
+    </row>
+    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A45" s="3"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="3"/>
+      <c r="D45" s="3"/>
+      <c r="E45" s="3"/>
+      <c r="F45" s="3"/>
+      <c r="G45" s="3"/>
+      <c r="H45" s="3"/>
+      <c r="I45" s="3"/>
+      <c r="J45" s="3"/>
+      <c r="M45" s="3"/>
       <c r="N45" s="3"/>
-      <c r="S45" s="5"/>
-      <c r="T45" s="1"/>
-    </row>
-    <row r="46" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="S46" s="5"/>
-      <c r="T46" s="1"/>
-    </row>
-    <row r="47" spans="1:21" x14ac:dyDescent="0.2">
-      <c r="N47" s="3"/>
-      <c r="S47" s="5"/>
-      <c r="T47" s="1"/>
-    </row>
-    <row r="48" spans="1:21" x14ac:dyDescent="0.2">
+      <c r="O45" s="3"/>
+      <c r="U45" s="5"/>
+      <c r="V45" s="1"/>
+    </row>
+    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="N46" s="3"/>
+      <c r="U46" s="5"/>
+      <c r="V46" s="1"/>
+    </row>
+    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U47" s="5"/>
+      <c r="V47" s="1"/>
+    </row>
+    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
       <c r="N48" s="3"/>
-      <c r="S48" s="5"/>
-      <c r="T48" s="1"/>
-    </row>
-    <row r="49" spans="14:20" x14ac:dyDescent="0.2">
+      <c r="U48" s="5"/>
+      <c r="V48" s="1"/>
+    </row>
+    <row r="49" spans="14:22" x14ac:dyDescent="0.2">
       <c r="N49" s="3"/>
-      <c r="S49" s="5"/>
-      <c r="T49" s="1"/>
-    </row>
-    <row r="50" spans="14:20" x14ac:dyDescent="0.2">
+      <c r="U49" s="5"/>
+      <c r="V49" s="1"/>
+    </row>
+    <row r="50" spans="14:22" x14ac:dyDescent="0.2">
       <c r="N50" s="3"/>
-      <c r="S50" s="5"/>
-      <c r="T50" s="1"/>
-    </row>
-    <row r="51" spans="14:20" x14ac:dyDescent="0.2">
+      <c r="U50" s="5"/>
+      <c r="V50" s="1"/>
+    </row>
+    <row r="51" spans="14:22" x14ac:dyDescent="0.2">
       <c r="N51" s="3"/>
-      <c r="S51" s="5"/>
-      <c r="T51" s="1"/>
-    </row>
-    <row r="52" spans="14:20" x14ac:dyDescent="0.2">
+      <c r="U51" s="5"/>
+      <c r="V51" s="1"/>
+    </row>
+    <row r="52" spans="14:22" x14ac:dyDescent="0.2">
       <c r="N52" s="3"/>
-      <c r="S52" s="5"/>
-      <c r="T52" s="1"/>
-    </row>
-    <row r="53" spans="14:20" x14ac:dyDescent="0.2">
+      <c r="U52" s="5"/>
+      <c r="V52" s="1"/>
+    </row>
+    <row r="53" spans="14:22" x14ac:dyDescent="0.2">
       <c r="N53" s="3"/>
-      <c r="S53" s="5"/>
-      <c r="T53" s="1"/>
+      <c r="U53" s="5"/>
+      <c r="V53" s="1"/>
+    </row>
+    <row r="54" spans="14:22" x14ac:dyDescent="0.2">
+      <c r="N54" s="3"/>
+      <c r="U54" s="5"/>
+      <c r="V54" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:U35" xr:uid="{0BCD43CD-D15C-C44C-860E-27B2AEF78201}"/>
+  <autoFilter ref="A2:W36" xr:uid="{0BCD43CD-D15C-C44C-860E-27B2AEF78201}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add authorize4 for webtest to enhance async performance, more test result
</commit_message>
<xml_diff>
--- a/kafka_benchmark/benchmark_stats.xlsx
+++ b/kafka_benchmark/benchmark_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lijjin/Documents/work/git_ws/redistest/kafka_benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C1C9311E-B9AC-E942-8967-57B9FB4B9BD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9E95E8-C3F7-0B43-BD25-6D591C82309F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{35590E01-C7C5-464A-8FB5-DBB7ECFA3BB7}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="600 executor" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Authz!$A$2:$W$36</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Authz!$A$2:$AB$41</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Kafka Producer'!$A$1:$AD$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2674" uniqueCount="267">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2755" uniqueCount="288">
   <si>
     <t>Partition</t>
   </si>
@@ -791,9 +791,6 @@
     <t>Heap (G)</t>
   </si>
   <si>
-    <t>k8s_1ng_1j_3r_9600t_600e_4cpu</t>
-  </si>
-  <si>
     <t>43679852 user-role mapping</t>
   </si>
   <si>
@@ -810,9 +807,6 @@
   </si>
   <si>
     <t>k8s_1ng_1j_3r_4800t_600e_4cpu.1</t>
-  </si>
-  <si>
-    <t>It seems that for 4800 concurrency, the response time is intermittently high</t>
   </si>
   <si>
     <t>k8s_1ng_1j_3r_2400t_600e_4cpu</t>
@@ -846,6 +840,75 @@
   </si>
   <si>
     <t>k8s_2ng_1j_3r_4800t_600e_4cpu</t>
+  </si>
+  <si>
+    <t>JVM CPU #</t>
+  </si>
+  <si>
+    <t>JVM Heap (G)</t>
+  </si>
+  <si>
+    <t>GW Request CPU</t>
+  </si>
+  <si>
+    <t>8G</t>
+  </si>
+  <si>
+    <t>90M</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_19200t_600e_4cpu_ngenhance</t>
+  </si>
+  <si>
+    <t>Nginx Worker #</t>
+  </si>
+  <si>
+    <t>Upstream Keepalive #/Worker</t>
+  </si>
+  <si>
+    <t>It seems that for 4800 concurrency, the response time is mostly high, intermittently low</t>
+  </si>
+  <si>
+    <t>Sync/Async</t>
+  </si>
+  <si>
+    <t>Async</t>
+  </si>
+  <si>
+    <t>Sync</t>
+  </si>
+  <si>
+    <t>sync_k8s_1ng_1j_3r_300t_600e_4cpu</t>
+  </si>
+  <si>
+    <t>Async2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_300t_600e_4cpu_async2</t>
+  </si>
+  <si>
+    <t>Async uses authorize, Async2 uses authorize4, Sync uses authorize0</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_19200t_600e_4cpu_async2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_4800t_600e_4cpu_async2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_2400t_600e_4cpu_async2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_1200t_600e_4cpu_async2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_600t_600e_4cpu_async2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_9600t_600e_4cpu.2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_9600t_600e_4cpu_async2.1</t>
   </si>
 </sst>
 </file>
@@ -1246,10 +1309,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1D1567-5C01-D845-B094-708B919E4B92}">
-  <dimension ref="A1:W54"/>
+  <dimension ref="A1:AB59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L1" workbookViewId="0">
-      <selection activeCell="V14" sqref="V14"/>
+    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J5" sqref="J5:K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1259,35 +1322,38 @@
     <col min="4" max="4" width="17.33203125" customWidth="1"/>
     <col min="5" max="5" width="12.83203125" customWidth="1"/>
     <col min="6" max="6" width="15.83203125" customWidth="1"/>
-    <col min="7" max="7" width="11.83203125" customWidth="1"/>
+    <col min="7" max="7" width="11.33203125" customWidth="1"/>
     <col min="8" max="8" width="9.1640625" customWidth="1"/>
-    <col min="9" max="9" width="9" customWidth="1"/>
-    <col min="10" max="10" width="16.33203125" customWidth="1"/>
-    <col min="11" max="11" width="15" customWidth="1"/>
-    <col min="12" max="13" width="21.1640625" customWidth="1"/>
-    <col min="14" max="14" width="24.5" customWidth="1"/>
-    <col min="15" max="18" width="21.1640625" customWidth="1"/>
-    <col min="19" max="19" width="14.6640625" customWidth="1"/>
-    <col min="20" max="21" width="11.33203125" customWidth="1"/>
-    <col min="22" max="22" width="37.6640625" customWidth="1"/>
-    <col min="23" max="23" width="31.6640625" customWidth="1"/>
+    <col min="9" max="11" width="9" customWidth="1"/>
+    <col min="12" max="15" width="12" customWidth="1"/>
+    <col min="16" max="16" width="15" customWidth="1"/>
+    <col min="17" max="18" width="21.1640625" customWidth="1"/>
+    <col min="19" max="19" width="24.5" customWidth="1"/>
+    <col min="20" max="23" width="21.1640625" customWidth="1"/>
+    <col min="24" max="24" width="14.6640625" customWidth="1"/>
+    <col min="25" max="26" width="11.33203125" customWidth="1"/>
+    <col min="27" max="27" width="37.6640625" customWidth="1"/>
+    <col min="28" max="28" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="6" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:28" s="6" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
+        <v>248</v>
+      </c>
+      <c r="B1" s="6" t="s">
         <v>249</v>
       </c>
-      <c r="B1" s="6" t="s">
+      <c r="C1" s="6" t="s">
         <v>250</v>
       </c>
-      <c r="C1" s="6" t="s">
+      <c r="D1" s="6" t="s">
         <v>251</v>
       </c>
-      <c r="D1" s="6" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="E1" s="6" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>244</v>
       </c>
@@ -1310,55 +1376,67 @@
         <v>198</v>
       </c>
       <c r="H2" t="s">
-        <v>210</v>
+        <v>265</v>
       </c>
       <c r="I2" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="J2" t="s">
+        <v>267</v>
+      </c>
+      <c r="L2" t="s">
         <v>184</v>
       </c>
-      <c r="K2" t="s">
+      <c r="M2" t="s">
+        <v>271</v>
+      </c>
+      <c r="N2" t="s">
+        <v>272</v>
+      </c>
+      <c r="O2" t="s">
+        <v>274</v>
+      </c>
+      <c r="P2" t="s">
         <v>129</v>
       </c>
-      <c r="L2" t="s">
+      <c r="Q2" t="s">
         <v>134</v>
       </c>
-      <c r="M2" t="s">
+      <c r="R2" t="s">
         <v>135</v>
       </c>
-      <c r="N2" s="3" t="s">
+      <c r="S2" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="O2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="P2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="Q2" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="R2" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="S2" s="3" t="s">
+      <c r="V2" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="X2" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="V2" t="s">
+      <c r="AA2" t="s">
         <v>7</v>
       </c>
-      <c r="W2" t="s">
+      <c r="AB2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1386,45 +1464,61 @@
       <c r="I3">
         <v>6</v>
       </c>
-      <c r="J3" t="s">
+      <c r="J3">
+        <v>4</v>
+      </c>
+      <c r="K3" t="s">
+        <v>268</v>
+      </c>
+      <c r="L3" t="s">
         <v>186</v>
       </c>
-      <c r="K3">
-        <v>994.96</v>
-      </c>
-      <c r="L3">
-        <v>1263.78</v>
-      </c>
       <c r="M3">
-        <v>11563</v>
-      </c>
-      <c r="N3" s="3">
-        <v>85</v>
-      </c>
-      <c r="O3">
-        <v>6388.95</v>
+        <v>16</v>
+      </c>
+      <c r="N3">
+        <v>320</v>
+      </c>
+      <c r="O3" t="s">
+        <v>275</v>
       </c>
       <c r="P3">
-        <v>6853</v>
+        <v>1000.51</v>
+      </c>
+      <c r="Q3">
+        <v>1437.21</v>
+      </c>
+      <c r="R3">
+        <v>11377</v>
       </c>
       <c r="S3">
-        <v>915679</v>
-      </c>
-      <c r="T3">
-        <v>133</v>
-      </c>
-      <c r="U3" s="8">
-        <f t="shared" ref="U3:U13" si="0">T3/S3</f>
-        <v>1.4524740656933271E-4</v>
-      </c>
-      <c r="V3" s="1" t="s">
-        <v>260</v>
-      </c>
-      <c r="W3" t="s">
-        <v>261</v>
-      </c>
-    </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+        <v>3098</v>
+      </c>
+      <c r="T3" s="3"/>
+      <c r="U3">
+        <v>5381.99</v>
+      </c>
+      <c r="V3">
+        <v>6223</v>
+      </c>
+      <c r="W3">
+        <v>6314.99</v>
+      </c>
+      <c r="X3">
+        <v>917790</v>
+      </c>
+      <c r="Y3" s="3">
+        <v>0</v>
+      </c>
+      <c r="Z3" s="8">
+        <f t="shared" ref="Z3:Z22" si="0">Y3/X3</f>
+        <v>0</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1435,7 +1529,7 @@
         <v>173</v>
       </c>
       <c r="D4">
-        <v>9600</v>
+        <v>19200</v>
       </c>
       <c r="E4">
         <v>600</v>
@@ -1452,42 +1546,60 @@
       <c r="I4">
         <v>6</v>
       </c>
-      <c r="J4" t="s">
+      <c r="J4">
+        <v>0.1</v>
+      </c>
+      <c r="K4" t="s">
+        <v>269</v>
+      </c>
+      <c r="L4" t="s">
         <v>186</v>
       </c>
-      <c r="K4">
-        <v>999.47</v>
-      </c>
-      <c r="L4">
-        <v>689.52</v>
-      </c>
       <c r="M4">
-        <v>9334</v>
+        <v>16</v>
       </c>
       <c r="N4">
-        <v>35</v>
-      </c>
-      <c r="O4">
-        <v>304</v>
+        <v>320</v>
+      </c>
+      <c r="O4" t="s">
+        <v>275</v>
       </c>
       <c r="P4">
-        <v>535</v>
-      </c>
-      <c r="S4">
-        <v>909782</v>
+        <v>994.96</v>
+      </c>
+      <c r="Q4">
+        <v>1263.78</v>
+      </c>
+      <c r="R4">
+        <v>11563</v>
+      </c>
+      <c r="S4" s="3">
+        <v>85</v>
       </c>
       <c r="T4">
-        <v>0</v>
-      </c>
-      <c r="U4" s="7">
+        <v>6388.95</v>
+      </c>
+      <c r="U4">
+        <v>6853</v>
+      </c>
+      <c r="X4">
+        <v>915679</v>
+      </c>
+      <c r="Y4">
+        <v>133</v>
+      </c>
+      <c r="Z4" s="8">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>248</v>
-      </c>
-    </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
+        <v>1.4524740656933271E-4</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="AB4" t="s">
+        <v>259</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1498,7 +1610,7 @@
         <v>173</v>
       </c>
       <c r="D5">
-        <v>4800</v>
+        <v>9600</v>
       </c>
       <c r="E5">
         <v>600</v>
@@ -1515,42 +1627,60 @@
       <c r="I5">
         <v>6</v>
       </c>
-      <c r="J5" t="s">
+      <c r="J5" s="3">
+        <v>4</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>268</v>
+      </c>
+      <c r="L5" t="s">
         <v>186</v>
       </c>
-      <c r="K5">
-        <v>997.84</v>
-      </c>
-      <c r="L5">
-        <v>361.26</v>
-      </c>
       <c r="M5">
-        <v>3952</v>
+        <v>16</v>
       </c>
       <c r="N5">
-        <v>65</v>
-      </c>
-      <c r="O5">
-        <v>116</v>
+        <v>320</v>
+      </c>
+      <c r="O5" t="s">
+        <v>275</v>
       </c>
       <c r="P5">
-        <v>236</v>
+        <v>999.99</v>
+      </c>
+      <c r="Q5">
+        <v>684.69</v>
+      </c>
+      <c r="R5">
+        <v>6792</v>
       </c>
       <c r="S5">
-        <v>903334</v>
-      </c>
-      <c r="T5">
-        <v>0</v>
-      </c>
-      <c r="U5" s="7">
+        <v>240</v>
+      </c>
+      <c r="U5">
+        <v>3527</v>
+      </c>
+      <c r="V5">
+        <v>3564</v>
+      </c>
+      <c r="W5">
+        <v>4128</v>
+      </c>
+      <c r="X5">
+        <v>909719</v>
+      </c>
+      <c r="Y5">
+        <v>0</v>
+      </c>
+      <c r="Z5" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V5" s="1" t="s">
-        <v>253</v>
-      </c>
-    </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AA5" s="1" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1578,45 +1708,57 @@
       <c r="I6">
         <v>6</v>
       </c>
-      <c r="J6" t="s">
+      <c r="J6">
+        <v>0.1</v>
+      </c>
+      <c r="K6" t="s">
+        <v>269</v>
+      </c>
+      <c r="L6" t="s">
         <v>186</v>
       </c>
-      <c r="K6">
-        <v>992.45</v>
-      </c>
-      <c r="L6">
-        <v>350.12</v>
-      </c>
       <c r="M6">
-        <v>4931</v>
+        <v>16</v>
       </c>
       <c r="N6">
-        <v>892</v>
-      </c>
-      <c r="O6">
-        <v>1858</v>
+        <v>320</v>
+      </c>
+      <c r="O6" t="s">
+        <v>275</v>
       </c>
       <c r="P6">
-        <v>1927</v>
+        <v>997.84</v>
+      </c>
+      <c r="Q6">
+        <v>361.26</v>
+      </c>
+      <c r="R6">
+        <v>3952</v>
       </c>
       <c r="S6">
-        <v>899083</v>
+        <v>65</v>
       </c>
       <c r="T6">
-        <v>0</v>
-      </c>
-      <c r="U6" s="7">
+        <v>116</v>
+      </c>
+      <c r="U6">
+        <v>236</v>
+      </c>
+      <c r="X6">
+        <v>903334</v>
+      </c>
+      <c r="Y6">
+        <v>0</v>
+      </c>
+      <c r="Z6" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V6" s="1" t="s">
-        <v>254</v>
-      </c>
-      <c r="W6" t="s">
-        <v>255</v>
-      </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AA6" s="1" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1627,7 +1769,7 @@
         <v>173</v>
       </c>
       <c r="D7">
-        <v>2400</v>
+        <v>4800</v>
       </c>
       <c r="E7">
         <v>600</v>
@@ -1644,42 +1786,60 @@
       <c r="I7">
         <v>6</v>
       </c>
-      <c r="J7" t="s">
+      <c r="J7">
+        <v>0.1</v>
+      </c>
+      <c r="K7" t="s">
+        <v>269</v>
+      </c>
+      <c r="L7" t="s">
         <v>186</v>
       </c>
-      <c r="K7">
-        <v>997.24</v>
-      </c>
-      <c r="L7">
-        <v>323.60000000000002</v>
-      </c>
       <c r="M7">
-        <v>2039</v>
+        <v>16</v>
       </c>
       <c r="N7">
-        <v>63</v>
-      </c>
-      <c r="O7">
-        <v>102</v>
+        <v>320</v>
+      </c>
+      <c r="O7" t="s">
+        <v>275</v>
       </c>
       <c r="P7">
-        <v>135</v>
+        <v>992.45</v>
+      </c>
+      <c r="Q7">
+        <v>350.12</v>
+      </c>
+      <c r="R7">
+        <v>4931</v>
       </c>
       <c r="S7">
-        <v>900303</v>
+        <v>892</v>
       </c>
       <c r="T7">
-        <v>0</v>
-      </c>
-      <c r="U7" s="7">
+        <v>1858</v>
+      </c>
+      <c r="U7">
+        <v>1927</v>
+      </c>
+      <c r="X7">
+        <v>899083</v>
+      </c>
+      <c r="Y7">
+        <v>0</v>
+      </c>
+      <c r="Z7" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V7" s="1" t="s">
-        <v>256</v>
-      </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AA7" s="1" t="s">
+        <v>253</v>
+      </c>
+      <c r="AB7" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1690,7 +1850,7 @@
         <v>173</v>
       </c>
       <c r="D8">
-        <v>1200</v>
+        <v>2400</v>
       </c>
       <c r="E8">
         <v>600</v>
@@ -1707,42 +1867,60 @@
       <c r="I8">
         <v>6</v>
       </c>
-      <c r="J8" t="s">
+      <c r="J8">
+        <v>0.1</v>
+      </c>
+      <c r="K8" t="s">
+        <v>269</v>
+      </c>
+      <c r="L8" t="s">
         <v>186</v>
       </c>
-      <c r="K8">
-        <v>997.36</v>
-      </c>
-      <c r="L8">
-        <v>175.85</v>
-      </c>
       <c r="M8">
-        <v>844</v>
+        <v>16</v>
       </c>
       <c r="N8">
-        <v>73</v>
-      </c>
-      <c r="O8">
-        <v>512</v>
+        <v>320</v>
+      </c>
+      <c r="O8" t="s">
+        <v>275</v>
       </c>
       <c r="P8">
-        <v>567.99</v>
+        <v>999.27</v>
+      </c>
+      <c r="Q8">
+        <v>296.02</v>
+      </c>
+      <c r="R8">
+        <v>2501</v>
       </c>
       <c r="S8">
-        <v>898286</v>
-      </c>
-      <c r="T8">
-        <v>0</v>
-      </c>
-      <c r="U8" s="7">
+        <v>347</v>
+      </c>
+      <c r="U8">
+        <v>1087</v>
+      </c>
+      <c r="V8">
+        <v>1118</v>
+      </c>
+      <c r="W8">
+        <v>1125</v>
+      </c>
+      <c r="X8">
+        <v>900120</v>
+      </c>
+      <c r="Y8">
+        <v>0</v>
+      </c>
+      <c r="Z8" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V8" s="1" t="s">
-        <v>257</v>
-      </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AA8" s="1" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1753,7 +1931,7 @@
         <v>173</v>
       </c>
       <c r="D9">
-        <v>600</v>
+        <v>1200</v>
       </c>
       <c r="E9">
         <v>600</v>
@@ -1770,42 +1948,57 @@
       <c r="I9">
         <v>6</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J9">
+        <v>0.1</v>
+      </c>
+      <c r="K9" t="s">
+        <v>269</v>
+      </c>
+      <c r="L9" t="s">
         <v>186</v>
       </c>
-      <c r="K9">
-        <v>994.77</v>
-      </c>
-      <c r="L9">
-        <v>95.03</v>
-      </c>
       <c r="M9">
-        <v>520</v>
+        <v>16</v>
       </c>
       <c r="N9">
-        <v>64</v>
-      </c>
-      <c r="O9">
-        <v>274</v>
+        <v>320</v>
+      </c>
+      <c r="O9" t="s">
+        <v>275</v>
       </c>
       <c r="P9">
-        <v>329</v>
+        <v>997.36</v>
+      </c>
+      <c r="Q9">
+        <v>175.85</v>
+      </c>
+      <c r="R9">
+        <v>844</v>
       </c>
       <c r="S9">
-        <v>895808</v>
+        <v>73</v>
       </c>
       <c r="T9">
-        <v>0</v>
-      </c>
-      <c r="U9" s="7">
+        <v>512</v>
+      </c>
+      <c r="U9">
+        <v>567.99</v>
+      </c>
+      <c r="X9">
+        <v>898286</v>
+      </c>
+      <c r="Y9">
+        <v>0</v>
+      </c>
+      <c r="Z9" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V9" s="1" t="s">
-        <v>258</v>
-      </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AA9" s="1" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -1816,7 +2009,7 @@
         <v>173</v>
       </c>
       <c r="D10">
-        <v>300</v>
+        <v>600</v>
       </c>
       <c r="E10">
         <v>600</v>
@@ -1833,42 +2026,57 @@
       <c r="I10">
         <v>6</v>
       </c>
-      <c r="J10" t="s">
+      <c r="J10">
+        <v>0.1</v>
+      </c>
+      <c r="K10" t="s">
+        <v>269</v>
+      </c>
+      <c r="L10" t="s">
         <v>186</v>
       </c>
-      <c r="K10">
-        <v>996.89</v>
-      </c>
-      <c r="L10">
-        <v>71.040000000000006</v>
-      </c>
       <c r="M10">
-        <v>330</v>
+        <v>16</v>
       </c>
       <c r="N10">
-        <v>63</v>
-      </c>
-      <c r="O10">
-        <v>113</v>
+        <v>320</v>
+      </c>
+      <c r="O10" t="s">
+        <v>275</v>
       </c>
       <c r="P10">
-        <v>164</v>
+        <v>994.77</v>
+      </c>
+      <c r="Q10">
+        <v>95.03</v>
+      </c>
+      <c r="R10">
+        <v>520</v>
       </c>
       <c r="S10">
-        <v>897305</v>
+        <v>64</v>
       </c>
       <c r="T10">
-        <v>0</v>
-      </c>
-      <c r="U10" s="7">
+        <v>274</v>
+      </c>
+      <c r="U10">
+        <v>329</v>
+      </c>
+      <c r="X10">
+        <v>895808</v>
+      </c>
+      <c r="Y10">
+        <v>0</v>
+      </c>
+      <c r="Z10" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V10" s="1" t="s">
-        <v>259</v>
-      </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AA10" s="1" t="s">
+        <v>256</v>
+      </c>
+    </row>
+    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -1879,7 +2087,7 @@
         <v>173</v>
       </c>
       <c r="D11">
-        <v>19200</v>
+        <v>300</v>
       </c>
       <c r="E11">
         <v>600</v>
@@ -1888,7 +2096,7 @@
         <v>211</v>
       </c>
       <c r="G11">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="H11">
         <v>4</v>
@@ -1896,42 +2104,57 @@
       <c r="I11">
         <v>6</v>
       </c>
-      <c r="J11" t="s">
+      <c r="J11">
+        <v>0.1</v>
+      </c>
+      <c r="K11" t="s">
+        <v>269</v>
+      </c>
+      <c r="L11" t="s">
         <v>186</v>
       </c>
-      <c r="K11">
-        <v>1015.9</v>
-      </c>
-      <c r="L11">
-        <v>2280.6799999999998</v>
-      </c>
       <c r="M11">
-        <v>12474</v>
+        <v>16</v>
       </c>
       <c r="N11">
-        <v>255</v>
-      </c>
-      <c r="O11">
-        <v>4845</v>
+        <v>320</v>
+      </c>
+      <c r="O11" t="s">
+        <v>275</v>
       </c>
       <c r="P11">
-        <v>5355</v>
+        <v>996.89</v>
+      </c>
+      <c r="Q11">
+        <v>71.040000000000006</v>
+      </c>
+      <c r="R11">
+        <v>330</v>
       </c>
       <c r="S11">
-        <v>933808</v>
+        <v>63</v>
       </c>
       <c r="T11">
-        <v>0</v>
-      </c>
-      <c r="U11" s="7">
+        <v>113</v>
+      </c>
+      <c r="U11">
+        <v>164</v>
+      </c>
+      <c r="X11">
+        <v>897305</v>
+      </c>
+      <c r="Y11">
+        <v>0</v>
+      </c>
+      <c r="Z11" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V11" s="1" t="s">
-        <v>262</v>
-      </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AA11" s="1" t="s">
+        <v>257</v>
+      </c>
+    </row>
+    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -1942,7 +2165,7 @@
         <v>173</v>
       </c>
       <c r="D12">
-        <v>9600</v>
+        <v>19200</v>
       </c>
       <c r="E12">
         <v>600</v>
@@ -1959,42 +2182,57 @@
       <c r="I12">
         <v>6</v>
       </c>
-      <c r="J12" t="s">
+      <c r="J12">
+        <v>0.1</v>
+      </c>
+      <c r="K12" t="s">
+        <v>269</v>
+      </c>
+      <c r="L12" t="s">
         <v>186</v>
       </c>
-      <c r="K12">
-        <v>999.93</v>
-      </c>
-      <c r="L12">
-        <v>545.72</v>
-      </c>
       <c r="M12">
-        <v>6965</v>
+        <v>16</v>
       </c>
       <c r="N12">
-        <v>61</v>
-      </c>
-      <c r="O12">
-        <v>242</v>
+        <v>320</v>
+      </c>
+      <c r="O12" t="s">
+        <v>275</v>
       </c>
       <c r="P12">
-        <v>375</v>
+        <v>1015.9</v>
+      </c>
+      <c r="Q12">
+        <v>2280.6799999999998</v>
+      </c>
+      <c r="R12">
+        <v>12474</v>
       </c>
       <c r="S12">
-        <v>914739</v>
+        <v>255</v>
       </c>
       <c r="T12">
-        <v>0</v>
-      </c>
-      <c r="U12" s="7">
+        <v>4845</v>
+      </c>
+      <c r="U12">
+        <v>5355</v>
+      </c>
+      <c r="X12">
+        <v>933808</v>
+      </c>
+      <c r="Y12">
+        <v>0</v>
+      </c>
+      <c r="Z12" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V12" s="1" t="s">
-        <v>263</v>
-      </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="AA12" s="1" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2005,7 +2243,7 @@
         <v>173</v>
       </c>
       <c r="D13">
-        <v>4800</v>
+        <v>9600</v>
       </c>
       <c r="E13">
         <v>600</v>
@@ -2022,239 +2260,978 @@
       <c r="I13">
         <v>6</v>
       </c>
-      <c r="J13" t="s">
+      <c r="J13">
+        <v>0.1</v>
+      </c>
+      <c r="K13" t="s">
+        <v>269</v>
+      </c>
+      <c r="L13" t="s">
         <v>186</v>
       </c>
-      <c r="K13">
+      <c r="M13">
+        <v>16</v>
+      </c>
+      <c r="N13">
+        <v>320</v>
+      </c>
+      <c r="O13" t="s">
+        <v>275</v>
+      </c>
+      <c r="P13">
+        <v>999.93</v>
+      </c>
+      <c r="Q13">
+        <v>545.72</v>
+      </c>
+      <c r="R13">
+        <v>6965</v>
+      </c>
+      <c r="S13">
+        <v>61</v>
+      </c>
+      <c r="T13">
+        <v>242</v>
+      </c>
+      <c r="U13">
+        <v>375</v>
+      </c>
+      <c r="X13">
+        <v>914739</v>
+      </c>
+      <c r="Y13">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA13" s="1" t="s">
+        <v>261</v>
+      </c>
+    </row>
+    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A14">
+        <v>1</v>
+      </c>
+      <c r="B14">
+        <v>3</v>
+      </c>
+      <c r="C14" t="s">
+        <v>173</v>
+      </c>
+      <c r="D14">
+        <v>4800</v>
+      </c>
+      <c r="E14">
+        <v>600</v>
+      </c>
+      <c r="F14" t="s">
+        <v>211</v>
+      </c>
+      <c r="G14">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>4</v>
+      </c>
+      <c r="I14">
+        <v>6</v>
+      </c>
+      <c r="J14">
+        <v>0.1</v>
+      </c>
+      <c r="K14" t="s">
+        <v>269</v>
+      </c>
+      <c r="L14" t="s">
+        <v>186</v>
+      </c>
+      <c r="M14">
+        <v>16</v>
+      </c>
+      <c r="N14">
+        <v>320</v>
+      </c>
+      <c r="O14" t="s">
+        <v>275</v>
+      </c>
+      <c r="P14">
         <v>998.89</v>
       </c>
-      <c r="L13">
+      <c r="Q14">
         <v>443.15</v>
       </c>
-      <c r="M13">
+      <c r="R14">
         <v>3530</v>
       </c>
-      <c r="N13">
+      <c r="S14">
         <v>65</v>
       </c>
-      <c r="P13">
+      <c r="U14">
         <v>112</v>
       </c>
-      <c r="Q13">
+      <c r="V14">
         <v>117</v>
       </c>
-      <c r="R13">
+      <c r="W14">
         <v>459.97</v>
       </c>
-      <c r="S13">
+      <c r="X14">
         <v>904625</v>
       </c>
-      <c r="T13">
-        <v>0</v>
-      </c>
-      <c r="U13" s="7">
+      <c r="Y14">
+        <v>0</v>
+      </c>
+      <c r="Z14" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="V13" s="1" t="s">
-        <v>266</v>
-      </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="V14" s="1"/>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="V15" s="1"/>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="V16" s="1"/>
-    </row>
-    <row r="17" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="V17" s="1"/>
-    </row>
-    <row r="18" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="V18" s="1"/>
-    </row>
-    <row r="19" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="V19" s="1"/>
-    </row>
-    <row r="20" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="V20" s="1"/>
-    </row>
-    <row r="21" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="V21" s="1"/>
-    </row>
-    <row r="22" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="V22" s="1"/>
-    </row>
-    <row r="23" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="U23" s="5"/>
-      <c r="V23" s="1"/>
-    </row>
-    <row r="24" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="U24" s="5"/>
-      <c r="V24" s="1"/>
-    </row>
-    <row r="25" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="U25" s="5"/>
-      <c r="V25" s="1"/>
-    </row>
-    <row r="26" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="U26" s="5"/>
-      <c r="V26" s="1"/>
-    </row>
-    <row r="27" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="U27" s="5"/>
-      <c r="V27" s="1"/>
-    </row>
-    <row r="28" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="U28" s="5"/>
-      <c r="V28" s="1"/>
-    </row>
-    <row r="29" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="U29" s="5"/>
-      <c r="V29" s="1"/>
-    </row>
-    <row r="30" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="U30" s="5"/>
-      <c r="V30" s="1"/>
-    </row>
-    <row r="31" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="U31" s="5"/>
-      <c r="V31" s="1"/>
-    </row>
-    <row r="32" spans="21:22" x14ac:dyDescent="0.2">
-      <c r="U32" s="5"/>
-      <c r="V32" s="1"/>
-    </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U33" s="5"/>
-      <c r="V33" s="1"/>
-    </row>
-    <row r="34" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U34" s="5"/>
-      <c r="V34" s="1"/>
-    </row>
-    <row r="35" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U35" s="5"/>
-      <c r="V35" s="1"/>
-    </row>
-    <row r="36" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U36" s="5"/>
-      <c r="V36" s="1"/>
-    </row>
-    <row r="37" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U37" s="5"/>
-      <c r="V37" s="1"/>
-    </row>
-    <row r="38" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U38" s="5"/>
-      <c r="V38" s="1"/>
-    </row>
-    <row r="39" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U39" s="5"/>
-      <c r="V39" s="1"/>
-      <c r="W39" s="6"/>
-    </row>
-    <row r="40" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U40" s="5"/>
-      <c r="V40" s="1"/>
-    </row>
-    <row r="41" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U41" s="5"/>
-      <c r="V41" s="1"/>
-    </row>
-    <row r="42" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U42" s="5"/>
-      <c r="V42" s="1"/>
-    </row>
-    <row r="43" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U43" s="5"/>
-      <c r="V43" s="1"/>
-    </row>
-    <row r="44" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A44" s="3"/>
-      <c r="B44" s="3"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="3"/>
-      <c r="E44" s="3"/>
-      <c r="F44" s="3"/>
-      <c r="G44" s="3"/>
-      <c r="H44" s="3"/>
-      <c r="I44" s="3"/>
-      <c r="J44" s="3"/>
-      <c r="M44" s="3"/>
-      <c r="N44" s="3"/>
-      <c r="O44" s="3"/>
-      <c r="P44" s="3"/>
-      <c r="Q44" s="3"/>
-      <c r="R44" s="3"/>
-      <c r="U44" s="5"/>
-      <c r="V44" s="1"/>
-    </row>
-    <row r="45" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="A45" s="3"/>
-      <c r="B45" s="3"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="3"/>
-      <c r="E45" s="3"/>
-      <c r="F45" s="3"/>
-      <c r="G45" s="3"/>
-      <c r="H45" s="3"/>
-      <c r="I45" s="3"/>
-      <c r="J45" s="3"/>
-      <c r="M45" s="3"/>
-      <c r="N45" s="3"/>
-      <c r="O45" s="3"/>
-      <c r="U45" s="5"/>
-      <c r="V45" s="1"/>
-    </row>
-    <row r="46" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="N46" s="3"/>
-      <c r="U46" s="5"/>
-      <c r="V46" s="1"/>
-    </row>
-    <row r="47" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="U47" s="5"/>
-      <c r="V47" s="1"/>
-    </row>
-    <row r="48" spans="1:23" x14ac:dyDescent="0.2">
-      <c r="N48" s="3"/>
-      <c r="U48" s="5"/>
-      <c r="V48" s="1"/>
-    </row>
-    <row r="49" spans="14:22" x14ac:dyDescent="0.2">
+      <c r="AA14" s="1" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A15">
+        <v>1</v>
+      </c>
+      <c r="B15">
+        <v>3</v>
+      </c>
+      <c r="C15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D15">
+        <v>300</v>
+      </c>
+      <c r="E15">
+        <v>600</v>
+      </c>
+      <c r="F15" t="s">
+        <v>211</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+      <c r="H15">
+        <v>4</v>
+      </c>
+      <c r="I15">
+        <v>6</v>
+      </c>
+      <c r="J15">
+        <v>0.1</v>
+      </c>
+      <c r="K15" t="s">
+        <v>269</v>
+      </c>
+      <c r="L15" t="s">
+        <v>186</v>
+      </c>
+      <c r="M15">
+        <v>16</v>
+      </c>
+      <c r="N15">
+        <v>320</v>
+      </c>
+      <c r="O15" t="s">
+        <v>276</v>
+      </c>
+      <c r="P15">
+        <v>632.79</v>
+      </c>
+      <c r="Q15">
+        <v>303.64</v>
+      </c>
+      <c r="R15">
+        <v>5665</v>
+      </c>
+      <c r="S15">
+        <v>26</v>
+      </c>
+      <c r="U15">
+        <v>315.99</v>
+      </c>
+      <c r="V15">
+        <v>474</v>
+      </c>
+      <c r="W15">
+        <v>582</v>
+      </c>
+      <c r="X15">
+        <v>569571</v>
+      </c>
+      <c r="Y15">
+        <v>0</v>
+      </c>
+      <c r="Z15" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA15" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A16">
+        <v>1</v>
+      </c>
+      <c r="B16">
+        <v>3</v>
+      </c>
+      <c r="C16" t="s">
+        <v>173</v>
+      </c>
+      <c r="D16">
+        <v>300</v>
+      </c>
+      <c r="E16">
+        <v>600</v>
+      </c>
+      <c r="F16" t="s">
+        <v>211</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+      <c r="H16">
+        <v>4</v>
+      </c>
+      <c r="I16">
+        <v>6</v>
+      </c>
+      <c r="J16">
+        <v>4</v>
+      </c>
+      <c r="K16" t="s">
+        <v>268</v>
+      </c>
+      <c r="L16" t="s">
+        <v>186</v>
+      </c>
+      <c r="M16">
+        <v>16</v>
+      </c>
+      <c r="N16">
+        <v>320</v>
+      </c>
+      <c r="O16" t="s">
+        <v>278</v>
+      </c>
+      <c r="P16">
+        <v>996.18</v>
+      </c>
+      <c r="Q16">
+        <v>26.24</v>
+      </c>
+      <c r="R16">
+        <v>215</v>
+      </c>
+      <c r="S16">
+        <v>21</v>
+      </c>
+      <c r="U16">
+        <v>122</v>
+      </c>
+      <c r="V16">
+        <v>144</v>
+      </c>
+      <c r="W16">
+        <v>151</v>
+      </c>
+      <c r="X16">
+        <v>896683</v>
+      </c>
+      <c r="Y16">
+        <v>0</v>
+      </c>
+      <c r="Z16" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA16" s="1" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A17" s="3">
+        <v>1</v>
+      </c>
+      <c r="B17" s="3">
+        <v>3</v>
+      </c>
+      <c r="C17" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D17" s="3">
+        <v>600</v>
+      </c>
+      <c r="E17" s="3">
+        <v>600</v>
+      </c>
+      <c r="F17" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1</v>
+      </c>
+      <c r="H17" s="3">
+        <v>4</v>
+      </c>
+      <c r="I17" s="3">
+        <v>6</v>
+      </c>
+      <c r="J17">
+        <v>4</v>
+      </c>
+      <c r="K17" t="s">
+        <v>268</v>
+      </c>
+      <c r="L17" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="M17" s="3">
+        <v>16</v>
+      </c>
+      <c r="N17" s="3">
+        <v>320</v>
+      </c>
+      <c r="O17" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="P17">
+        <v>996.61</v>
+      </c>
+      <c r="Q17">
+        <v>41.68</v>
+      </c>
+      <c r="R17" s="3">
+        <v>348</v>
+      </c>
+      <c r="S17" s="3">
+        <v>23</v>
+      </c>
+      <c r="U17">
+        <v>270</v>
+      </c>
+      <c r="V17">
+        <v>304</v>
+      </c>
+      <c r="W17">
+        <v>312</v>
+      </c>
+      <c r="X17">
+        <v>897508</v>
+      </c>
+      <c r="Y17">
+        <v>0</v>
+      </c>
+      <c r="Z17" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA17" s="1" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A18" s="3">
+        <v>1</v>
+      </c>
+      <c r="B18" s="3">
+        <v>3</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1200</v>
+      </c>
+      <c r="E18" s="3">
+        <v>600</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1</v>
+      </c>
+      <c r="H18" s="3">
+        <v>4</v>
+      </c>
+      <c r="I18" s="3">
+        <v>6</v>
+      </c>
+      <c r="J18">
+        <v>4</v>
+      </c>
+      <c r="K18" t="s">
+        <v>268</v>
+      </c>
+      <c r="L18" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="M18" s="3">
+        <v>16</v>
+      </c>
+      <c r="N18" s="3">
+        <v>320</v>
+      </c>
+      <c r="O18" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="P18">
+        <v>996.53</v>
+      </c>
+      <c r="Q18">
+        <v>91.06</v>
+      </c>
+      <c r="R18">
+        <v>1070</v>
+      </c>
+      <c r="S18">
+        <v>27</v>
+      </c>
+      <c r="U18">
+        <v>417</v>
+      </c>
+      <c r="V18">
+        <v>442</v>
+      </c>
+      <c r="W18">
+        <v>446</v>
+      </c>
+      <c r="X18">
+        <v>898225</v>
+      </c>
+      <c r="Y18">
+        <v>0</v>
+      </c>
+      <c r="Z18" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA18" s="1" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A19" s="3">
+        <v>1</v>
+      </c>
+      <c r="B19" s="3">
+        <v>3</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>173</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2400</v>
+      </c>
+      <c r="E19" s="3">
+        <v>600</v>
+      </c>
+      <c r="F19" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1</v>
+      </c>
+      <c r="H19" s="3">
+        <v>4</v>
+      </c>
+      <c r="I19" s="3">
+        <v>6</v>
+      </c>
+      <c r="J19">
+        <v>4</v>
+      </c>
+      <c r="K19" t="s">
+        <v>268</v>
+      </c>
+      <c r="L19" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="M19" s="3">
+        <v>16</v>
+      </c>
+      <c r="N19" s="3">
+        <v>320</v>
+      </c>
+      <c r="O19" s="3" t="s">
+        <v>278</v>
+      </c>
+      <c r="P19">
+        <v>997.26</v>
+      </c>
+      <c r="Q19">
+        <v>212.8</v>
+      </c>
+      <c r="R19">
+        <v>3066</v>
+      </c>
+      <c r="S19">
+        <v>287</v>
+      </c>
+      <c r="U19">
+        <v>860</v>
+      </c>
+      <c r="V19">
+        <v>888</v>
+      </c>
+      <c r="W19">
+        <v>898</v>
+      </c>
+      <c r="X19">
+        <v>901434</v>
+      </c>
+      <c r="Y19">
+        <v>0</v>
+      </c>
+      <c r="Z19" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA19" s="1" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A20">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>173</v>
+      </c>
+      <c r="D20">
+        <v>4800</v>
+      </c>
+      <c r="E20">
+        <v>600</v>
+      </c>
+      <c r="F20" t="s">
+        <v>211</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+      <c r="H20">
+        <v>4</v>
+      </c>
+      <c r="I20">
+        <v>6</v>
+      </c>
+      <c r="J20">
+        <v>4</v>
+      </c>
+      <c r="K20" t="s">
+        <v>268</v>
+      </c>
+      <c r="L20" t="s">
+        <v>186</v>
+      </c>
+      <c r="M20">
+        <v>16</v>
+      </c>
+      <c r="N20">
+        <v>320</v>
+      </c>
+      <c r="O20" t="s">
+        <v>278</v>
+      </c>
+      <c r="P20">
+        <v>999.91</v>
+      </c>
+      <c r="Q20">
+        <v>356.87</v>
+      </c>
+      <c r="R20">
+        <v>3087</v>
+      </c>
+      <c r="S20">
+        <v>119</v>
+      </c>
+      <c r="U20">
+        <v>1646</v>
+      </c>
+      <c r="V20">
+        <v>1684</v>
+      </c>
+      <c r="W20">
+        <v>1694</v>
+      </c>
+      <c r="X20">
+        <v>904721</v>
+      </c>
+      <c r="Y20">
+        <v>0</v>
+      </c>
+      <c r="Z20" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA20" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A21">
+        <v>1</v>
+      </c>
+      <c r="B21">
+        <v>3</v>
+      </c>
+      <c r="C21" t="s">
+        <v>173</v>
+      </c>
+      <c r="D21">
+        <v>9600</v>
+      </c>
+      <c r="E21">
+        <v>600</v>
+      </c>
+      <c r="F21" t="s">
+        <v>211</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+      <c r="H21">
+        <v>4</v>
+      </c>
+      <c r="I21">
+        <v>6</v>
+      </c>
+      <c r="J21">
+        <v>4</v>
+      </c>
+      <c r="K21" t="s">
+        <v>268</v>
+      </c>
+      <c r="L21" t="s">
+        <v>186</v>
+      </c>
+      <c r="M21">
+        <v>16</v>
+      </c>
+      <c r="N21">
+        <v>320</v>
+      </c>
+      <c r="O21" t="s">
+        <v>278</v>
+      </c>
+      <c r="P21">
+        <v>993.99</v>
+      </c>
+      <c r="Q21">
+        <v>587.75</v>
+      </c>
+      <c r="R21">
+        <v>4946</v>
+      </c>
+      <c r="S21">
+        <v>25</v>
+      </c>
+      <c r="U21">
+        <v>2142</v>
+      </c>
+      <c r="V21">
+        <v>2201</v>
+      </c>
+      <c r="W21">
+        <v>4159</v>
+      </c>
+      <c r="X21">
+        <v>902995</v>
+      </c>
+      <c r="Y21">
+        <v>0</v>
+      </c>
+      <c r="Z21" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA21" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A22">
+        <v>1</v>
+      </c>
+      <c r="B22">
+        <v>3</v>
+      </c>
+      <c r="C22" t="s">
+        <v>173</v>
+      </c>
+      <c r="D22">
+        <v>19200</v>
+      </c>
+      <c r="E22">
+        <v>600</v>
+      </c>
+      <c r="F22" t="s">
+        <v>211</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+      <c r="H22">
+        <v>4</v>
+      </c>
+      <c r="I22">
+        <v>6</v>
+      </c>
+      <c r="J22">
+        <v>4</v>
+      </c>
+      <c r="K22" t="s">
+        <v>268</v>
+      </c>
+      <c r="L22" t="s">
+        <v>186</v>
+      </c>
+      <c r="M22">
+        <v>16</v>
+      </c>
+      <c r="N22">
+        <v>320</v>
+      </c>
+      <c r="O22" t="s">
+        <v>278</v>
+      </c>
+      <c r="P22">
+        <v>981.93</v>
+      </c>
+      <c r="Q22">
+        <v>1209.79</v>
+      </c>
+      <c r="R22">
+        <v>9932</v>
+      </c>
+      <c r="S22">
+        <v>35</v>
+      </c>
+      <c r="U22">
+        <v>5715</v>
+      </c>
+      <c r="V22">
+        <v>5785</v>
+      </c>
+      <c r="W22">
+        <v>5791</v>
+      </c>
+      <c r="X22">
+        <v>906691</v>
+      </c>
+      <c r="Y22">
+        <v>0</v>
+      </c>
+      <c r="Z22" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AA22" s="1" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA23" s="1"/>
+    </row>
+    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA24" s="1"/>
+    </row>
+    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA25" s="1"/>
+    </row>
+    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA26" s="1"/>
+    </row>
+    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="AA27" s="1"/>
+    </row>
+    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Z28" s="5"/>
+      <c r="AA28" s="1"/>
+    </row>
+    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Z29" s="5"/>
+      <c r="AA29" s="1"/>
+    </row>
+    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Z30" s="5"/>
+      <c r="AA30" s="1"/>
+    </row>
+    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Z31" s="5"/>
+      <c r="AA31" s="1"/>
+    </row>
+    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Z32" s="5"/>
+      <c r="AA32" s="1"/>
+    </row>
+    <row r="33" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z33" s="5"/>
+      <c r="AA33" s="1"/>
+    </row>
+    <row r="34" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z34" s="5"/>
+      <c r="AA34" s="1"/>
+    </row>
+    <row r="35" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z35" s="5"/>
+      <c r="AA35" s="1"/>
+    </row>
+    <row r="36" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z36" s="5"/>
+      <c r="AA36" s="1"/>
+    </row>
+    <row r="37" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z37" s="5"/>
+      <c r="AA37" s="1"/>
+    </row>
+    <row r="38" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z38" s="5"/>
+      <c r="AA38" s="1"/>
+    </row>
+    <row r="39" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z39" s="5"/>
+      <c r="AA39" s="1"/>
+    </row>
+    <row r="40" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z40" s="5"/>
+      <c r="AA40" s="1"/>
+    </row>
+    <row r="41" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z41" s="5"/>
+      <c r="AA41" s="1"/>
+    </row>
+    <row r="42" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z42" s="5"/>
+      <c r="AA42" s="1"/>
+    </row>
+    <row r="43" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z43" s="5"/>
+      <c r="AA43" s="1"/>
+    </row>
+    <row r="44" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z44" s="5"/>
+      <c r="AA44" s="1"/>
+      <c r="AB44" s="6"/>
+    </row>
+    <row r="45" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z45" s="5"/>
+      <c r="AA45" s="1"/>
+    </row>
+    <row r="46" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z46" s="5"/>
+      <c r="AA46" s="1"/>
+    </row>
+    <row r="47" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z47" s="5"/>
+      <c r="AA47" s="1"/>
+    </row>
+    <row r="48" spans="26:28" x14ac:dyDescent="0.2">
+      <c r="Z48" s="5"/>
+      <c r="AA48" s="1"/>
+    </row>
+    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A49" s="3"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="3"/>
+      <c r="D49" s="3"/>
+      <c r="E49" s="3"/>
+      <c r="F49" s="3"/>
+      <c r="G49" s="3"/>
+      <c r="H49" s="3"/>
+      <c r="I49" s="3"/>
+      <c r="J49" s="3"/>
+      <c r="K49" s="3"/>
+      <c r="L49" s="3"/>
+      <c r="M49" s="3"/>
       <c r="N49" s="3"/>
-      <c r="U49" s="5"/>
-      <c r="V49" s="1"/>
-    </row>
-    <row r="50" spans="14:22" x14ac:dyDescent="0.2">
+      <c r="O49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3"/>
+      <c r="T49" s="3"/>
+      <c r="U49" s="3"/>
+      <c r="V49" s="3"/>
+      <c r="W49" s="3"/>
+      <c r="Z49" s="5"/>
+      <c r="AA49" s="1"/>
+    </row>
+    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="A50" s="3"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
+      <c r="E50" s="3"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="3"/>
+      <c r="H50" s="3"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="3"/>
+      <c r="L50" s="3"/>
+      <c r="M50" s="3"/>
       <c r="N50" s="3"/>
-      <c r="U50" s="5"/>
-      <c r="V50" s="1"/>
-    </row>
-    <row r="51" spans="14:22" x14ac:dyDescent="0.2">
-      <c r="N51" s="3"/>
-      <c r="U51" s="5"/>
-      <c r="V51" s="1"/>
-    </row>
-    <row r="52" spans="14:22" x14ac:dyDescent="0.2">
-      <c r="N52" s="3"/>
-      <c r="U52" s="5"/>
-      <c r="V52" s="1"/>
-    </row>
-    <row r="53" spans="14:22" x14ac:dyDescent="0.2">
-      <c r="N53" s="3"/>
-      <c r="U53" s="5"/>
-      <c r="V53" s="1"/>
-    </row>
-    <row r="54" spans="14:22" x14ac:dyDescent="0.2">
-      <c r="N54" s="3"/>
-      <c r="U54" s="5"/>
-      <c r="V54" s="1"/>
+      <c r="O50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3"/>
+      <c r="T50" s="3"/>
+      <c r="Z50" s="5"/>
+      <c r="AA50" s="1"/>
+    </row>
+    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="S51" s="3"/>
+      <c r="Z51" s="5"/>
+      <c r="AA51" s="1"/>
+    </row>
+    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="Z52" s="5"/>
+      <c r="AA52" s="1"/>
+    </row>
+    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="S53" s="3"/>
+      <c r="Z53" s="5"/>
+      <c r="AA53" s="1"/>
+    </row>
+    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="S54" s="3"/>
+      <c r="Z54" s="5"/>
+      <c r="AA54" s="1"/>
+    </row>
+    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="S55" s="3"/>
+      <c r="Z55" s="5"/>
+      <c r="AA55" s="1"/>
+    </row>
+    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="S56" s="3"/>
+      <c r="Z56" s="5"/>
+      <c r="AA56" s="1"/>
+    </row>
+    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="S57" s="3"/>
+      <c r="Z57" s="5"/>
+      <c r="AA57" s="1"/>
+    </row>
+    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="S58" s="3"/>
+      <c r="Z58" s="5"/>
+      <c r="AA58" s="1"/>
+    </row>
+    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="S59" s="3"/>
+      <c r="Z59" s="5"/>
+      <c r="AA59" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:W36" xr:uid="{0BCD43CD-D15C-C44C-860E-27B2AEF78201}"/>
+  <autoFilter ref="A2:AB41" xr:uid="{0BCD43CD-D15C-C44C-860E-27B2AEF78201}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
more log, customize http connection logic, disable http2
</commit_message>
<xml_diff>
--- a/kafka_benchmark/benchmark_stats.xlsx
+++ b/kafka_benchmark/benchmark_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lijjin/Documents/work/git_ws/redistest/kafka_benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA9E95E8-C3F7-0B43-BD25-6D591C82309F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E5BC3E-43BD-004E-925B-75D70F27CCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{35590E01-C7C5-464A-8FB5-DBB7ECFA3BB7}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="600 executor" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Authz!$A$2:$AB$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Authz!$A$2:$AC$42</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Kafka Producer'!$A$1:$AD$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2755" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2847" uniqueCount="303">
   <si>
     <t>Partition</t>
   </si>
@@ -909,6 +909,51 @@
   </si>
   <si>
     <t>k8s_1ng_1j_3r_9600t_600e_4cpu_async2.1</t>
+  </si>
+  <si>
+    <t>http 1.1</t>
+  </si>
+  <si>
+    <t>https 1.1</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_9600t_600e_4cpu_async2_https</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_19200t_600e_4cpu_async2_https</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_4800t_600e_4cpu_async2_https</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_1200t_600e_4cpu_async2_https</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_600t_600e_4cpu_async2_https.1</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_300t_600e_4cpu_async2_https</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_2400t_600e_4cpu_async2_https.2</t>
+  </si>
+  <si>
+    <t>GW Protocol</t>
+  </si>
+  <si>
+    <t>https 2.0</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_300t_600e_4cpu_async2_https_http2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_600t_600e_4cpu_async2_https_http2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_1000t_600e_4cpu_async2_https_http2</t>
+  </si>
+  <si>
+    <t>client -(http2 or http1.1/https)-&gt;Nginx-(http1.1/http)-&gt;service</t>
   </si>
 </sst>
 </file>
@@ -1309,10 +1354,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1D1567-5C01-D845-B094-708B919E4B92}">
-  <dimension ref="A1:AB59"/>
+  <dimension ref="A1:AC60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" workbookViewId="0">
-      <selection activeCell="J5" sqref="J5:K5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1326,17 +1371,18 @@
     <col min="8" max="8" width="9.1640625" customWidth="1"/>
     <col min="9" max="11" width="9" customWidth="1"/>
     <col min="12" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="15" customWidth="1"/>
-    <col min="17" max="18" width="21.1640625" customWidth="1"/>
-    <col min="19" max="19" width="24.5" customWidth="1"/>
-    <col min="20" max="23" width="21.1640625" customWidth="1"/>
-    <col min="24" max="24" width="14.6640625" customWidth="1"/>
-    <col min="25" max="26" width="11.33203125" customWidth="1"/>
-    <col min="27" max="27" width="37.6640625" customWidth="1"/>
-    <col min="28" max="28" width="31.6640625" customWidth="1"/>
+    <col min="16" max="16" width="9.33203125" customWidth="1"/>
+    <col min="17" max="17" width="15" customWidth="1"/>
+    <col min="18" max="19" width="21.1640625" customWidth="1"/>
+    <col min="20" max="20" width="24.5" customWidth="1"/>
+    <col min="21" max="24" width="21.1640625" customWidth="1"/>
+    <col min="25" max="25" width="14.6640625" customWidth="1"/>
+    <col min="26" max="27" width="11.33203125" customWidth="1"/>
+    <col min="28" max="28" width="37.6640625" customWidth="1"/>
+    <col min="29" max="29" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" s="6" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:29" s="6" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>248</v>
       </c>
@@ -1352,8 +1398,11 @@
       <c r="E1" s="6" t="s">
         <v>280</v>
       </c>
-    </row>
-    <row r="2" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="F1" s="6" t="s">
+        <v>302</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>244</v>
       </c>
@@ -1397,46 +1446,49 @@
         <v>274</v>
       </c>
       <c r="P2" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q2" t="s">
         <v>129</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="R2" t="s">
         <v>134</v>
       </c>
-      <c r="R2" t="s">
+      <c r="S2" t="s">
         <v>135</v>
       </c>
-      <c r="S2" s="3" t="s">
+      <c r="T2" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="U2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>7</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AC2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1482,43 +1534,46 @@
       <c r="O3" t="s">
         <v>275</v>
       </c>
-      <c r="P3">
+      <c r="P3" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q3">
         <v>1000.51</v>
       </c>
-      <c r="Q3">
+      <c r="R3">
         <v>1437.21</v>
       </c>
-      <c r="R3">
+      <c r="S3">
         <v>11377</v>
       </c>
-      <c r="S3">
+      <c r="T3">
         <v>3098</v>
       </c>
-      <c r="T3" s="3"/>
-      <c r="U3">
+      <c r="U3" s="3"/>
+      <c r="V3">
         <v>5381.99</v>
       </c>
-      <c r="V3">
+      <c r="W3">
         <v>6223</v>
       </c>
-      <c r="W3">
+      <c r="X3">
         <v>6314.99</v>
       </c>
-      <c r="X3">
+      <c r="Y3">
         <v>917790</v>
       </c>
-      <c r="Y3" s="3">
-        <v>0</v>
-      </c>
-      <c r="Z3" s="8">
-        <f t="shared" ref="Z3:Z22" si="0">Y3/X3</f>
-        <v>0</v>
-      </c>
-      <c r="AA3" s="1" t="s">
+      <c r="Z3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="8">
+        <f t="shared" ref="AA3:AA32" si="0">Z3/Y3</f>
+        <v>0</v>
+      </c>
+      <c r="AB3" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1564,42 +1619,45 @@
       <c r="O4" t="s">
         <v>275</v>
       </c>
-      <c r="P4">
+      <c r="P4" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q4">
         <v>994.96</v>
       </c>
-      <c r="Q4">
+      <c r="R4">
         <v>1263.78</v>
       </c>
-      <c r="R4">
+      <c r="S4">
         <v>11563</v>
       </c>
-      <c r="S4" s="3">
+      <c r="T4" s="3">
         <v>85</v>
       </c>
-      <c r="T4">
+      <c r="U4">
         <v>6388.95</v>
       </c>
-      <c r="U4">
+      <c r="V4">
         <v>6853</v>
       </c>
-      <c r="X4">
+      <c r="Y4">
         <v>915679</v>
       </c>
-      <c r="Y4">
+      <c r="Z4">
         <v>133</v>
       </c>
-      <c r="Z4" s="8">
+      <c r="AA4" s="8">
         <f t="shared" si="0"/>
         <v>1.4524740656933271E-4</v>
       </c>
-      <c r="AA4" s="1" t="s">
+      <c r="AB4" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="AB4" t="s">
+      <c r="AC4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1645,42 +1703,45 @@
       <c r="O5" t="s">
         <v>275</v>
       </c>
-      <c r="P5">
+      <c r="P5" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q5">
         <v>999.99</v>
       </c>
-      <c r="Q5">
+      <c r="R5">
         <v>684.69</v>
       </c>
-      <c r="R5">
+      <c r="S5">
         <v>6792</v>
       </c>
-      <c r="S5">
+      <c r="T5">
         <v>240</v>
       </c>
-      <c r="U5">
+      <c r="V5">
         <v>3527</v>
       </c>
-      <c r="V5">
+      <c r="W5">
         <v>3564</v>
       </c>
-      <c r="W5">
+      <c r="X5">
         <v>4128</v>
       </c>
-      <c r="X5">
+      <c r="Y5">
         <v>909719</v>
       </c>
-      <c r="Y5">
-        <v>0</v>
-      </c>
-      <c r="Z5" s="7">
+      <c r="Z5">
+        <v>0</v>
+      </c>
+      <c r="AA5" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA5" s="1" t="s">
+      <c r="AB5" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1726,39 +1787,42 @@
       <c r="O6" t="s">
         <v>275</v>
       </c>
-      <c r="P6">
+      <c r="P6" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q6">
         <v>997.84</v>
       </c>
-      <c r="Q6">
+      <c r="R6">
         <v>361.26</v>
       </c>
-      <c r="R6">
+      <c r="S6">
         <v>3952</v>
       </c>
-      <c r="S6">
+      <c r="T6">
         <v>65</v>
       </c>
-      <c r="T6">
+      <c r="U6">
         <v>116</v>
       </c>
-      <c r="U6">
+      <c r="V6">
         <v>236</v>
       </c>
-      <c r="X6">
+      <c r="Y6">
         <v>903334</v>
       </c>
-      <c r="Y6">
-        <v>0</v>
-      </c>
-      <c r="Z6" s="7">
+      <c r="Z6">
+        <v>0</v>
+      </c>
+      <c r="AA6" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA6" s="1" t="s">
+      <c r="AB6" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="7" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1804,42 +1868,45 @@
       <c r="O7" t="s">
         <v>275</v>
       </c>
-      <c r="P7">
+      <c r="P7" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q7">
         <v>992.45</v>
       </c>
-      <c r="Q7">
+      <c r="R7">
         <v>350.12</v>
       </c>
-      <c r="R7">
+      <c r="S7">
         <v>4931</v>
       </c>
-      <c r="S7">
+      <c r="T7">
         <v>892</v>
       </c>
-      <c r="T7">
+      <c r="U7">
         <v>1858</v>
       </c>
-      <c r="U7">
+      <c r="V7">
         <v>1927</v>
       </c>
-      <c r="X7">
+      <c r="Y7">
         <v>899083</v>
       </c>
-      <c r="Y7">
-        <v>0</v>
-      </c>
-      <c r="Z7" s="7">
+      <c r="Z7">
+        <v>0</v>
+      </c>
+      <c r="AA7" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA7" s="1" t="s">
+      <c r="AB7" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="AB7" t="s">
+      <c r="AC7" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1885,42 +1952,45 @@
       <c r="O8" t="s">
         <v>275</v>
       </c>
-      <c r="P8">
+      <c r="P8" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q8">
         <v>999.27</v>
       </c>
-      <c r="Q8">
+      <c r="R8">
         <v>296.02</v>
       </c>
-      <c r="R8">
+      <c r="S8">
         <v>2501</v>
       </c>
-      <c r="S8">
+      <c r="T8">
         <v>347</v>
       </c>
-      <c r="U8">
+      <c r="V8">
         <v>1087</v>
       </c>
-      <c r="V8">
+      <c r="W8">
         <v>1118</v>
       </c>
-      <c r="W8">
+      <c r="X8">
         <v>1125</v>
       </c>
-      <c r="X8">
+      <c r="Y8">
         <v>900120</v>
       </c>
-      <c r="Y8">
-        <v>0</v>
-      </c>
-      <c r="Z8" s="7">
+      <c r="Z8">
+        <v>0</v>
+      </c>
+      <c r="AA8" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA8" s="1" t="s">
+      <c r="AB8" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="9" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1966,39 +2036,42 @@
       <c r="O9" t="s">
         <v>275</v>
       </c>
-      <c r="P9">
+      <c r="P9" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q9">
         <v>997.36</v>
       </c>
-      <c r="Q9">
+      <c r="R9">
         <v>175.85</v>
       </c>
-      <c r="R9">
+      <c r="S9">
         <v>844</v>
       </c>
-      <c r="S9">
+      <c r="T9">
         <v>73</v>
       </c>
-      <c r="T9">
+      <c r="U9">
         <v>512</v>
       </c>
-      <c r="U9">
+      <c r="V9">
         <v>567.99</v>
       </c>
-      <c r="X9">
+      <c r="Y9">
         <v>898286</v>
       </c>
-      <c r="Y9">
-        <v>0</v>
-      </c>
-      <c r="Z9" s="7">
+      <c r="Z9">
+        <v>0</v>
+      </c>
+      <c r="AA9" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA9" s="1" t="s">
+      <c r="AB9" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="10" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2044,39 +2117,42 @@
       <c r="O10" t="s">
         <v>275</v>
       </c>
-      <c r="P10">
+      <c r="P10" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q10">
         <v>994.77</v>
       </c>
-      <c r="Q10">
+      <c r="R10">
         <v>95.03</v>
       </c>
-      <c r="R10">
+      <c r="S10">
         <v>520</v>
       </c>
-      <c r="S10">
+      <c r="T10">
         <v>64</v>
       </c>
-      <c r="T10">
+      <c r="U10">
         <v>274</v>
       </c>
-      <c r="U10">
+      <c r="V10">
         <v>329</v>
       </c>
-      <c r="X10">
+      <c r="Y10">
         <v>895808</v>
       </c>
-      <c r="Y10">
-        <v>0</v>
-      </c>
-      <c r="Z10" s="7">
+      <c r="Z10">
+        <v>0</v>
+      </c>
+      <c r="AA10" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA10" s="1" t="s">
+      <c r="AB10" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2122,39 +2198,42 @@
       <c r="O11" t="s">
         <v>275</v>
       </c>
-      <c r="P11">
+      <c r="P11" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q11">
         <v>996.89</v>
       </c>
-      <c r="Q11">
+      <c r="R11">
         <v>71.040000000000006</v>
       </c>
-      <c r="R11">
+      <c r="S11">
         <v>330</v>
       </c>
-      <c r="S11">
+      <c r="T11">
         <v>63</v>
       </c>
-      <c r="T11">
+      <c r="U11">
         <v>113</v>
       </c>
-      <c r="U11">
+      <c r="V11">
         <v>164</v>
       </c>
-      <c r="X11">
+      <c r="Y11">
         <v>897305</v>
       </c>
-      <c r="Y11">
-        <v>0</v>
-      </c>
-      <c r="Z11" s="7">
+      <c r="Z11">
+        <v>0</v>
+      </c>
+      <c r="AA11" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA11" s="1" t="s">
+      <c r="AB11" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2200,39 +2279,42 @@
       <c r="O12" t="s">
         <v>275</v>
       </c>
-      <c r="P12">
+      <c r="P12" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q12">
         <v>1015.9</v>
       </c>
-      <c r="Q12">
+      <c r="R12">
         <v>2280.6799999999998</v>
       </c>
-      <c r="R12">
+      <c r="S12">
         <v>12474</v>
       </c>
-      <c r="S12">
+      <c r="T12">
         <v>255</v>
       </c>
-      <c r="T12">
+      <c r="U12">
         <v>4845</v>
       </c>
-      <c r="U12">
+      <c r="V12">
         <v>5355</v>
       </c>
-      <c r="X12">
+      <c r="Y12">
         <v>933808</v>
       </c>
-      <c r="Y12">
-        <v>0</v>
-      </c>
-      <c r="Z12" s="7">
+      <c r="Z12">
+        <v>0</v>
+      </c>
+      <c r="AA12" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA12" s="1" t="s">
+      <c r="AB12" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="13" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2278,39 +2360,42 @@
       <c r="O13" t="s">
         <v>275</v>
       </c>
-      <c r="P13">
+      <c r="P13" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q13">
         <v>999.93</v>
       </c>
-      <c r="Q13">
+      <c r="R13">
         <v>545.72</v>
       </c>
-      <c r="R13">
+      <c r="S13">
         <v>6965</v>
       </c>
-      <c r="S13">
+      <c r="T13">
         <v>61</v>
       </c>
-      <c r="T13">
+      <c r="U13">
         <v>242</v>
       </c>
-      <c r="U13">
+      <c r="V13">
         <v>375</v>
       </c>
-      <c r="X13">
+      <c r="Y13">
         <v>914739</v>
       </c>
-      <c r="Y13">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="7">
+      <c r="Z13">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA13" s="1" t="s">
+      <c r="AB13" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2356,42 +2441,45 @@
       <c r="O14" t="s">
         <v>275</v>
       </c>
-      <c r="P14">
+      <c r="P14" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q14">
         <v>998.89</v>
       </c>
-      <c r="Q14">
+      <c r="R14">
         <v>443.15</v>
       </c>
-      <c r="R14">
+      <c r="S14">
         <v>3530</v>
       </c>
-      <c r="S14">
+      <c r="T14">
         <v>65</v>
       </c>
-      <c r="U14">
+      <c r="V14">
         <v>112</v>
       </c>
-      <c r="V14">
+      <c r="W14">
         <v>117</v>
       </c>
-      <c r="W14">
+      <c r="X14">
         <v>459.97</v>
       </c>
-      <c r="X14">
+      <c r="Y14">
         <v>904625</v>
       </c>
-      <c r="Y14">
-        <v>0</v>
-      </c>
-      <c r="Z14" s="7">
+      <c r="Z14">
+        <v>0</v>
+      </c>
+      <c r="AA14" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA14" s="1" t="s">
+      <c r="AB14" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2437,42 +2525,45 @@
       <c r="O15" t="s">
         <v>276</v>
       </c>
-      <c r="P15">
+      <c r="P15" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q15">
         <v>632.79</v>
       </c>
-      <c r="Q15">
+      <c r="R15">
         <v>303.64</v>
       </c>
-      <c r="R15">
+      <c r="S15">
         <v>5665</v>
       </c>
-      <c r="S15">
+      <c r="T15">
         <v>26</v>
       </c>
-      <c r="U15">
+      <c r="V15">
         <v>315.99</v>
       </c>
-      <c r="V15">
+      <c r="W15">
         <v>474</v>
       </c>
-      <c r="W15">
+      <c r="X15">
         <v>582</v>
       </c>
-      <c r="X15">
+      <c r="Y15">
         <v>569571</v>
       </c>
-      <c r="Y15">
-        <v>0</v>
-      </c>
-      <c r="Z15" s="7">
+      <c r="Z15">
+        <v>0</v>
+      </c>
+      <c r="AA15" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA15" s="1" t="s">
+      <c r="AB15" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="16" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2518,42 +2609,45 @@
       <c r="O16" t="s">
         <v>278</v>
       </c>
-      <c r="P16">
+      <c r="P16" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q16">
         <v>996.18</v>
       </c>
-      <c r="Q16">
+      <c r="R16">
         <v>26.24</v>
       </c>
-      <c r="R16">
+      <c r="S16">
         <v>215</v>
       </c>
-      <c r="S16">
+      <c r="T16">
         <v>21</v>
       </c>
-      <c r="U16">
+      <c r="V16">
         <v>122</v>
       </c>
-      <c r="V16">
+      <c r="W16">
         <v>144</v>
       </c>
-      <c r="W16">
+      <c r="X16">
         <v>151</v>
       </c>
-      <c r="X16">
+      <c r="Y16">
         <v>896683</v>
       </c>
-      <c r="Y16">
-        <v>0</v>
-      </c>
-      <c r="Z16" s="7">
+      <c r="Z16">
+        <v>0</v>
+      </c>
+      <c r="AA16" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA16" s="1" t="s">
+      <c r="AB16" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>1</v>
       </c>
@@ -2599,42 +2693,45 @@
       <c r="O17" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="P17">
+      <c r="P17" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q17">
         <v>996.61</v>
       </c>
-      <c r="Q17">
+      <c r="R17">
         <v>41.68</v>
       </c>
-      <c r="R17" s="3">
+      <c r="S17" s="3">
         <v>348</v>
       </c>
-      <c r="S17" s="3">
+      <c r="T17" s="3">
         <v>23</v>
       </c>
-      <c r="U17">
+      <c r="V17">
         <v>270</v>
       </c>
-      <c r="V17">
+      <c r="W17">
         <v>304</v>
       </c>
-      <c r="W17">
+      <c r="X17">
         <v>312</v>
       </c>
-      <c r="X17">
+      <c r="Y17">
         <v>897508</v>
       </c>
-      <c r="Y17">
-        <v>0</v>
-      </c>
-      <c r="Z17" s="7">
+      <c r="Z17">
+        <v>0</v>
+      </c>
+      <c r="AA17" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA17" s="1" t="s">
+      <c r="AB17" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>1</v>
       </c>
@@ -2680,42 +2777,45 @@
       <c r="O18" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="P18">
+      <c r="P18" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q18">
         <v>996.53</v>
       </c>
-      <c r="Q18">
+      <c r="R18">
         <v>91.06</v>
       </c>
-      <c r="R18">
+      <c r="S18">
         <v>1070</v>
       </c>
-      <c r="S18">
+      <c r="T18">
         <v>27</v>
       </c>
-      <c r="U18">
+      <c r="V18">
         <v>417</v>
       </c>
-      <c r="V18">
+      <c r="W18">
         <v>442</v>
       </c>
-      <c r="W18">
+      <c r="X18">
         <v>446</v>
       </c>
-      <c r="X18">
+      <c r="Y18">
         <v>898225</v>
       </c>
-      <c r="Y18">
-        <v>0</v>
-      </c>
-      <c r="Z18" s="7">
+      <c r="Z18">
+        <v>0</v>
+      </c>
+      <c r="AA18" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA18" s="1" t="s">
+      <c r="AB18" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>1</v>
       </c>
@@ -2761,42 +2861,45 @@
       <c r="O19" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="P19">
+      <c r="P19" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q19">
         <v>997.26</v>
       </c>
-      <c r="Q19">
+      <c r="R19">
         <v>212.8</v>
       </c>
-      <c r="R19">
+      <c r="S19">
         <v>3066</v>
       </c>
-      <c r="S19">
+      <c r="T19">
         <v>287</v>
       </c>
-      <c r="U19">
+      <c r="V19">
         <v>860</v>
       </c>
-      <c r="V19">
+      <c r="W19">
         <v>888</v>
       </c>
-      <c r="W19">
+      <c r="X19">
         <v>898</v>
       </c>
-      <c r="X19">
+      <c r="Y19">
         <v>901434</v>
       </c>
-      <c r="Y19">
-        <v>0</v>
-      </c>
-      <c r="Z19" s="7">
+      <c r="Z19">
+        <v>0</v>
+      </c>
+      <c r="AA19" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA19" s="1" t="s">
+      <c r="AB19" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2842,42 +2945,45 @@
       <c r="O20" t="s">
         <v>278</v>
       </c>
-      <c r="P20">
+      <c r="P20" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q20">
         <v>999.91</v>
       </c>
-      <c r="Q20">
+      <c r="R20">
         <v>356.87</v>
       </c>
-      <c r="R20">
+      <c r="S20">
         <v>3087</v>
       </c>
-      <c r="S20">
+      <c r="T20">
         <v>119</v>
       </c>
-      <c r="U20">
+      <c r="V20">
         <v>1646</v>
       </c>
-      <c r="V20">
+      <c r="W20">
         <v>1684</v>
       </c>
-      <c r="W20">
+      <c r="X20">
         <v>1694</v>
       </c>
-      <c r="X20">
+      <c r="Y20">
         <v>904721</v>
       </c>
-      <c r="Y20">
-        <v>0</v>
-      </c>
-      <c r="Z20" s="7">
+      <c r="Z20">
+        <v>0</v>
+      </c>
+      <c r="AA20" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA20" s="1" t="s">
+      <c r="AB20" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -2923,42 +3029,45 @@
       <c r="O21" t="s">
         <v>278</v>
       </c>
-      <c r="P21">
+      <c r="P21" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q21">
         <v>993.99</v>
       </c>
-      <c r="Q21">
+      <c r="R21">
         <v>587.75</v>
       </c>
-      <c r="R21">
+      <c r="S21">
         <v>4946</v>
       </c>
-      <c r="S21">
+      <c r="T21">
         <v>25</v>
       </c>
-      <c r="U21">
+      <c r="V21">
         <v>2142</v>
       </c>
-      <c r="V21">
+      <c r="W21">
         <v>2201</v>
       </c>
-      <c r="W21">
+      <c r="X21">
         <v>4159</v>
       </c>
-      <c r="X21">
+      <c r="Y21">
         <v>902995</v>
       </c>
-      <c r="Y21">
-        <v>0</v>
-      </c>
-      <c r="Z21" s="7">
+      <c r="Z21">
+        <v>0</v>
+      </c>
+      <c r="AA21" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA21" s="1" t="s">
+      <c r="AB21" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -3004,167 +3113,954 @@
       <c r="O22" t="s">
         <v>278</v>
       </c>
-      <c r="P22">
+      <c r="P22" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q22">
         <v>981.93</v>
       </c>
-      <c r="Q22">
+      <c r="R22">
         <v>1209.79</v>
       </c>
-      <c r="R22">
+      <c r="S22">
         <v>9932</v>
       </c>
-      <c r="S22">
-        <v>35</v>
-      </c>
-      <c r="U22">
+      <c r="T22">
+        <v>35</v>
+      </c>
+      <c r="V22">
         <v>5715</v>
       </c>
-      <c r="V22">
+      <c r="W22">
         <v>5785</v>
       </c>
-      <c r="W22">
+      <c r="X22">
         <v>5791</v>
       </c>
-      <c r="X22">
+      <c r="Y22">
         <v>906691</v>
       </c>
-      <c r="Y22">
-        <v>0</v>
-      </c>
-      <c r="Z22" s="7">
+      <c r="Z22">
+        <v>0</v>
+      </c>
+      <c r="AA22" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AA22" s="1" t="s">
+      <c r="AB22" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA23" s="1"/>
-    </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA24" s="1"/>
-    </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA25" s="1"/>
-    </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA26" s="1"/>
-    </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="AA27" s="1"/>
-    </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="Z28" s="5"/>
-      <c r="AA28" s="1"/>
-    </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="Z29" s="5"/>
-      <c r="AA29" s="1"/>
-    </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="Z30" s="5"/>
-      <c r="AA30" s="1"/>
-    </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="Z31" s="5"/>
-      <c r="AA31" s="1"/>
-    </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="Z32" s="5"/>
-      <c r="AA32" s="1"/>
-    </row>
-    <row r="33" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z33" s="5"/>
-      <c r="AA33" s="1"/>
-    </row>
-    <row r="34" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z34" s="5"/>
-      <c r="AA34" s="1"/>
-    </row>
-    <row r="35" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z35" s="5"/>
-      <c r="AA35" s="1"/>
-    </row>
-    <row r="36" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z36" s="5"/>
-      <c r="AA36" s="1"/>
-    </row>
-    <row r="37" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z37" s="5"/>
-      <c r="AA37" s="1"/>
-    </row>
-    <row r="38" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z38" s="5"/>
-      <c r="AA38" s="1"/>
-    </row>
-    <row r="39" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z39" s="5"/>
-      <c r="AA39" s="1"/>
-    </row>
-    <row r="40" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z40" s="5"/>
-      <c r="AA40" s="1"/>
-    </row>
-    <row r="41" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z41" s="5"/>
-      <c r="AA41" s="1"/>
-    </row>
-    <row r="42" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z42" s="5"/>
-      <c r="AA42" s="1"/>
-    </row>
-    <row r="43" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z43" s="5"/>
-      <c r="AA43" s="1"/>
-    </row>
-    <row r="44" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z44" s="5"/>
-      <c r="AA44" s="1"/>
-      <c r="AB44" s="6"/>
-    </row>
-    <row r="45" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z45" s="5"/>
-      <c r="AA45" s="1"/>
-    </row>
-    <row r="46" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z46" s="5"/>
-      <c r="AA46" s="1"/>
-    </row>
-    <row r="47" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z47" s="5"/>
-      <c r="AA47" s="1"/>
-    </row>
-    <row r="48" spans="26:28" x14ac:dyDescent="0.2">
-      <c r="Z48" s="5"/>
-      <c r="AA48" s="1"/>
-    </row>
-    <row r="49" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="A49" s="3"/>
-      <c r="B49" s="3"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="3"/>
-      <c r="E49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-      <c r="H49" s="3"/>
-      <c r="I49" s="3"/>
-      <c r="J49" s="3"/>
-      <c r="K49" s="3"/>
-      <c r="L49" s="3"/>
-      <c r="M49" s="3"/>
-      <c r="N49" s="3"/>
-      <c r="O49" s="3"/>
-      <c r="R49" s="3"/>
-      <c r="S49" s="3"/>
-      <c r="T49" s="3"/>
-      <c r="U49" s="3"/>
-      <c r="V49" s="3"/>
-      <c r="W49" s="3"/>
-      <c r="Z49" s="5"/>
-      <c r="AA49" s="1"/>
-    </row>
-    <row r="50" spans="1:27" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A23">
+        <v>1</v>
+      </c>
+      <c r="B23">
+        <v>3</v>
+      </c>
+      <c r="C23" t="s">
+        <v>173</v>
+      </c>
+      <c r="D23">
+        <v>19200</v>
+      </c>
+      <c r="E23">
+        <v>600</v>
+      </c>
+      <c r="F23" t="s">
+        <v>211</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+      <c r="H23">
+        <v>4</v>
+      </c>
+      <c r="I23">
+        <v>6</v>
+      </c>
+      <c r="J23">
+        <v>4</v>
+      </c>
+      <c r="K23" t="s">
+        <v>268</v>
+      </c>
+      <c r="L23" t="s">
+        <v>186</v>
+      </c>
+      <c r="M23">
+        <v>16</v>
+      </c>
+      <c r="N23">
+        <v>320</v>
+      </c>
+      <c r="O23" t="s">
+        <v>278</v>
+      </c>
+      <c r="P23" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q23">
+        <v>978.51</v>
+      </c>
+      <c r="R23">
+        <v>269</v>
+      </c>
+      <c r="S23">
+        <v>11717</v>
+      </c>
+      <c r="T23">
+        <v>36</v>
+      </c>
+      <c r="V23">
+        <v>466</v>
+      </c>
+      <c r="W23">
+        <v>3382</v>
+      </c>
+      <c r="X23">
+        <v>5100</v>
+      </c>
+      <c r="Y23">
+        <v>925197</v>
+      </c>
+      <c r="Z23">
+        <v>0</v>
+      </c>
+      <c r="AA23" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB23" s="1" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A24">
+        <v>1</v>
+      </c>
+      <c r="B24">
+        <v>3</v>
+      </c>
+      <c r="C24" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24">
+        <v>9600</v>
+      </c>
+      <c r="E24">
+        <v>600</v>
+      </c>
+      <c r="F24" t="s">
+        <v>211</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>4</v>
+      </c>
+      <c r="I24">
+        <v>6</v>
+      </c>
+      <c r="J24">
+        <v>4</v>
+      </c>
+      <c r="K24" t="s">
+        <v>268</v>
+      </c>
+      <c r="L24" t="s">
+        <v>186</v>
+      </c>
+      <c r="M24">
+        <v>16</v>
+      </c>
+      <c r="N24">
+        <v>320</v>
+      </c>
+      <c r="O24" t="s">
+        <v>278</v>
+      </c>
+      <c r="P24" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q24">
+        <v>983.68</v>
+      </c>
+      <c r="R24">
+        <v>394.29</v>
+      </c>
+      <c r="S24">
+        <v>12917</v>
+      </c>
+      <c r="T24">
+        <v>626</v>
+      </c>
+      <c r="V24">
+        <v>1441.99</v>
+      </c>
+      <c r="W24">
+        <v>1841</v>
+      </c>
+      <c r="X24">
+        <v>2288</v>
+      </c>
+      <c r="Y24">
+        <v>913854</v>
+      </c>
+      <c r="Z24">
+        <v>0</v>
+      </c>
+      <c r="AA24" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB24" s="1" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A25">
+        <v>1</v>
+      </c>
+      <c r="B25">
+        <v>3</v>
+      </c>
+      <c r="C25" t="s">
+        <v>173</v>
+      </c>
+      <c r="D25">
+        <v>4800</v>
+      </c>
+      <c r="E25">
+        <v>600</v>
+      </c>
+      <c r="F25" t="s">
+        <v>211</v>
+      </c>
+      <c r="G25">
+        <v>1</v>
+      </c>
+      <c r="H25">
+        <v>4</v>
+      </c>
+      <c r="I25">
+        <v>6</v>
+      </c>
+      <c r="J25">
+        <v>4</v>
+      </c>
+      <c r="K25" t="s">
+        <v>268</v>
+      </c>
+      <c r="L25" t="s">
+        <v>186</v>
+      </c>
+      <c r="M25">
+        <v>16</v>
+      </c>
+      <c r="N25">
+        <v>320</v>
+      </c>
+      <c r="O25" t="s">
+        <v>278</v>
+      </c>
+      <c r="P25" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q25">
+        <v>991.55</v>
+      </c>
+      <c r="R25">
+        <v>233.41</v>
+      </c>
+      <c r="S25">
+        <v>6544</v>
+      </c>
+      <c r="T25">
+        <v>20</v>
+      </c>
+      <c r="V25">
+        <v>165.99</v>
+      </c>
+      <c r="W25">
+        <v>859</v>
+      </c>
+      <c r="X25">
+        <v>861</v>
+      </c>
+      <c r="Y25">
+        <v>907183</v>
+      </c>
+      <c r="Z25">
+        <v>0</v>
+      </c>
+      <c r="AA25" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB25" s="1" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A26">
+        <v>1</v>
+      </c>
+      <c r="B26">
+        <v>3</v>
+      </c>
+      <c r="C26" t="s">
+        <v>173</v>
+      </c>
+      <c r="D26">
+        <v>2400</v>
+      </c>
+      <c r="E26">
+        <v>600</v>
+      </c>
+      <c r="F26" t="s">
+        <v>211</v>
+      </c>
+      <c r="G26">
+        <v>1</v>
+      </c>
+      <c r="H26">
+        <v>4</v>
+      </c>
+      <c r="I26">
+        <v>6</v>
+      </c>
+      <c r="J26">
+        <v>4</v>
+      </c>
+      <c r="K26" t="s">
+        <v>268</v>
+      </c>
+      <c r="L26" t="s">
+        <v>186</v>
+      </c>
+      <c r="M26">
+        <v>16</v>
+      </c>
+      <c r="N26">
+        <v>320</v>
+      </c>
+      <c r="O26" t="s">
+        <v>278</v>
+      </c>
+      <c r="P26" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q26">
+        <v>989.15</v>
+      </c>
+      <c r="R26">
+        <v>208.7</v>
+      </c>
+      <c r="S26">
+        <v>9825</v>
+      </c>
+      <c r="T26">
+        <v>287</v>
+      </c>
+      <c r="V26">
+        <v>803</v>
+      </c>
+      <c r="W26">
+        <v>823</v>
+      </c>
+      <c r="X26">
+        <v>827</v>
+      </c>
+      <c r="Y26">
+        <v>899870</v>
+      </c>
+      <c r="Z26">
+        <v>0</v>
+      </c>
+      <c r="AA26" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB26" s="1" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A27">
+        <v>1</v>
+      </c>
+      <c r="B27">
+        <v>3</v>
+      </c>
+      <c r="C27" t="s">
+        <v>173</v>
+      </c>
+      <c r="D27">
+        <v>1200</v>
+      </c>
+      <c r="E27">
+        <v>600</v>
+      </c>
+      <c r="F27" t="s">
+        <v>211</v>
+      </c>
+      <c r="G27">
+        <v>1</v>
+      </c>
+      <c r="H27">
+        <v>4</v>
+      </c>
+      <c r="I27">
+        <v>6</v>
+      </c>
+      <c r="J27">
+        <v>4</v>
+      </c>
+      <c r="K27" t="s">
+        <v>268</v>
+      </c>
+      <c r="L27" t="s">
+        <v>186</v>
+      </c>
+      <c r="M27">
+        <v>16</v>
+      </c>
+      <c r="N27">
+        <v>320</v>
+      </c>
+      <c r="O27" t="s">
+        <v>278</v>
+      </c>
+      <c r="P27" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q27">
+        <v>988.79</v>
+      </c>
+      <c r="R27">
+        <v>87.64</v>
+      </c>
+      <c r="S27">
+        <v>8668</v>
+      </c>
+      <c r="T27">
+        <v>24</v>
+      </c>
+      <c r="V27">
+        <v>424</v>
+      </c>
+      <c r="W27">
+        <v>467</v>
+      </c>
+      <c r="X27">
+        <v>479</v>
+      </c>
+      <c r="Y27">
+        <v>901191</v>
+      </c>
+      <c r="Z27">
+        <v>0</v>
+      </c>
+      <c r="AA27" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB27" s="1" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A28">
+        <v>1</v>
+      </c>
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28" t="s">
+        <v>173</v>
+      </c>
+      <c r="D28">
+        <v>600</v>
+      </c>
+      <c r="E28">
+        <v>600</v>
+      </c>
+      <c r="F28" t="s">
+        <v>211</v>
+      </c>
+      <c r="G28">
+        <v>1</v>
+      </c>
+      <c r="H28">
+        <v>4</v>
+      </c>
+      <c r="I28">
+        <v>6</v>
+      </c>
+      <c r="J28">
+        <v>4</v>
+      </c>
+      <c r="K28" t="s">
+        <v>268</v>
+      </c>
+      <c r="L28" t="s">
+        <v>186</v>
+      </c>
+      <c r="M28">
+        <v>16</v>
+      </c>
+      <c r="N28">
+        <v>320</v>
+      </c>
+      <c r="O28" t="s">
+        <v>278</v>
+      </c>
+      <c r="P28" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q28">
+        <v>986.07</v>
+      </c>
+      <c r="R28">
+        <v>43.57</v>
+      </c>
+      <c r="S28">
+        <v>10390</v>
+      </c>
+      <c r="T28">
+        <v>20</v>
+      </c>
+      <c r="V28">
+        <v>199.99</v>
+      </c>
+      <c r="W28">
+        <v>218</v>
+      </c>
+      <c r="X28">
+        <v>226</v>
+      </c>
+      <c r="Y28">
+        <v>895335</v>
+      </c>
+      <c r="Z28">
+        <v>0</v>
+      </c>
+      <c r="AA28" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB28" s="1" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A29">
+        <v>1</v>
+      </c>
+      <c r="B29">
+        <v>3</v>
+      </c>
+      <c r="C29" t="s">
+        <v>173</v>
+      </c>
+      <c r="D29">
+        <v>300</v>
+      </c>
+      <c r="E29">
+        <v>600</v>
+      </c>
+      <c r="F29" t="s">
+        <v>211</v>
+      </c>
+      <c r="G29">
+        <v>1</v>
+      </c>
+      <c r="H29">
+        <v>4</v>
+      </c>
+      <c r="I29">
+        <v>6</v>
+      </c>
+      <c r="J29">
+        <v>4</v>
+      </c>
+      <c r="K29" t="s">
+        <v>268</v>
+      </c>
+      <c r="L29" t="s">
+        <v>186</v>
+      </c>
+      <c r="M29">
+        <v>16</v>
+      </c>
+      <c r="N29">
+        <v>320</v>
+      </c>
+      <c r="O29" t="s">
+        <v>278</v>
+      </c>
+      <c r="P29" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q29">
+        <v>988.94</v>
+      </c>
+      <c r="R29">
+        <v>26.12</v>
+      </c>
+      <c r="S29">
+        <v>7961</v>
+      </c>
+      <c r="T29">
+        <v>20</v>
+      </c>
+      <c r="V29">
+        <v>122</v>
+      </c>
+      <c r="W29">
+        <v>151</v>
+      </c>
+      <c r="X29">
+        <v>156</v>
+      </c>
+      <c r="Y29">
+        <v>890172</v>
+      </c>
+      <c r="Z29">
+        <v>0</v>
+      </c>
+      <c r="AA29" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB29" s="1" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A30">
+        <v>1</v>
+      </c>
+      <c r="B30">
+        <v>3</v>
+      </c>
+      <c r="C30" t="s">
+        <v>173</v>
+      </c>
+      <c r="D30">
+        <v>300</v>
+      </c>
+      <c r="E30">
+        <v>600</v>
+      </c>
+      <c r="F30" t="s">
+        <v>211</v>
+      </c>
+      <c r="G30">
+        <v>1</v>
+      </c>
+      <c r="H30">
+        <v>4</v>
+      </c>
+      <c r="I30">
+        <v>6</v>
+      </c>
+      <c r="J30">
+        <v>4</v>
+      </c>
+      <c r="K30" t="s">
+        <v>268</v>
+      </c>
+      <c r="L30" t="s">
+        <v>186</v>
+      </c>
+      <c r="M30">
+        <v>16</v>
+      </c>
+      <c r="N30">
+        <v>320</v>
+      </c>
+      <c r="O30" t="s">
+        <v>278</v>
+      </c>
+      <c r="P30" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q30">
+        <v>2766.4</v>
+      </c>
+      <c r="R30">
+        <v>107.69</v>
+      </c>
+      <c r="S30">
+        <v>1707</v>
+      </c>
+      <c r="T30">
+        <v>47</v>
+      </c>
+      <c r="V30">
+        <v>162</v>
+      </c>
+      <c r="W30">
+        <v>174</v>
+      </c>
+      <c r="X30">
+        <v>287</v>
+      </c>
+      <c r="Y30">
+        <v>2499413</v>
+      </c>
+      <c r="Z30">
+        <v>0</v>
+      </c>
+      <c r="AA30" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB30" s="1" t="s">
+        <v>299</v>
+      </c>
+    </row>
+    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A31">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>3</v>
+      </c>
+      <c r="C31" t="s">
+        <v>173</v>
+      </c>
+      <c r="D31">
+        <v>600</v>
+      </c>
+      <c r="E31">
+        <v>600</v>
+      </c>
+      <c r="F31" t="s">
+        <v>211</v>
+      </c>
+      <c r="G31">
+        <v>1</v>
+      </c>
+      <c r="H31">
+        <v>4</v>
+      </c>
+      <c r="I31">
+        <v>6</v>
+      </c>
+      <c r="J31">
+        <v>4</v>
+      </c>
+      <c r="K31" t="s">
+        <v>268</v>
+      </c>
+      <c r="L31" t="s">
+        <v>186</v>
+      </c>
+      <c r="M31">
+        <v>16</v>
+      </c>
+      <c r="N31">
+        <v>320</v>
+      </c>
+      <c r="O31" t="s">
+        <v>278</v>
+      </c>
+      <c r="P31" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q31">
+        <v>2762.97</v>
+      </c>
+      <c r="R31">
+        <v>214.31</v>
+      </c>
+      <c r="S31">
+        <v>1301</v>
+      </c>
+      <c r="T31">
+        <v>92</v>
+      </c>
+      <c r="V31">
+        <v>177.99</v>
+      </c>
+      <c r="W31">
+        <v>194</v>
+      </c>
+      <c r="X31">
+        <v>199</v>
+      </c>
+      <c r="Y31">
+        <v>2514537</v>
+      </c>
+      <c r="Z31">
+        <v>0</v>
+      </c>
+      <c r="AA31" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB31" s="1" t="s">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32">
+        <v>3</v>
+      </c>
+      <c r="C32" t="s">
+        <v>173</v>
+      </c>
+      <c r="D32">
+        <v>1000</v>
+      </c>
+      <c r="E32">
+        <v>600</v>
+      </c>
+      <c r="F32" t="s">
+        <v>211</v>
+      </c>
+      <c r="G32">
+        <v>1</v>
+      </c>
+      <c r="H32">
+        <v>4</v>
+      </c>
+      <c r="I32">
+        <v>6</v>
+      </c>
+      <c r="J32">
+        <v>4</v>
+      </c>
+      <c r="K32" t="s">
+        <v>268</v>
+      </c>
+      <c r="L32" t="s">
+        <v>186</v>
+      </c>
+      <c r="M32">
+        <v>16</v>
+      </c>
+      <c r="N32">
+        <v>320</v>
+      </c>
+      <c r="O32" t="s">
+        <v>278</v>
+      </c>
+      <c r="P32" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q32">
+        <v>2481.89</v>
+      </c>
+      <c r="R32">
+        <v>396.67</v>
+      </c>
+      <c r="S32">
+        <v>18637</v>
+      </c>
+      <c r="T32">
+        <v>172</v>
+      </c>
+      <c r="V32">
+        <v>530</v>
+      </c>
+      <c r="W32">
+        <v>549</v>
+      </c>
+      <c r="X32">
+        <v>560</v>
+      </c>
+      <c r="Y32">
+        <v>2266488</v>
+      </c>
+      <c r="Z32">
+        <v>0</v>
+      </c>
+      <c r="AA32" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB32" s="1" t="s">
+        <v>301</v>
+      </c>
+    </row>
+    <row r="33" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA33" s="5"/>
+      <c r="AB33" s="1"/>
+    </row>
+    <row r="34" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA34" s="5"/>
+      <c r="AB34" s="1"/>
+    </row>
+    <row r="35" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA35" s="5"/>
+      <c r="AB35" s="1"/>
+    </row>
+    <row r="36" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA36" s="5"/>
+      <c r="AB36" s="1"/>
+    </row>
+    <row r="37" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA37" s="5"/>
+      <c r="AB37" s="1"/>
+    </row>
+    <row r="38" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA38" s="5"/>
+      <c r="AB38" s="1"/>
+    </row>
+    <row r="39" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA39" s="5"/>
+      <c r="AB39" s="1"/>
+    </row>
+    <row r="40" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA40" s="5"/>
+      <c r="AB40" s="1"/>
+    </row>
+    <row r="41" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA41" s="5"/>
+      <c r="AB41" s="1"/>
+    </row>
+    <row r="42" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA42" s="5"/>
+      <c r="AB42" s="1"/>
+    </row>
+    <row r="43" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA43" s="5"/>
+      <c r="AB43" s="1"/>
+    </row>
+    <row r="44" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA44" s="5"/>
+      <c r="AB44" s="1"/>
+    </row>
+    <row r="45" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA45" s="5"/>
+      <c r="AB45" s="1"/>
+      <c r="AC45" s="6"/>
+    </row>
+    <row r="46" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA46" s="5"/>
+      <c r="AB46" s="1"/>
+    </row>
+    <row r="47" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA47" s="5"/>
+      <c r="AB47" s="1"/>
+    </row>
+    <row r="48" spans="27:29" x14ac:dyDescent="0.2">
+      <c r="AA48" s="5"/>
+      <c r="AB48" s="1"/>
+    </row>
+    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA49" s="5"/>
+      <c r="AB49" s="1"/>
+    </row>
+    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -3180,58 +4076,86 @@
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
-      <c r="R50" s="3"/>
+      <c r="P50" s="3"/>
       <c r="S50" s="3"/>
       <c r="T50" s="3"/>
-      <c r="Z50" s="5"/>
-      <c r="AA50" s="1"/>
-    </row>
-    <row r="51" spans="1:27" x14ac:dyDescent="0.2">
+      <c r="U50" s="3"/>
+      <c r="V50" s="3"/>
+      <c r="W50" s="3"/>
+      <c r="X50" s="3"/>
+      <c r="AA50" s="5"/>
+      <c r="AB50" s="1"/>
+    </row>
+    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="A51" s="3"/>
+      <c r="B51" s="3"/>
+      <c r="C51" s="3"/>
+      <c r="D51" s="3"/>
+      <c r="E51" s="3"/>
+      <c r="F51" s="3"/>
+      <c r="G51" s="3"/>
+      <c r="H51" s="3"/>
+      <c r="I51" s="3"/>
+      <c r="J51" s="3"/>
+      <c r="K51" s="3"/>
+      <c r="L51" s="3"/>
+      <c r="M51" s="3"/>
+      <c r="N51" s="3"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
       <c r="S51" s="3"/>
-      <c r="Z51" s="5"/>
-      <c r="AA51" s="1"/>
-    </row>
-    <row r="52" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="Z52" s="5"/>
-      <c r="AA52" s="1"/>
-    </row>
-    <row r="53" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="S53" s="3"/>
-      <c r="Z53" s="5"/>
-      <c r="AA53" s="1"/>
-    </row>
-    <row r="54" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="S54" s="3"/>
-      <c r="Z54" s="5"/>
-      <c r="AA54" s="1"/>
-    </row>
-    <row r="55" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="S55" s="3"/>
-      <c r="Z55" s="5"/>
-      <c r="AA55" s="1"/>
-    </row>
-    <row r="56" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="S56" s="3"/>
-      <c r="Z56" s="5"/>
-      <c r="AA56" s="1"/>
-    </row>
-    <row r="57" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="S57" s="3"/>
-      <c r="Z57" s="5"/>
-      <c r="AA57" s="1"/>
-    </row>
-    <row r="58" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="S58" s="3"/>
-      <c r="Z58" s="5"/>
-      <c r="AA58" s="1"/>
-    </row>
-    <row r="59" spans="1:27" x14ac:dyDescent="0.2">
-      <c r="S59" s="3"/>
-      <c r="Z59" s="5"/>
-      <c r="AA59" s="1"/>
+      <c r="T51" s="3"/>
+      <c r="U51" s="3"/>
+      <c r="AA51" s="5"/>
+      <c r="AB51" s="1"/>
+    </row>
+    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="T52" s="3"/>
+      <c r="AA52" s="5"/>
+      <c r="AB52" s="1"/>
+    </row>
+    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="AA53" s="5"/>
+      <c r="AB53" s="1"/>
+    </row>
+    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="T54" s="3"/>
+      <c r="AA54" s="5"/>
+      <c r="AB54" s="1"/>
+    </row>
+    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="T55" s="3"/>
+      <c r="AA55" s="5"/>
+      <c r="AB55" s="1"/>
+    </row>
+    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="T56" s="3"/>
+      <c r="AA56" s="5"/>
+      <c r="AB56" s="1"/>
+    </row>
+    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="T57" s="3"/>
+      <c r="AA57" s="5"/>
+      <c r="AB57" s="1"/>
+    </row>
+    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="T58" s="3"/>
+      <c r="AA58" s="5"/>
+      <c r="AB58" s="1"/>
+    </row>
+    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="T59" s="3"/>
+      <c r="AA59" s="5"/>
+      <c r="AB59" s="1"/>
+    </row>
+    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="T60" s="3"/>
+      <c r="AA60" s="5"/>
+      <c r="AB60" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AB41" xr:uid="{0BCD43CD-D15C-C44C-860E-27B2AEF78201}"/>
+  <autoFilter ref="A2:AC42" xr:uid="{0BCD43CD-D15C-C44C-860E-27B2AEF78201}"/>
+  <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add http2 load test
</commit_message>
<xml_diff>
--- a/kafka_benchmark/benchmark_stats.xlsx
+++ b/kafka_benchmark/benchmark_stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10912"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lijjin/Documents/work/git_ws/redistest/kafka_benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E1E5BC3E-43BD-004E-925B-75D70F27CCE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E6EE8E-4AEB-E04F-96FC-E4218ABEE1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{35590E01-C7C5-464A-8FB5-DBB7ECFA3BB7}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2847" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2887" uniqueCount="309">
   <si>
     <t>Partition</t>
   </si>
@@ -954,6 +954,24 @@
   </si>
   <si>
     <t>client -(http2 or http1.1/https)-&gt;Nginx-(http1.1/http)-&gt;service</t>
+  </si>
+  <si>
+    <t>h2load</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_1000t_1200e_4cpu_async2_https_http2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_1000t_2400e_4cpu_async2_https_http2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_1000t_4800e_4cpu_async2_https_http2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_1000t_9600e_4cpu_async2_https_http2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_1000t_19200e_4cpu_async2_https_http2</t>
   </si>
 </sst>
 </file>
@@ -962,7 +980,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000000%"/>
-    <numFmt numFmtId="171" formatCode="0.0000%"/>
+    <numFmt numFmtId="165" formatCode="0.0000%"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1038,7 +1056,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1356,8 +1374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1D1567-5C01-D845-B094-708B919E4B92}">
   <dimension ref="A1:AC60"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1"/>
+    <sheetView tabSelected="1" topLeftCell="T12" workbookViewId="0">
+      <selection activeCell="AC38" sqref="AC38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1378,7 +1396,7 @@
     <col min="21" max="24" width="21.1640625" customWidth="1"/>
     <col min="25" max="25" width="14.6640625" customWidth="1"/>
     <col min="26" max="27" width="11.33203125" customWidth="1"/>
-    <col min="28" max="28" width="37.6640625" customWidth="1"/>
+    <col min="28" max="28" width="57.1640625" customWidth="1"/>
     <col min="29" max="29" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1566,7 +1584,7 @@
         <v>0</v>
       </c>
       <c r="AA3" s="8">
-        <f t="shared" ref="AA3:AA32" si="0">Z3/Y3</f>
+        <f t="shared" ref="AA3:AA37" si="0">Z3/Y3</f>
         <v>0</v>
       </c>
       <c r="AB3" s="1" t="s">
@@ -3991,68 +4009,483 @@
         <v>301</v>
       </c>
     </row>
-    <row r="33" spans="27:29" x14ac:dyDescent="0.2">
-      <c r="AA33" s="5"/>
-      <c r="AB33" s="1"/>
-    </row>
-    <row r="34" spans="27:29" x14ac:dyDescent="0.2">
-      <c r="AA34" s="5"/>
-      <c r="AB34" s="1"/>
-    </row>
-    <row r="35" spans="27:29" x14ac:dyDescent="0.2">
-      <c r="AA35" s="5"/>
-      <c r="AB35" s="1"/>
-    </row>
-    <row r="36" spans="27:29" x14ac:dyDescent="0.2">
-      <c r="AA36" s="5"/>
-      <c r="AB36" s="1"/>
-    </row>
-    <row r="37" spans="27:29" x14ac:dyDescent="0.2">
-      <c r="AA37" s="5"/>
-      <c r="AB37" s="1"/>
-    </row>
-    <row r="38" spans="27:29" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A33">
+        <v>1</v>
+      </c>
+      <c r="B33">
+        <v>3</v>
+      </c>
+      <c r="C33" t="s">
+        <v>173</v>
+      </c>
+      <c r="D33">
+        <v>1200</v>
+      </c>
+      <c r="E33">
+        <v>600</v>
+      </c>
+      <c r="F33" t="s">
+        <v>211</v>
+      </c>
+      <c r="G33">
+        <v>1</v>
+      </c>
+      <c r="H33">
+        <v>4</v>
+      </c>
+      <c r="I33">
+        <v>6</v>
+      </c>
+      <c r="J33">
+        <v>4</v>
+      </c>
+      <c r="K33" t="s">
+        <v>268</v>
+      </c>
+      <c r="L33" t="s">
+        <v>186</v>
+      </c>
+      <c r="M33">
+        <v>16</v>
+      </c>
+      <c r="N33">
+        <v>320</v>
+      </c>
+      <c r="O33" t="s">
+        <v>278</v>
+      </c>
+      <c r="P33" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q33">
+        <v>2833.3</v>
+      </c>
+      <c r="R33">
+        <v>423.14</v>
+      </c>
+      <c r="S33">
+        <v>1495.75</v>
+      </c>
+      <c r="T33">
+        <v>416.71</v>
+      </c>
+      <c r="V33">
+        <v>535.92999999999995</v>
+      </c>
+      <c r="W33">
+        <v>773.38</v>
+      </c>
+      <c r="X33">
+        <v>850.45</v>
+      </c>
+      <c r="Y33">
+        <v>2549970</v>
+      </c>
+      <c r="Z33">
+        <v>0</v>
+      </c>
+      <c r="AA33" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB33" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="AC33" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A34">
+        <v>1</v>
+      </c>
+      <c r="B34">
+        <v>3</v>
+      </c>
+      <c r="C34" t="s">
+        <v>173</v>
+      </c>
+      <c r="D34">
+        <v>2400</v>
+      </c>
+      <c r="E34">
+        <v>600</v>
+      </c>
+      <c r="F34" t="s">
+        <v>211</v>
+      </c>
+      <c r="G34">
+        <v>1</v>
+      </c>
+      <c r="H34">
+        <v>4</v>
+      </c>
+      <c r="I34">
+        <v>6</v>
+      </c>
+      <c r="J34">
+        <v>4</v>
+      </c>
+      <c r="K34" t="s">
+        <v>268</v>
+      </c>
+      <c r="L34" t="s">
+        <v>186</v>
+      </c>
+      <c r="M34">
+        <v>16</v>
+      </c>
+      <c r="N34">
+        <v>320</v>
+      </c>
+      <c r="O34" t="s">
+        <v>278</v>
+      </c>
+      <c r="P34" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q34">
+        <v>2758.85</v>
+      </c>
+      <c r="R34">
+        <v>868.39</v>
+      </c>
+      <c r="S34">
+        <v>10996.44</v>
+      </c>
+      <c r="T34">
+        <v>846.49</v>
+      </c>
+      <c r="V34">
+        <v>1054.3800000000001</v>
+      </c>
+      <c r="W34">
+        <v>2585.58</v>
+      </c>
+      <c r="X34">
+        <v>10977.49</v>
+      </c>
+      <c r="Y34">
+        <v>2482966</v>
+      </c>
+      <c r="Z34">
+        <v>0</v>
+      </c>
+      <c r="AA34" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB34" s="1" t="s">
+        <v>305</v>
+      </c>
+      <c r="AC34" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A35">
+        <v>1</v>
+      </c>
+      <c r="B35">
+        <v>3</v>
+      </c>
+      <c r="C35" t="s">
+        <v>173</v>
+      </c>
+      <c r="D35">
+        <v>4800</v>
+      </c>
+      <c r="E35">
+        <v>600</v>
+      </c>
+      <c r="F35" t="s">
+        <v>211</v>
+      </c>
+      <c r="G35">
+        <v>1</v>
+      </c>
+      <c r="H35">
+        <v>4</v>
+      </c>
+      <c r="I35">
+        <v>6</v>
+      </c>
+      <c r="J35">
+        <v>4</v>
+      </c>
+      <c r="K35" t="s">
+        <v>268</v>
+      </c>
+      <c r="L35" t="s">
+        <v>186</v>
+      </c>
+      <c r="M35">
+        <v>16</v>
+      </c>
+      <c r="N35">
+        <v>320</v>
+      </c>
+      <c r="O35" t="s">
+        <v>278</v>
+      </c>
+      <c r="P35" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q35">
+        <v>2785.19</v>
+      </c>
+      <c r="R35">
+        <v>1717.29</v>
+      </c>
+      <c r="S35">
+        <v>5277.52</v>
+      </c>
+      <c r="T35">
+        <v>1700.94</v>
+      </c>
+      <c r="V35">
+        <v>2042.76</v>
+      </c>
+      <c r="W35">
+        <v>2380.39</v>
+      </c>
+      <c r="X35">
+        <v>3535.87</v>
+      </c>
+      <c r="Y35">
+        <v>2506675</v>
+      </c>
+      <c r="Z35">
+        <v>0</v>
+      </c>
+      <c r="AA35" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB35" s="1" t="s">
+        <v>306</v>
+      </c>
+      <c r="AC35" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A36">
+        <v>1</v>
+      </c>
+      <c r="B36">
+        <v>3</v>
+      </c>
+      <c r="C36" t="s">
+        <v>173</v>
+      </c>
+      <c r="D36">
+        <v>9600</v>
+      </c>
+      <c r="E36">
+        <v>600</v>
+      </c>
+      <c r="F36" t="s">
+        <v>211</v>
+      </c>
+      <c r="G36">
+        <v>1</v>
+      </c>
+      <c r="H36">
+        <v>4</v>
+      </c>
+      <c r="I36">
+        <v>6</v>
+      </c>
+      <c r="J36">
+        <v>4</v>
+      </c>
+      <c r="K36" t="s">
+        <v>268</v>
+      </c>
+      <c r="L36" t="s">
+        <v>186</v>
+      </c>
+      <c r="M36">
+        <v>16</v>
+      </c>
+      <c r="N36">
+        <v>320</v>
+      </c>
+      <c r="O36" t="s">
+        <v>278</v>
+      </c>
+      <c r="P36" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q36">
+        <v>2777.95</v>
+      </c>
+      <c r="R36">
+        <v>3432.6</v>
+      </c>
+      <c r="S36">
+        <v>7428.99</v>
+      </c>
+      <c r="T36">
+        <v>3402.41</v>
+      </c>
+      <c r="V36">
+        <v>3984.68</v>
+      </c>
+      <c r="W36">
+        <v>4255.13</v>
+      </c>
+      <c r="X36">
+        <v>7068.19</v>
+      </c>
+      <c r="Y36">
+        <v>2500154</v>
+      </c>
+      <c r="Z36">
+        <v>0</v>
+      </c>
+      <c r="AA36" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB36" s="1" t="s">
+        <v>307</v>
+      </c>
+      <c r="AC36" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A37">
+        <v>1</v>
+      </c>
+      <c r="B37">
+        <v>3</v>
+      </c>
+      <c r="C37" t="s">
+        <v>173</v>
+      </c>
+      <c r="D37">
+        <v>19200</v>
+      </c>
+      <c r="E37">
+        <v>600</v>
+      </c>
+      <c r="F37" t="s">
+        <v>211</v>
+      </c>
+      <c r="G37">
+        <v>1</v>
+      </c>
+      <c r="H37">
+        <v>4</v>
+      </c>
+      <c r="I37">
+        <v>6</v>
+      </c>
+      <c r="J37">
+        <v>4</v>
+      </c>
+      <c r="K37" t="s">
+        <v>268</v>
+      </c>
+      <c r="L37" t="s">
+        <v>186</v>
+      </c>
+      <c r="M37">
+        <v>16</v>
+      </c>
+      <c r="N37">
+        <v>320</v>
+      </c>
+      <c r="O37" t="s">
+        <v>278</v>
+      </c>
+      <c r="P37" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q37">
+        <v>2740.49</v>
+      </c>
+      <c r="R37">
+        <v>6907.07</v>
+      </c>
+      <c r="S37">
+        <v>20530.78</v>
+      </c>
+      <c r="T37">
+        <v>6905.32</v>
+      </c>
+      <c r="V37">
+        <v>7718.24</v>
+      </c>
+      <c r="W37">
+        <v>8366.3700000000008</v>
+      </c>
+      <c r="X37">
+        <v>10219.85</v>
+      </c>
+      <c r="Y37">
+        <v>2466438</v>
+      </c>
+      <c r="Z37">
+        <v>0</v>
+      </c>
+      <c r="AA37" s="7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="AB37" s="1" t="s">
+        <v>308</v>
+      </c>
+      <c r="AC37" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AA38" s="5"/>
       <c r="AB38" s="1"/>
     </row>
-    <row r="39" spans="27:29" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AA39" s="5"/>
       <c r="AB39" s="1"/>
     </row>
-    <row r="40" spans="27:29" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AA40" s="5"/>
       <c r="AB40" s="1"/>
     </row>
-    <row r="41" spans="27:29" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AA41" s="5"/>
       <c r="AB41" s="1"/>
     </row>
-    <row r="42" spans="27:29" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AA42" s="5"/>
       <c r="AB42" s="1"/>
     </row>
-    <row r="43" spans="27:29" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AA43" s="5"/>
       <c r="AB43" s="1"/>
     </row>
-    <row r="44" spans="27:29" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AA44" s="5"/>
       <c r="AB44" s="1"/>
     </row>
-    <row r="45" spans="27:29" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AA45" s="5"/>
       <c r="AB45" s="1"/>
       <c r="AC45" s="6"/>
     </row>
-    <row r="46" spans="27:29" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AA46" s="5"/>
       <c r="AB46" s="1"/>
     </row>
-    <row r="47" spans="27:29" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AA47" s="5"/>
       <c r="AB47" s="1"/>
     </row>
-    <row r="48" spans="27:29" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AA48" s="5"/>
       <c r="AB48" s="1"/>
     </row>

</xml_diff>

<commit_message>
benchmark after adding pod cpu or memory
</commit_message>
<xml_diff>
--- a/kafka_benchmark/benchmark_stats.xlsx
+++ b/kafka_benchmark/benchmark_stats.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lijjin/Documents/work/git_ws/redistest/kafka_benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50E6EE8E-4AEB-E04F-96FC-E4218ABEE1B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548E28DD-7959-6E4F-B900-3E2A8E28FAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{35590E01-C7C5-464A-8FB5-DBB7ECFA3BB7}"/>
   </bookViews>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2887" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2910" uniqueCount="312">
   <si>
     <t>Partition</t>
   </si>
@@ -959,19 +959,28 @@
     <t>h2load</t>
   </si>
   <si>
-    <t>k8s_1ng_1j_3r_1000t_1200e_4cpu_async2_https_http2</t>
-  </si>
-  <si>
-    <t>k8s_1ng_1j_3r_1000t_2400e_4cpu_async2_https_http2</t>
-  </si>
-  <si>
-    <t>k8s_1ng_1j_3r_1000t_4800e_4cpu_async2_https_http2</t>
-  </si>
-  <si>
-    <t>k8s_1ng_1j_3r_1000t_9600e_4cpu_async2_https_http2</t>
-  </si>
-  <si>
-    <t>k8s_1ng_1j_3r_1000t_19200e_4cpu_async2_https_http2</t>
+    <t>k8s_1ng_1j_3r_1000t_9600e_4cpu_10g_async2_https_http2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_1200t_600e_4cpu_async2_https_http2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_2400t_600e_4cpu_async2_https_http2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_4800t_600e_4cpu_async2_https_http2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_9600t_600e_4cpu_async2_https_http2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_19200t_600e_4cpu_async2_https_http2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_9600t_600e_6cpu_async2_https_http2</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_9600t_600e_6cpu_async2_https</t>
   </si>
 </sst>
 </file>
@@ -1045,7 +1054,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1057,6 +1066,7 @@
     </xf>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1374,8 +1384,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1D1567-5C01-D845-B094-708B919E4B92}">
   <dimension ref="A1:AC60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T12" workbookViewId="0">
-      <selection activeCell="AC38" sqref="AC38"/>
+    <sheetView tabSelected="1" topLeftCell="T15" workbookViewId="0">
+      <selection activeCell="AB40" sqref="AB40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -4090,7 +4100,7 @@
         <v>0</v>
       </c>
       <c r="AB33" s="1" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AC33" t="s">
         <v>303</v>
@@ -4177,7 +4187,7 @@
         <v>0</v>
       </c>
       <c r="AB34" s="1" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AC34" t="s">
         <v>303</v>
@@ -4264,7 +4274,7 @@
         <v>0</v>
       </c>
       <c r="AB35" s="1" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="AC35" t="s">
         <v>303</v>
@@ -4351,7 +4361,7 @@
         <v>0</v>
       </c>
       <c r="AB36" s="1" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AC36" t="s">
         <v>303</v>
@@ -4438,23 +4448,269 @@
         <v>0</v>
       </c>
       <c r="AB37" s="1" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="AC37" t="s">
         <v>303</v>
       </c>
     </row>
     <row r="38" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AA38" s="5"/>
-      <c r="AB38" s="1"/>
+      <c r="A38">
+        <v>1</v>
+      </c>
+      <c r="B38">
+        <v>3</v>
+      </c>
+      <c r="C38" t="s">
+        <v>173</v>
+      </c>
+      <c r="D38">
+        <v>9600</v>
+      </c>
+      <c r="E38">
+        <v>600</v>
+      </c>
+      <c r="F38" t="s">
+        <v>211</v>
+      </c>
+      <c r="G38">
+        <v>1</v>
+      </c>
+      <c r="H38">
+        <v>4</v>
+      </c>
+      <c r="I38">
+        <v>10</v>
+      </c>
+      <c r="J38">
+        <v>4</v>
+      </c>
+      <c r="K38" t="s">
+        <v>268</v>
+      </c>
+      <c r="L38" t="s">
+        <v>186</v>
+      </c>
+      <c r="M38">
+        <v>16</v>
+      </c>
+      <c r="N38">
+        <v>320</v>
+      </c>
+      <c r="O38" t="s">
+        <v>278</v>
+      </c>
+      <c r="P38" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q38">
+        <v>2493.92</v>
+      </c>
+      <c r="R38">
+        <v>3822.88</v>
+      </c>
+      <c r="S38">
+        <v>7328.76</v>
+      </c>
+      <c r="T38">
+        <v>3818.39</v>
+      </c>
+      <c r="V38">
+        <v>4271.87</v>
+      </c>
+      <c r="W38">
+        <v>4458.07</v>
+      </c>
+      <c r="X38">
+        <v>5492.43</v>
+      </c>
+      <c r="Y38">
+        <v>2244524</v>
+      </c>
+      <c r="Z38">
+        <v>0</v>
+      </c>
+      <c r="AA38" s="7">
+        <f t="shared" ref="AA38:AA40" si="1">Z38/Y38</f>
+        <v>0</v>
+      </c>
+      <c r="AB38" s="1" t="s">
+        <v>304</v>
+      </c>
+      <c r="AC38" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="39" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AA39" s="5"/>
-      <c r="AB39" s="1"/>
+      <c r="A39">
+        <v>1</v>
+      </c>
+      <c r="B39">
+        <v>3</v>
+      </c>
+      <c r="C39" t="s">
+        <v>173</v>
+      </c>
+      <c r="D39">
+        <v>9600</v>
+      </c>
+      <c r="E39">
+        <v>600</v>
+      </c>
+      <c r="F39" t="s">
+        <v>211</v>
+      </c>
+      <c r="G39">
+        <v>1</v>
+      </c>
+      <c r="H39">
+        <v>6</v>
+      </c>
+      <c r="I39">
+        <v>6</v>
+      </c>
+      <c r="J39">
+        <v>4</v>
+      </c>
+      <c r="K39" t="s">
+        <v>268</v>
+      </c>
+      <c r="L39" t="s">
+        <v>186</v>
+      </c>
+      <c r="M39">
+        <v>16</v>
+      </c>
+      <c r="N39">
+        <v>320</v>
+      </c>
+      <c r="O39" t="s">
+        <v>278</v>
+      </c>
+      <c r="P39" t="s">
+        <v>298</v>
+      </c>
+      <c r="Q39">
+        <v>2748.75</v>
+      </c>
+      <c r="R39">
+        <v>3469.27</v>
+      </c>
+      <c r="S39">
+        <v>5024.18</v>
+      </c>
+      <c r="T39">
+        <v>3469.75</v>
+      </c>
+      <c r="V39">
+        <v>3840.38</v>
+      </c>
+      <c r="W39">
+        <v>3913.95</v>
+      </c>
+      <c r="X39">
+        <v>3983.14</v>
+      </c>
+      <c r="Y39">
+        <v>2473874</v>
+      </c>
+      <c r="Z39">
+        <v>0</v>
+      </c>
+      <c r="AA39" s="7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB39" s="1" t="s">
+        <v>310</v>
+      </c>
+      <c r="AC39" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="40" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AA40" s="5"/>
-      <c r="AB40" s="1"/>
+      <c r="A40">
+        <v>1</v>
+      </c>
+      <c r="B40">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>173</v>
+      </c>
+      <c r="D40">
+        <v>9600</v>
+      </c>
+      <c r="E40">
+        <v>600</v>
+      </c>
+      <c r="F40" t="s">
+        <v>211</v>
+      </c>
+      <c r="G40">
+        <v>1</v>
+      </c>
+      <c r="H40">
+        <v>6</v>
+      </c>
+      <c r="I40">
+        <v>6</v>
+      </c>
+      <c r="J40">
+        <v>4</v>
+      </c>
+      <c r="K40" t="s">
+        <v>268</v>
+      </c>
+      <c r="L40" t="s">
+        <v>186</v>
+      </c>
+      <c r="M40">
+        <v>16</v>
+      </c>
+      <c r="N40">
+        <v>320</v>
+      </c>
+      <c r="O40" t="s">
+        <v>278</v>
+      </c>
+      <c r="P40" t="s">
+        <v>289</v>
+      </c>
+      <c r="Q40">
+        <v>987.13</v>
+      </c>
+      <c r="R40">
+        <v>433.48</v>
+      </c>
+      <c r="S40">
+        <v>12635</v>
+      </c>
+      <c r="T40">
+        <v>503</v>
+      </c>
+      <c r="V40">
+        <v>2263</v>
+      </c>
+      <c r="W40">
+        <v>3052</v>
+      </c>
+      <c r="X40">
+        <v>3213</v>
+      </c>
+      <c r="Y40">
+        <v>913639</v>
+      </c>
+      <c r="Z40">
+        <v>0</v>
+      </c>
+      <c r="AA40" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AB40" s="1" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="41" spans="1:29" x14ac:dyDescent="0.2">
       <c r="AA41" s="5"/>

</xml_diff>

<commit_message>
zgc support. Use log4j2 2.15.0 to fix log4j security holes
</commit_message>
<xml_diff>
--- a/kafka_benchmark/benchmark_stats.xlsx
+++ b/kafka_benchmark/benchmark_stats.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11010"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11114"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lijjin/Documents/work/git_ws/redistest/kafka_benchmark/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548E28DD-7959-6E4F-B900-3E2A8E28FAAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F98291C8-0F3B-4044-9982-203F8AA1F50A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16460" xr2:uid="{35590E01-C7C5-464A-8FB5-DBB7ECFA3BB7}"/>
   </bookViews>
@@ -21,7 +21,7 @@
     <sheet name="600 executor" sheetId="3" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Authz!$A$2:$AC$42</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Authz!$A$2:$AE$47</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Kafka Producer'!$A$1:$AD$35</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2910" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3008" uniqueCount="324">
   <si>
     <t>Partition</t>
   </si>
@@ -981,6 +981,42 @@
   </si>
   <si>
     <t>k8s_1ng_1j_3r_9600t_600e_6cpu_async2_https</t>
+  </si>
+  <si>
+    <t>GW Memory</t>
+  </si>
+  <si>
+    <t>Jdk Version</t>
+  </si>
+  <si>
+    <t>GC Alg.</t>
+  </si>
+  <si>
+    <t>G1</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_9600t_600e_4cpu_async2_https_jdk11_zgc</t>
+  </si>
+  <si>
+    <t>ZGC</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_9600t_600e_4cpu_async2_https_jdk17_zgc.1</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_9600t_600e_4cpu_async2_https_http2_jdk17_zgc</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_19200t_600e_4cpu_async2_https_jdk17_zgc</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_4800t_600e_4cpu_async2_https_jdk17_zgc</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_1200t_600e_4cpu_async2_https_jdk17_zgc</t>
+  </si>
+  <si>
+    <t>k8s_1ng_1j_3r_2400t_600e_4cpu_async2_https_jdk17_zgc.1</t>
   </si>
 </sst>
 </file>
@@ -1382,10 +1418,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ED1D1567-5C01-D845-B094-708B919E4B92}">
-  <dimension ref="A1:AC60"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:AE60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="T15" workbookViewId="0">
-      <selection activeCell="AB40" sqref="AB40"/>
+    <sheetView tabSelected="1" topLeftCell="T1" workbookViewId="0">
+      <selection activeCell="Y46" sqref="Y46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1397,20 +1434,20 @@
     <col min="6" max="6" width="15.83203125" customWidth="1"/>
     <col min="7" max="7" width="11.33203125" customWidth="1"/>
     <col min="8" max="8" width="9.1640625" customWidth="1"/>
-    <col min="9" max="11" width="9" customWidth="1"/>
-    <col min="12" max="15" width="12" customWidth="1"/>
-    <col min="16" max="16" width="9.33203125" customWidth="1"/>
-    <col min="17" max="17" width="15" customWidth="1"/>
-    <col min="18" max="19" width="21.1640625" customWidth="1"/>
-    <col min="20" max="20" width="24.5" customWidth="1"/>
-    <col min="21" max="24" width="21.1640625" customWidth="1"/>
-    <col min="25" max="25" width="14.6640625" customWidth="1"/>
-    <col min="26" max="27" width="11.33203125" customWidth="1"/>
-    <col min="28" max="28" width="57.1640625" customWidth="1"/>
-    <col min="29" max="29" width="31.6640625" customWidth="1"/>
+    <col min="9" max="13" width="9" customWidth="1"/>
+    <col min="14" max="17" width="12" customWidth="1"/>
+    <col min="18" max="18" width="9.33203125" customWidth="1"/>
+    <col min="19" max="19" width="15" customWidth="1"/>
+    <col min="20" max="21" width="21.1640625" customWidth="1"/>
+    <col min="22" max="22" width="24.5" customWidth="1"/>
+    <col min="23" max="26" width="21.1640625" customWidth="1"/>
+    <col min="27" max="27" width="14.6640625" customWidth="1"/>
+    <col min="28" max="29" width="11.33203125" customWidth="1"/>
+    <col min="30" max="30" width="62.1640625" customWidth="1"/>
+    <col min="31" max="31" width="31.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:29" s="6" customFormat="1" ht="119" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" s="6" customFormat="1" ht="119" x14ac:dyDescent="0.2">
       <c r="A1" s="6" t="s">
         <v>248</v>
       </c>
@@ -1430,7 +1467,7 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>244</v>
       </c>
@@ -1459,64 +1496,73 @@
         <v>266</v>
       </c>
       <c r="J2" t="s">
+        <v>313</v>
+      </c>
+      <c r="K2" t="s">
+        <v>314</v>
+      </c>
+      <c r="L2" t="s">
         <v>267</v>
       </c>
-      <c r="L2" t="s">
+      <c r="M2" t="s">
+        <v>312</v>
+      </c>
+      <c r="N2" t="s">
         <v>184</v>
       </c>
-      <c r="M2" t="s">
+      <c r="O2" t="s">
         <v>271</v>
       </c>
-      <c r="N2" t="s">
+      <c r="P2" t="s">
         <v>272</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" t="s">
         <v>274</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>297</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" t="s">
         <v>129</v>
       </c>
-      <c r="R2" t="s">
+      <c r="T2" t="s">
         <v>134</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
         <v>135</v>
       </c>
-      <c r="T2" s="3" t="s">
+      <c r="V2" s="3" t="s">
         <v>136</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="Y2" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="X2" s="3" t="s">
+      <c r="Z2" s="3" t="s">
         <v>263</v>
       </c>
-      <c r="Y2" s="3" t="s">
+      <c r="AA2" s="3" t="s">
         <v>157</v>
       </c>
-      <c r="Z2" s="3" t="s">
+      <c r="AB2" s="3" t="s">
         <v>188</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>194</v>
       </c>
-      <c r="AB2" t="s">
+      <c r="AD2" t="s">
         <v>7</v>
       </c>
-      <c r="AC2" t="s">
+      <c r="AE2" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="3" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1545,63 +1591,69 @@
         <v>6</v>
       </c>
       <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3" t="s">
+        <v>315</v>
+      </c>
+      <c r="L3">
         <v>4</v>
       </c>
-      <c r="K3" t="s">
+      <c r="M3" t="s">
         <v>268</v>
       </c>
-      <c r="L3" t="s">
+      <c r="N3" t="s">
         <v>186</v>
       </c>
-      <c r="M3">
+      <c r="O3">
         <v>16</v>
       </c>
-      <c r="N3">
+      <c r="P3">
         <v>320</v>
       </c>
-      <c r="O3" t="s">
+      <c r="Q3" t="s">
         <v>275</v>
       </c>
-      <c r="P3" t="s">
+      <c r="R3" t="s">
         <v>288</v>
       </c>
-      <c r="Q3">
+      <c r="S3">
         <v>1000.51</v>
       </c>
-      <c r="R3">
+      <c r="T3">
         <v>1437.21</v>
       </c>
-      <c r="S3">
+      <c r="U3">
         <v>11377</v>
       </c>
-      <c r="T3">
+      <c r="V3">
         <v>3098</v>
       </c>
-      <c r="U3" s="3"/>
-      <c r="V3">
+      <c r="W3" s="3"/>
+      <c r="X3">
         <v>5381.99</v>
       </c>
-      <c r="W3">
+      <c r="Y3">
         <v>6223</v>
       </c>
-      <c r="X3">
+      <c r="Z3">
         <v>6314.99</v>
       </c>
-      <c r="Y3">
+      <c r="AA3">
         <v>917790</v>
       </c>
-      <c r="Z3" s="3">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="8">
-        <f t="shared" ref="AA3:AA37" si="0">Z3/Y3</f>
-        <v>0</v>
-      </c>
-      <c r="AB3" s="1" t="s">
+      <c r="AB3" s="3">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="8">
+        <f t="shared" ref="AC3:AC37" si="0">AB3/AA3</f>
+        <v>0</v>
+      </c>
+      <c r="AD3" s="1" t="s">
         <v>270</v>
       </c>
     </row>
-    <row r="4" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>1</v>
       </c>
@@ -1630,62 +1682,68 @@
         <v>6</v>
       </c>
       <c r="J4">
+        <v>11</v>
+      </c>
+      <c r="K4" t="s">
+        <v>315</v>
+      </c>
+      <c r="L4">
         <v>0.1</v>
       </c>
-      <c r="K4" t="s">
+      <c r="M4" t="s">
         <v>269</v>
       </c>
-      <c r="L4" t="s">
+      <c r="N4" t="s">
         <v>186</v>
       </c>
-      <c r="M4">
+      <c r="O4">
         <v>16</v>
       </c>
-      <c r="N4">
+      <c r="P4">
         <v>320</v>
       </c>
-      <c r="O4" t="s">
+      <c r="Q4" t="s">
         <v>275</v>
       </c>
-      <c r="P4" t="s">
+      <c r="R4" t="s">
         <v>288</v>
       </c>
-      <c r="Q4">
+      <c r="S4">
         <v>994.96</v>
       </c>
-      <c r="R4">
+      <c r="T4">
         <v>1263.78</v>
       </c>
-      <c r="S4">
+      <c r="U4">
         <v>11563</v>
       </c>
-      <c r="T4" s="3">
+      <c r="V4" s="3">
         <v>85</v>
       </c>
-      <c r="U4">
+      <c r="W4">
         <v>6388.95</v>
       </c>
-      <c r="V4">
+      <c r="X4">
         <v>6853</v>
       </c>
-      <c r="Y4">
+      <c r="AA4">
         <v>915679</v>
       </c>
-      <c r="Z4">
+      <c r="AB4">
         <v>133</v>
       </c>
-      <c r="AA4" s="8">
+      <c r="AC4" s="8">
         <f t="shared" si="0"/>
         <v>1.4524740656933271E-4</v>
       </c>
-      <c r="AB4" s="1" t="s">
+      <c r="AD4" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="AC4" t="s">
+      <c r="AE4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="5" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>1</v>
       </c>
@@ -1713,63 +1771,69 @@
       <c r="I5">
         <v>6</v>
       </c>
-      <c r="J5" s="3">
+      <c r="J5">
+        <v>11</v>
+      </c>
+      <c r="K5" t="s">
+        <v>315</v>
+      </c>
+      <c r="L5" s="3">
         <v>4</v>
       </c>
-      <c r="K5" s="3" t="s">
+      <c r="M5" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="L5" t="s">
+      <c r="N5" t="s">
         <v>186</v>
       </c>
-      <c r="M5">
+      <c r="O5">
         <v>16</v>
       </c>
-      <c r="N5">
+      <c r="P5">
         <v>320</v>
       </c>
-      <c r="O5" t="s">
+      <c r="Q5" t="s">
         <v>275</v>
       </c>
-      <c r="P5" t="s">
+      <c r="R5" t="s">
         <v>288</v>
       </c>
-      <c r="Q5">
+      <c r="S5">
         <v>999.99</v>
       </c>
-      <c r="R5">
+      <c r="T5">
         <v>684.69</v>
       </c>
-      <c r="S5">
+      <c r="U5">
         <v>6792</v>
       </c>
-      <c r="T5">
+      <c r="V5">
         <v>240</v>
       </c>
-      <c r="V5">
+      <c r="X5">
         <v>3527</v>
       </c>
-      <c r="W5">
+      <c r="Y5">
         <v>3564</v>
       </c>
-      <c r="X5">
+      <c r="Z5">
         <v>4128</v>
       </c>
-      <c r="Y5">
+      <c r="AA5">
         <v>909719</v>
       </c>
-      <c r="Z5">
-        <v>0</v>
-      </c>
-      <c r="AA5" s="7">
+      <c r="AB5">
+        <v>0</v>
+      </c>
+      <c r="AC5" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB5" s="1" t="s">
+      <c r="AD5" s="1" t="s">
         <v>286</v>
       </c>
     </row>
-    <row r="6" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1798,59 +1862,65 @@
         <v>6</v>
       </c>
       <c r="J6">
+        <v>11</v>
+      </c>
+      <c r="K6" t="s">
+        <v>315</v>
+      </c>
+      <c r="L6">
         <v>0.1</v>
       </c>
-      <c r="K6" t="s">
+      <c r="M6" t="s">
         <v>269</v>
       </c>
-      <c r="L6" t="s">
+      <c r="N6" t="s">
         <v>186</v>
       </c>
-      <c r="M6">
+      <c r="O6">
         <v>16</v>
       </c>
-      <c r="N6">
+      <c r="P6">
         <v>320</v>
       </c>
-      <c r="O6" t="s">
+      <c r="Q6" t="s">
         <v>275</v>
       </c>
-      <c r="P6" t="s">
+      <c r="R6" t="s">
         <v>288</v>
       </c>
-      <c r="Q6">
+      <c r="S6">
         <v>997.84</v>
       </c>
-      <c r="R6">
+      <c r="T6">
         <v>361.26</v>
       </c>
-      <c r="S6">
+      <c r="U6">
         <v>3952</v>
       </c>
-      <c r="T6">
+      <c r="V6">
         <v>65</v>
       </c>
-      <c r="U6">
+      <c r="W6">
         <v>116</v>
       </c>
-      <c r="V6">
+      <c r="X6">
         <v>236</v>
       </c>
-      <c r="Y6">
+      <c r="AA6">
         <v>903334</v>
       </c>
-      <c r="Z6">
-        <v>0</v>
-      </c>
-      <c r="AA6" s="7">
+      <c r="AB6">
+        <v>0</v>
+      </c>
+      <c r="AC6" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB6" s="1" t="s">
+      <c r="AD6" s="1" t="s">
         <v>252</v>
       </c>
     </row>
-    <row r="7" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A7">
         <v>1</v>
       </c>
@@ -1879,62 +1949,68 @@
         <v>6</v>
       </c>
       <c r="J7">
+        <v>11</v>
+      </c>
+      <c r="K7" t="s">
+        <v>315</v>
+      </c>
+      <c r="L7">
         <v>0.1</v>
       </c>
-      <c r="K7" t="s">
+      <c r="M7" t="s">
         <v>269</v>
       </c>
-      <c r="L7" t="s">
+      <c r="N7" t="s">
         <v>186</v>
       </c>
-      <c r="M7">
+      <c r="O7">
         <v>16</v>
       </c>
-      <c r="N7">
+      <c r="P7">
         <v>320</v>
       </c>
-      <c r="O7" t="s">
+      <c r="Q7" t="s">
         <v>275</v>
       </c>
-      <c r="P7" t="s">
+      <c r="R7" t="s">
         <v>288</v>
       </c>
-      <c r="Q7">
+      <c r="S7">
         <v>992.45</v>
       </c>
-      <c r="R7">
+      <c r="T7">
         <v>350.12</v>
       </c>
-      <c r="S7">
+      <c r="U7">
         <v>4931</v>
       </c>
-      <c r="T7">
+      <c r="V7">
         <v>892</v>
       </c>
-      <c r="U7">
+      <c r="W7">
         <v>1858</v>
       </c>
-      <c r="V7">
+      <c r="X7">
         <v>1927</v>
       </c>
-      <c r="Y7">
+      <c r="AA7">
         <v>899083</v>
       </c>
-      <c r="Z7">
-        <v>0</v>
-      </c>
-      <c r="AA7" s="7">
+      <c r="AB7">
+        <v>0</v>
+      </c>
+      <c r="AC7" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB7" s="1" t="s">
+      <c r="AD7" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="AC7" t="s">
+      <c r="AE7" t="s">
         <v>273</v>
       </c>
     </row>
-    <row r="8" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A8">
         <v>1</v>
       </c>
@@ -1963,62 +2039,68 @@
         <v>6</v>
       </c>
       <c r="J8">
+        <v>11</v>
+      </c>
+      <c r="K8" t="s">
+        <v>315</v>
+      </c>
+      <c r="L8">
         <v>0.1</v>
       </c>
-      <c r="K8" t="s">
+      <c r="M8" t="s">
         <v>269</v>
       </c>
-      <c r="L8" t="s">
+      <c r="N8" t="s">
         <v>186</v>
       </c>
-      <c r="M8">
+      <c r="O8">
         <v>16</v>
       </c>
-      <c r="N8">
+      <c r="P8">
         <v>320</v>
       </c>
-      <c r="O8" t="s">
+      <c r="Q8" t="s">
         <v>275</v>
       </c>
-      <c r="P8" t="s">
+      <c r="R8" t="s">
         <v>288</v>
       </c>
-      <c r="Q8">
+      <c r="S8">
         <v>999.27</v>
       </c>
-      <c r="R8">
+      <c r="T8">
         <v>296.02</v>
       </c>
-      <c r="S8">
+      <c r="U8">
         <v>2501</v>
       </c>
-      <c r="T8">
+      <c r="V8">
         <v>347</v>
       </c>
-      <c r="V8">
+      <c r="X8">
         <v>1087</v>
       </c>
-      <c r="W8">
+      <c r="Y8">
         <v>1118</v>
       </c>
-      <c r="X8">
+      <c r="Z8">
         <v>1125</v>
       </c>
-      <c r="Y8">
+      <c r="AA8">
         <v>900120</v>
       </c>
-      <c r="Z8">
-        <v>0</v>
-      </c>
-      <c r="AA8" s="7">
+      <c r="AB8">
+        <v>0</v>
+      </c>
+      <c r="AC8" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB8" s="1" t="s">
+      <c r="AD8" s="1" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="9" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>1</v>
       </c>
@@ -2047,59 +2129,65 @@
         <v>6</v>
       </c>
       <c r="J9">
+        <v>11</v>
+      </c>
+      <c r="K9" t="s">
+        <v>315</v>
+      </c>
+      <c r="L9">
         <v>0.1</v>
       </c>
-      <c r="K9" t="s">
+      <c r="M9" t="s">
         <v>269</v>
       </c>
-      <c r="L9" t="s">
+      <c r="N9" t="s">
         <v>186</v>
       </c>
-      <c r="M9">
+      <c r="O9">
         <v>16</v>
       </c>
-      <c r="N9">
+      <c r="P9">
         <v>320</v>
       </c>
-      <c r="O9" t="s">
+      <c r="Q9" t="s">
         <v>275</v>
       </c>
-      <c r="P9" t="s">
+      <c r="R9" t="s">
         <v>288</v>
       </c>
-      <c r="Q9">
+      <c r="S9">
         <v>997.36</v>
       </c>
-      <c r="R9">
+      <c r="T9">
         <v>175.85</v>
       </c>
-      <c r="S9">
+      <c r="U9">
         <v>844</v>
       </c>
-      <c r="T9">
+      <c r="V9">
         <v>73</v>
       </c>
-      <c r="U9">
+      <c r="W9">
         <v>512</v>
       </c>
-      <c r="V9">
+      <c r="X9">
         <v>567.99</v>
       </c>
-      <c r="Y9">
+      <c r="AA9">
         <v>898286</v>
       </c>
-      <c r="Z9">
-        <v>0</v>
-      </c>
-      <c r="AA9" s="7">
+      <c r="AB9">
+        <v>0</v>
+      </c>
+      <c r="AC9" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB9" s="1" t="s">
+      <c r="AD9" s="1" t="s">
         <v>255</v>
       </c>
     </row>
-    <row r="10" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>1</v>
       </c>
@@ -2128,59 +2216,65 @@
         <v>6</v>
       </c>
       <c r="J10">
+        <v>11</v>
+      </c>
+      <c r="K10" t="s">
+        <v>315</v>
+      </c>
+      <c r="L10">
         <v>0.1</v>
       </c>
-      <c r="K10" t="s">
+      <c r="M10" t="s">
         <v>269</v>
       </c>
-      <c r="L10" t="s">
+      <c r="N10" t="s">
         <v>186</v>
       </c>
-      <c r="M10">
+      <c r="O10">
         <v>16</v>
       </c>
-      <c r="N10">
+      <c r="P10">
         <v>320</v>
       </c>
-      <c r="O10" t="s">
+      <c r="Q10" t="s">
         <v>275</v>
       </c>
-      <c r="P10" t="s">
+      <c r="R10" t="s">
         <v>288</v>
       </c>
-      <c r="Q10">
+      <c r="S10">
         <v>994.77</v>
       </c>
-      <c r="R10">
+      <c r="T10">
         <v>95.03</v>
       </c>
-      <c r="S10">
+      <c r="U10">
         <v>520</v>
       </c>
-      <c r="T10">
+      <c r="V10">
         <v>64</v>
       </c>
-      <c r="U10">
+      <c r="W10">
         <v>274</v>
       </c>
-      <c r="V10">
+      <c r="X10">
         <v>329</v>
       </c>
-      <c r="Y10">
+      <c r="AA10">
         <v>895808</v>
       </c>
-      <c r="Z10">
-        <v>0</v>
-      </c>
-      <c r="AA10" s="7">
+      <c r="AB10">
+        <v>0</v>
+      </c>
+      <c r="AC10" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB10" s="1" t="s">
+      <c r="AD10" s="1" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="11" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>1</v>
       </c>
@@ -2209,59 +2303,65 @@
         <v>6</v>
       </c>
       <c r="J11">
+        <v>11</v>
+      </c>
+      <c r="K11" t="s">
+        <v>315</v>
+      </c>
+      <c r="L11">
         <v>0.1</v>
       </c>
-      <c r="K11" t="s">
+      <c r="M11" t="s">
         <v>269</v>
       </c>
-      <c r="L11" t="s">
+      <c r="N11" t="s">
         <v>186</v>
       </c>
-      <c r="M11">
+      <c r="O11">
         <v>16</v>
       </c>
-      <c r="N11">
+      <c r="P11">
         <v>320</v>
       </c>
-      <c r="O11" t="s">
+      <c r="Q11" t="s">
         <v>275</v>
       </c>
-      <c r="P11" t="s">
+      <c r="R11" t="s">
         <v>288</v>
       </c>
-      <c r="Q11">
+      <c r="S11">
         <v>996.89</v>
       </c>
-      <c r="R11">
+      <c r="T11">
         <v>71.040000000000006</v>
       </c>
-      <c r="S11">
+      <c r="U11">
         <v>330</v>
       </c>
-      <c r="T11">
+      <c r="V11">
         <v>63</v>
       </c>
-      <c r="U11">
+      <c r="W11">
         <v>113</v>
       </c>
-      <c r="V11">
+      <c r="X11">
         <v>164</v>
       </c>
-      <c r="Y11">
+      <c r="AA11">
         <v>897305</v>
       </c>
-      <c r="Z11">
-        <v>0</v>
-      </c>
-      <c r="AA11" s="7">
+      <c r="AB11">
+        <v>0</v>
+      </c>
+      <c r="AC11" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB11" s="1" t="s">
+      <c r="AD11" s="1" t="s">
         <v>257</v>
       </c>
     </row>
-    <row r="12" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>1</v>
       </c>
@@ -2290,59 +2390,65 @@
         <v>6</v>
       </c>
       <c r="J12">
+        <v>11</v>
+      </c>
+      <c r="K12" t="s">
+        <v>315</v>
+      </c>
+      <c r="L12">
         <v>0.1</v>
       </c>
-      <c r="K12" t="s">
+      <c r="M12" t="s">
         <v>269</v>
       </c>
-      <c r="L12" t="s">
+      <c r="N12" t="s">
         <v>186</v>
       </c>
-      <c r="M12">
+      <c r="O12">
         <v>16</v>
       </c>
-      <c r="N12">
+      <c r="P12">
         <v>320</v>
       </c>
-      <c r="O12" t="s">
+      <c r="Q12" t="s">
         <v>275</v>
       </c>
-      <c r="P12" t="s">
+      <c r="R12" t="s">
         <v>288</v>
       </c>
-      <c r="Q12">
+      <c r="S12">
         <v>1015.9</v>
       </c>
-      <c r="R12">
+      <c r="T12">
         <v>2280.6799999999998</v>
       </c>
-      <c r="S12">
+      <c r="U12">
         <v>12474</v>
       </c>
-      <c r="T12">
+      <c r="V12">
         <v>255</v>
       </c>
-      <c r="U12">
+      <c r="W12">
         <v>4845</v>
       </c>
-      <c r="V12">
+      <c r="X12">
         <v>5355</v>
       </c>
-      <c r="Y12">
+      <c r="AA12">
         <v>933808</v>
       </c>
-      <c r="Z12">
-        <v>0</v>
-      </c>
-      <c r="AA12" s="7">
+      <c r="AB12">
+        <v>0</v>
+      </c>
+      <c r="AC12" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB12" s="1" t="s">
+      <c r="AD12" s="1" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="13" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A13">
         <v>1</v>
       </c>
@@ -2371,59 +2477,65 @@
         <v>6</v>
       </c>
       <c r="J13">
+        <v>11</v>
+      </c>
+      <c r="K13" t="s">
+        <v>315</v>
+      </c>
+      <c r="L13">
         <v>0.1</v>
       </c>
-      <c r="K13" t="s">
+      <c r="M13" t="s">
         <v>269</v>
       </c>
-      <c r="L13" t="s">
+      <c r="N13" t="s">
         <v>186</v>
       </c>
-      <c r="M13">
+      <c r="O13">
         <v>16</v>
       </c>
-      <c r="N13">
+      <c r="P13">
         <v>320</v>
       </c>
-      <c r="O13" t="s">
+      <c r="Q13" t="s">
         <v>275</v>
       </c>
-      <c r="P13" t="s">
+      <c r="R13" t="s">
         <v>288</v>
       </c>
-      <c r="Q13">
+      <c r="S13">
         <v>999.93</v>
       </c>
-      <c r="R13">
+      <c r="T13">
         <v>545.72</v>
       </c>
-      <c r="S13">
+      <c r="U13">
         <v>6965</v>
       </c>
-      <c r="T13">
+      <c r="V13">
         <v>61</v>
       </c>
-      <c r="U13">
+      <c r="W13">
         <v>242</v>
       </c>
-      <c r="V13">
+      <c r="X13">
         <v>375</v>
       </c>
-      <c r="Y13">
+      <c r="AA13">
         <v>914739</v>
       </c>
-      <c r="Z13">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="7">
+      <c r="AB13">
+        <v>0</v>
+      </c>
+      <c r="AC13" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB13" s="1" t="s">
+      <c r="AD13" s="1" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="14" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A14">
         <v>1</v>
       </c>
@@ -2452,62 +2564,68 @@
         <v>6</v>
       </c>
       <c r="J14">
+        <v>11</v>
+      </c>
+      <c r="K14" t="s">
+        <v>315</v>
+      </c>
+      <c r="L14">
         <v>0.1</v>
       </c>
-      <c r="K14" t="s">
+      <c r="M14" t="s">
         <v>269</v>
       </c>
-      <c r="L14" t="s">
+      <c r="N14" t="s">
         <v>186</v>
       </c>
-      <c r="M14">
+      <c r="O14">
         <v>16</v>
       </c>
-      <c r="N14">
+      <c r="P14">
         <v>320</v>
       </c>
-      <c r="O14" t="s">
+      <c r="Q14" t="s">
         <v>275</v>
       </c>
-      <c r="P14" t="s">
+      <c r="R14" t="s">
         <v>288</v>
       </c>
-      <c r="Q14">
+      <c r="S14">
         <v>998.89</v>
       </c>
-      <c r="R14">
+      <c r="T14">
         <v>443.15</v>
       </c>
-      <c r="S14">
+      <c r="U14">
         <v>3530</v>
       </c>
-      <c r="T14">
+      <c r="V14">
         <v>65</v>
       </c>
-      <c r="V14">
+      <c r="X14">
         <v>112</v>
       </c>
-      <c r="W14">
+      <c r="Y14">
         <v>117</v>
       </c>
-      <c r="X14">
+      <c r="Z14">
         <v>459.97</v>
       </c>
-      <c r="Y14">
+      <c r="AA14">
         <v>904625</v>
       </c>
-      <c r="Z14">
-        <v>0</v>
-      </c>
-      <c r="AA14" s="7">
+      <c r="AB14">
+        <v>0</v>
+      </c>
+      <c r="AC14" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB14" s="1" t="s">
+      <c r="AD14" s="1" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="15" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>1</v>
       </c>
@@ -2536,62 +2654,68 @@
         <v>6</v>
       </c>
       <c r="J15">
+        <v>11</v>
+      </c>
+      <c r="K15" t="s">
+        <v>315</v>
+      </c>
+      <c r="L15">
         <v>0.1</v>
       </c>
-      <c r="K15" t="s">
+      <c r="M15" t="s">
         <v>269</v>
       </c>
-      <c r="L15" t="s">
+      <c r="N15" t="s">
         <v>186</v>
       </c>
-      <c r="M15">
+      <c r="O15">
         <v>16</v>
       </c>
-      <c r="N15">
+      <c r="P15">
         <v>320</v>
       </c>
-      <c r="O15" t="s">
+      <c r="Q15" t="s">
         <v>276</v>
       </c>
-      <c r="P15" t="s">
+      <c r="R15" t="s">
         <v>288</v>
       </c>
-      <c r="Q15">
+      <c r="S15">
         <v>632.79</v>
       </c>
-      <c r="R15">
+      <c r="T15">
         <v>303.64</v>
       </c>
-      <c r="S15">
+      <c r="U15">
         <v>5665</v>
       </c>
-      <c r="T15">
+      <c r="V15">
         <v>26</v>
       </c>
-      <c r="V15">
+      <c r="X15">
         <v>315.99</v>
       </c>
-      <c r="W15">
+      <c r="Y15">
         <v>474</v>
       </c>
-      <c r="X15">
+      <c r="Z15">
         <v>582</v>
       </c>
-      <c r="Y15">
+      <c r="AA15">
         <v>569571</v>
       </c>
-      <c r="Z15">
-        <v>0</v>
-      </c>
-      <c r="AA15" s="7">
+      <c r="AB15">
+        <v>0</v>
+      </c>
+      <c r="AC15" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB15" s="1" t="s">
+      <c r="AD15" s="1" t="s">
         <v>277</v>
       </c>
     </row>
-    <row r="16" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>1</v>
       </c>
@@ -2620,62 +2744,68 @@
         <v>6</v>
       </c>
       <c r="J16">
+        <v>11</v>
+      </c>
+      <c r="K16" t="s">
+        <v>315</v>
+      </c>
+      <c r="L16">
         <v>4</v>
       </c>
-      <c r="K16" t="s">
+      <c r="M16" t="s">
         <v>268</v>
       </c>
-      <c r="L16" t="s">
+      <c r="N16" t="s">
         <v>186</v>
       </c>
-      <c r="M16">
+      <c r="O16">
         <v>16</v>
       </c>
-      <c r="N16">
+      <c r="P16">
         <v>320</v>
       </c>
-      <c r="O16" t="s">
+      <c r="Q16" t="s">
         <v>278</v>
       </c>
-      <c r="P16" t="s">
+      <c r="R16" t="s">
         <v>288</v>
       </c>
-      <c r="Q16">
+      <c r="S16">
         <v>996.18</v>
       </c>
-      <c r="R16">
+      <c r="T16">
         <v>26.24</v>
       </c>
-      <c r="S16">
+      <c r="U16">
         <v>215</v>
       </c>
-      <c r="T16">
+      <c r="V16">
         <v>21</v>
       </c>
-      <c r="V16">
+      <c r="X16">
         <v>122</v>
       </c>
-      <c r="W16">
+      <c r="Y16">
         <v>144</v>
       </c>
-      <c r="X16">
+      <c r="Z16">
         <v>151</v>
       </c>
-      <c r="Y16">
+      <c r="AA16">
         <v>896683</v>
       </c>
-      <c r="Z16">
-        <v>0</v>
-      </c>
-      <c r="AA16" s="7">
+      <c r="AB16">
+        <v>0</v>
+      </c>
+      <c r="AC16" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB16" s="1" t="s">
+      <c r="AD16" s="1" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="17" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>1</v>
       </c>
@@ -2704,62 +2834,68 @@
         <v>6</v>
       </c>
       <c r="J17">
+        <v>11</v>
+      </c>
+      <c r="K17" t="s">
+        <v>315</v>
+      </c>
+      <c r="L17">
         <v>4</v>
       </c>
-      <c r="K17" t="s">
+      <c r="M17" t="s">
         <v>268</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="N17" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="M17" s="3">
+      <c r="O17" s="3">
         <v>16</v>
       </c>
-      <c r="N17" s="3">
+      <c r="P17" s="3">
         <v>320</v>
       </c>
-      <c r="O17" s="3" t="s">
+      <c r="Q17" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="P17" t="s">
+      <c r="R17" t="s">
         <v>288</v>
       </c>
-      <c r="Q17">
+      <c r="S17">
         <v>996.61</v>
       </c>
-      <c r="R17">
+      <c r="T17">
         <v>41.68</v>
       </c>
-      <c r="S17" s="3">
+      <c r="U17" s="3">
         <v>348</v>
       </c>
-      <c r="T17" s="3">
+      <c r="V17" s="3">
         <v>23</v>
       </c>
-      <c r="V17">
+      <c r="X17">
         <v>270</v>
       </c>
-      <c r="W17">
+      <c r="Y17">
         <v>304</v>
       </c>
-      <c r="X17">
+      <c r="Z17">
         <v>312</v>
       </c>
-      <c r="Y17">
+      <c r="AA17">
         <v>897508</v>
       </c>
-      <c r="Z17">
-        <v>0</v>
-      </c>
-      <c r="AA17" s="7">
+      <c r="AB17">
+        <v>0</v>
+      </c>
+      <c r="AC17" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB17" s="1" t="s">
+      <c r="AD17" s="1" t="s">
         <v>285</v>
       </c>
     </row>
-    <row r="18" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>1</v>
       </c>
@@ -2788,62 +2924,68 @@
         <v>6</v>
       </c>
       <c r="J18">
+        <v>11</v>
+      </c>
+      <c r="K18" t="s">
+        <v>315</v>
+      </c>
+      <c r="L18">
         <v>4</v>
       </c>
-      <c r="K18" t="s">
+      <c r="M18" t="s">
         <v>268</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="N18" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="M18" s="3">
+      <c r="O18" s="3">
         <v>16</v>
       </c>
-      <c r="N18" s="3">
+      <c r="P18" s="3">
         <v>320</v>
       </c>
-      <c r="O18" s="3" t="s">
+      <c r="Q18" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="P18" t="s">
+      <c r="R18" t="s">
         <v>288</v>
       </c>
-      <c r="Q18">
+      <c r="S18">
         <v>996.53</v>
       </c>
-      <c r="R18">
+      <c r="T18">
         <v>91.06</v>
       </c>
-      <c r="S18">
+      <c r="U18">
         <v>1070</v>
       </c>
-      <c r="T18">
+      <c r="V18">
         <v>27</v>
       </c>
-      <c r="V18">
+      <c r="X18">
         <v>417</v>
       </c>
-      <c r="W18">
+      <c r="Y18">
         <v>442</v>
       </c>
-      <c r="X18">
+      <c r="Z18">
         <v>446</v>
       </c>
-      <c r="Y18">
+      <c r="AA18">
         <v>898225</v>
       </c>
-      <c r="Z18">
-        <v>0</v>
-      </c>
-      <c r="AA18" s="7">
+      <c r="AB18">
+        <v>0</v>
+      </c>
+      <c r="AC18" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB18" s="1" t="s">
+      <c r="AD18" s="1" t="s">
         <v>284</v>
       </c>
     </row>
-    <row r="19" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>1</v>
       </c>
@@ -2872,62 +3014,68 @@
         <v>6</v>
       </c>
       <c r="J19">
+        <v>11</v>
+      </c>
+      <c r="K19" t="s">
+        <v>315</v>
+      </c>
+      <c r="L19">
         <v>4</v>
       </c>
-      <c r="K19" t="s">
+      <c r="M19" t="s">
         <v>268</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="N19" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="M19" s="3">
+      <c r="O19" s="3">
         <v>16</v>
       </c>
-      <c r="N19" s="3">
+      <c r="P19" s="3">
         <v>320</v>
       </c>
-      <c r="O19" s="3" t="s">
+      <c r="Q19" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="P19" t="s">
+      <c r="R19" t="s">
         <v>288</v>
       </c>
-      <c r="Q19">
+      <c r="S19">
         <v>997.26</v>
       </c>
-      <c r="R19">
+      <c r="T19">
         <v>212.8</v>
       </c>
-      <c r="S19">
+      <c r="U19">
         <v>3066</v>
       </c>
-      <c r="T19">
+      <c r="V19">
         <v>287</v>
       </c>
-      <c r="V19">
+      <c r="X19">
         <v>860</v>
       </c>
-      <c r="W19">
+      <c r="Y19">
         <v>888</v>
       </c>
-      <c r="X19">
+      <c r="Z19">
         <v>898</v>
       </c>
-      <c r="Y19">
+      <c r="AA19">
         <v>901434</v>
       </c>
-      <c r="Z19">
-        <v>0</v>
-      </c>
-      <c r="AA19" s="7">
+      <c r="AB19">
+        <v>0</v>
+      </c>
+      <c r="AC19" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB19" s="1" t="s">
+      <c r="AD19" s="1" t="s">
         <v>283</v>
       </c>
     </row>
-    <row r="20" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A20">
         <v>1</v>
       </c>
@@ -2956,62 +3104,68 @@
         <v>6</v>
       </c>
       <c r="J20">
+        <v>11</v>
+      </c>
+      <c r="K20" t="s">
+        <v>315</v>
+      </c>
+      <c r="L20">
         <v>4</v>
       </c>
-      <c r="K20" t="s">
+      <c r="M20" t="s">
         <v>268</v>
       </c>
-      <c r="L20" t="s">
+      <c r="N20" t="s">
         <v>186</v>
       </c>
-      <c r="M20">
+      <c r="O20">
         <v>16</v>
       </c>
-      <c r="N20">
+      <c r="P20">
         <v>320</v>
       </c>
-      <c r="O20" t="s">
+      <c r="Q20" t="s">
         <v>278</v>
       </c>
-      <c r="P20" t="s">
+      <c r="R20" t="s">
         <v>288</v>
       </c>
-      <c r="Q20">
+      <c r="S20">
         <v>999.91</v>
       </c>
-      <c r="R20">
+      <c r="T20">
         <v>356.87</v>
       </c>
-      <c r="S20">
+      <c r="U20">
         <v>3087</v>
       </c>
-      <c r="T20">
+      <c r="V20">
         <v>119</v>
       </c>
-      <c r="V20">
+      <c r="X20">
         <v>1646</v>
       </c>
-      <c r="W20">
+      <c r="Y20">
         <v>1684</v>
       </c>
-      <c r="X20">
+      <c r="Z20">
         <v>1694</v>
       </c>
-      <c r="Y20">
+      <c r="AA20">
         <v>904721</v>
       </c>
-      <c r="Z20">
-        <v>0</v>
-      </c>
-      <c r="AA20" s="7">
+      <c r="AB20">
+        <v>0</v>
+      </c>
+      <c r="AC20" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB20" s="1" t="s">
+      <c r="AD20" s="1" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="21" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A21">
         <v>1</v>
       </c>
@@ -3040,62 +3194,68 @@
         <v>6</v>
       </c>
       <c r="J21">
+        <v>11</v>
+      </c>
+      <c r="K21" t="s">
+        <v>315</v>
+      </c>
+      <c r="L21">
         <v>4</v>
       </c>
-      <c r="K21" t="s">
+      <c r="M21" t="s">
         <v>268</v>
       </c>
-      <c r="L21" t="s">
+      <c r="N21" t="s">
         <v>186</v>
       </c>
-      <c r="M21">
+      <c r="O21">
         <v>16</v>
       </c>
-      <c r="N21">
+      <c r="P21">
         <v>320</v>
       </c>
-      <c r="O21" t="s">
+      <c r="Q21" t="s">
         <v>278</v>
       </c>
-      <c r="P21" t="s">
+      <c r="R21" t="s">
         <v>288</v>
       </c>
-      <c r="Q21">
+      <c r="S21">
         <v>993.99</v>
       </c>
-      <c r="R21">
+      <c r="T21">
         <v>587.75</v>
       </c>
-      <c r="S21">
+      <c r="U21">
         <v>4946</v>
       </c>
-      <c r="T21">
+      <c r="V21">
         <v>25</v>
       </c>
-      <c r="V21">
+      <c r="X21">
         <v>2142</v>
       </c>
-      <c r="W21">
+      <c r="Y21">
         <v>2201</v>
       </c>
-      <c r="X21">
+      <c r="Z21">
         <v>4159</v>
       </c>
-      <c r="Y21">
+      <c r="AA21">
         <v>902995</v>
       </c>
-      <c r="Z21">
-        <v>0</v>
-      </c>
-      <c r="AA21" s="7">
+      <c r="AB21">
+        <v>0</v>
+      </c>
+      <c r="AC21" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB21" s="1" t="s">
+      <c r="AD21" s="1" t="s">
         <v>287</v>
       </c>
     </row>
-    <row r="22" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A22">
         <v>1</v>
       </c>
@@ -3124,62 +3284,68 @@
         <v>6</v>
       </c>
       <c r="J22">
+        <v>11</v>
+      </c>
+      <c r="K22" t="s">
+        <v>315</v>
+      </c>
+      <c r="L22">
         <v>4</v>
       </c>
-      <c r="K22" t="s">
+      <c r="M22" t="s">
         <v>268</v>
       </c>
-      <c r="L22" t="s">
+      <c r="N22" t="s">
         <v>186</v>
       </c>
-      <c r="M22">
+      <c r="O22">
         <v>16</v>
       </c>
-      <c r="N22">
+      <c r="P22">
         <v>320</v>
       </c>
-      <c r="O22" t="s">
+      <c r="Q22" t="s">
         <v>278</v>
       </c>
-      <c r="P22" t="s">
+      <c r="R22" t="s">
         <v>288</v>
       </c>
-      <c r="Q22">
+      <c r="S22">
         <v>981.93</v>
       </c>
-      <c r="R22">
+      <c r="T22">
         <v>1209.79</v>
       </c>
-      <c r="S22">
+      <c r="U22">
         <v>9932</v>
       </c>
-      <c r="T22">
-        <v>35</v>
-      </c>
       <c r="V22">
+        <v>35</v>
+      </c>
+      <c r="X22">
         <v>5715</v>
       </c>
-      <c r="W22">
+      <c r="Y22">
         <v>5785</v>
       </c>
-      <c r="X22">
+      <c r="Z22">
         <v>5791</v>
       </c>
-      <c r="Y22">
+      <c r="AA22">
         <v>906691</v>
       </c>
-      <c r="Z22">
-        <v>0</v>
-      </c>
-      <c r="AA22" s="7">
+      <c r="AB22">
+        <v>0</v>
+      </c>
+      <c r="AC22" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB22" s="1" t="s">
+      <c r="AD22" s="1" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="23" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A23">
         <v>1</v>
       </c>
@@ -3208,62 +3374,68 @@
         <v>6</v>
       </c>
       <c r="J23">
+        <v>11</v>
+      </c>
+      <c r="K23" t="s">
+        <v>315</v>
+      </c>
+      <c r="L23">
         <v>4</v>
       </c>
-      <c r="K23" t="s">
+      <c r="M23" t="s">
         <v>268</v>
       </c>
-      <c r="L23" t="s">
+      <c r="N23" t="s">
         <v>186</v>
       </c>
-      <c r="M23">
+      <c r="O23">
         <v>16</v>
       </c>
-      <c r="N23">
+      <c r="P23">
         <v>320</v>
       </c>
-      <c r="O23" t="s">
+      <c r="Q23" t="s">
         <v>278</v>
       </c>
-      <c r="P23" t="s">
+      <c r="R23" t="s">
         <v>289</v>
       </c>
-      <c r="Q23">
+      <c r="S23">
         <v>978.51</v>
       </c>
-      <c r="R23">
+      <c r="T23">
         <v>269</v>
       </c>
-      <c r="S23">
+      <c r="U23">
         <v>11717</v>
       </c>
-      <c r="T23">
-        <v>36</v>
-      </c>
       <c r="V23">
+        <v>36</v>
+      </c>
+      <c r="X23">
         <v>466</v>
       </c>
-      <c r="W23">
+      <c r="Y23">
         <v>3382</v>
       </c>
-      <c r="X23">
+      <c r="Z23">
         <v>5100</v>
       </c>
-      <c r="Y23">
+      <c r="AA23">
         <v>925197</v>
       </c>
-      <c r="Z23">
-        <v>0</v>
-      </c>
-      <c r="AA23" s="7">
+      <c r="AB23">
+        <v>0</v>
+      </c>
+      <c r="AC23" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB23" s="1" t="s">
+      <c r="AD23" s="1" t="s">
         <v>291</v>
       </c>
     </row>
-    <row r="24" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A24">
         <v>1</v>
       </c>
@@ -3292,62 +3464,68 @@
         <v>6</v>
       </c>
       <c r="J24">
+        <v>11</v>
+      </c>
+      <c r="K24" t="s">
+        <v>315</v>
+      </c>
+      <c r="L24">
         <v>4</v>
       </c>
-      <c r="K24" t="s">
+      <c r="M24" t="s">
         <v>268</v>
       </c>
-      <c r="L24" t="s">
+      <c r="N24" t="s">
         <v>186</v>
       </c>
-      <c r="M24">
+      <c r="O24">
         <v>16</v>
       </c>
-      <c r="N24">
+      <c r="P24">
         <v>320</v>
       </c>
-      <c r="O24" t="s">
+      <c r="Q24" t="s">
         <v>278</v>
       </c>
-      <c r="P24" t="s">
+      <c r="R24" t="s">
         <v>289</v>
       </c>
-      <c r="Q24">
+      <c r="S24">
         <v>983.68</v>
       </c>
-      <c r="R24">
+      <c r="T24">
         <v>394.29</v>
       </c>
-      <c r="S24">
+      <c r="U24">
         <v>12917</v>
       </c>
-      <c r="T24">
+      <c r="V24">
         <v>626</v>
       </c>
-      <c r="V24">
+      <c r="X24">
         <v>1441.99</v>
       </c>
-      <c r="W24">
+      <c r="Y24">
         <v>1841</v>
       </c>
-      <c r="X24">
+      <c r="Z24">
         <v>2288</v>
       </c>
-      <c r="Y24">
+      <c r="AA24">
         <v>913854</v>
       </c>
-      <c r="Z24">
-        <v>0</v>
-      </c>
-      <c r="AA24" s="7">
+      <c r="AB24">
+        <v>0</v>
+      </c>
+      <c r="AC24" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB24" s="1" t="s">
+      <c r="AD24" s="1" t="s">
         <v>290</v>
       </c>
     </row>
-    <row r="25" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A25">
         <v>1</v>
       </c>
@@ -3376,62 +3554,68 @@
         <v>6</v>
       </c>
       <c r="J25">
+        <v>11</v>
+      </c>
+      <c r="K25" t="s">
+        <v>315</v>
+      </c>
+      <c r="L25">
         <v>4</v>
       </c>
-      <c r="K25" t="s">
+      <c r="M25" t="s">
         <v>268</v>
       </c>
-      <c r="L25" t="s">
+      <c r="N25" t="s">
         <v>186</v>
       </c>
-      <c r="M25">
+      <c r="O25">
         <v>16</v>
       </c>
-      <c r="N25">
+      <c r="P25">
         <v>320</v>
       </c>
-      <c r="O25" t="s">
+      <c r="Q25" t="s">
         <v>278</v>
       </c>
-      <c r="P25" t="s">
+      <c r="R25" t="s">
         <v>289</v>
       </c>
-      <c r="Q25">
+      <c r="S25">
         <v>991.55</v>
       </c>
-      <c r="R25">
+      <c r="T25">
         <v>233.41</v>
       </c>
-      <c r="S25">
+      <c r="U25">
         <v>6544</v>
       </c>
-      <c r="T25">
+      <c r="V25">
         <v>20</v>
       </c>
-      <c r="V25">
+      <c r="X25">
         <v>165.99</v>
       </c>
-      <c r="W25">
+      <c r="Y25">
         <v>859</v>
       </c>
-      <c r="X25">
+      <c r="Z25">
         <v>861</v>
       </c>
-      <c r="Y25">
+      <c r="AA25">
         <v>907183</v>
       </c>
-      <c r="Z25">
-        <v>0</v>
-      </c>
-      <c r="AA25" s="7">
+      <c r="AB25">
+        <v>0</v>
+      </c>
+      <c r="AC25" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB25" s="1" t="s">
+      <c r="AD25" s="1" t="s">
         <v>292</v>
       </c>
     </row>
-    <row r="26" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A26">
         <v>1</v>
       </c>
@@ -3460,62 +3644,68 @@
         <v>6</v>
       </c>
       <c r="J26">
+        <v>11</v>
+      </c>
+      <c r="K26" t="s">
+        <v>315</v>
+      </c>
+      <c r="L26">
         <v>4</v>
       </c>
-      <c r="K26" t="s">
+      <c r="M26" t="s">
         <v>268</v>
       </c>
-      <c r="L26" t="s">
+      <c r="N26" t="s">
         <v>186</v>
       </c>
-      <c r="M26">
+      <c r="O26">
         <v>16</v>
       </c>
-      <c r="N26">
+      <c r="P26">
         <v>320</v>
       </c>
-      <c r="O26" t="s">
+      <c r="Q26" t="s">
         <v>278</v>
       </c>
-      <c r="P26" t="s">
+      <c r="R26" t="s">
         <v>289</v>
       </c>
-      <c r="Q26">
+      <c r="S26">
         <v>989.15</v>
       </c>
-      <c r="R26">
+      <c r="T26">
         <v>208.7</v>
       </c>
-      <c r="S26">
+      <c r="U26">
         <v>9825</v>
       </c>
-      <c r="T26">
+      <c r="V26">
         <v>287</v>
       </c>
-      <c r="V26">
+      <c r="X26">
         <v>803</v>
       </c>
-      <c r="W26">
+      <c r="Y26">
         <v>823</v>
       </c>
-      <c r="X26">
+      <c r="Z26">
         <v>827</v>
       </c>
-      <c r="Y26">
+      <c r="AA26">
         <v>899870</v>
       </c>
-      <c r="Z26">
-        <v>0</v>
-      </c>
-      <c r="AA26" s="7">
+      <c r="AB26">
+        <v>0</v>
+      </c>
+      <c r="AC26" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB26" s="1" t="s">
+      <c r="AD26" s="1" t="s">
         <v>296</v>
       </c>
     </row>
-    <row r="27" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A27">
         <v>1</v>
       </c>
@@ -3544,62 +3734,68 @@
         <v>6</v>
       </c>
       <c r="J27">
+        <v>11</v>
+      </c>
+      <c r="K27" t="s">
+        <v>315</v>
+      </c>
+      <c r="L27">
         <v>4</v>
       </c>
-      <c r="K27" t="s">
+      <c r="M27" t="s">
         <v>268</v>
       </c>
-      <c r="L27" t="s">
+      <c r="N27" t="s">
         <v>186</v>
       </c>
-      <c r="M27">
+      <c r="O27">
         <v>16</v>
       </c>
-      <c r="N27">
+      <c r="P27">
         <v>320</v>
       </c>
-      <c r="O27" t="s">
+      <c r="Q27" t="s">
         <v>278</v>
       </c>
-      <c r="P27" t="s">
+      <c r="R27" t="s">
         <v>289</v>
       </c>
-      <c r="Q27">
+      <c r="S27">
         <v>988.79</v>
       </c>
-      <c r="R27">
+      <c r="T27">
         <v>87.64</v>
       </c>
-      <c r="S27">
+      <c r="U27">
         <v>8668</v>
       </c>
-      <c r="T27">
+      <c r="V27">
         <v>24</v>
       </c>
-      <c r="V27">
+      <c r="X27">
         <v>424</v>
       </c>
-      <c r="W27">
+      <c r="Y27">
         <v>467</v>
       </c>
-      <c r="X27">
+      <c r="Z27">
         <v>479</v>
       </c>
-      <c r="Y27">
+      <c r="AA27">
         <v>901191</v>
       </c>
-      <c r="Z27">
-        <v>0</v>
-      </c>
-      <c r="AA27" s="7">
+      <c r="AB27">
+        <v>0</v>
+      </c>
+      <c r="AC27" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB27" s="1" t="s">
+      <c r="AD27" s="1" t="s">
         <v>293</v>
       </c>
     </row>
-    <row r="28" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A28">
         <v>1</v>
       </c>
@@ -3628,62 +3824,68 @@
         <v>6</v>
       </c>
       <c r="J28">
+        <v>11</v>
+      </c>
+      <c r="K28" t="s">
+        <v>315</v>
+      </c>
+      <c r="L28">
         <v>4</v>
       </c>
-      <c r="K28" t="s">
+      <c r="M28" t="s">
         <v>268</v>
       </c>
-      <c r="L28" t="s">
+      <c r="N28" t="s">
         <v>186</v>
       </c>
-      <c r="M28">
+      <c r="O28">
         <v>16</v>
       </c>
-      <c r="N28">
+      <c r="P28">
         <v>320</v>
       </c>
-      <c r="O28" t="s">
+      <c r="Q28" t="s">
         <v>278</v>
       </c>
-      <c r="P28" t="s">
+      <c r="R28" t="s">
         <v>289</v>
       </c>
-      <c r="Q28">
+      <c r="S28">
         <v>986.07</v>
       </c>
-      <c r="R28">
+      <c r="T28">
         <v>43.57</v>
       </c>
-      <c r="S28">
+      <c r="U28">
         <v>10390</v>
       </c>
-      <c r="T28">
+      <c r="V28">
         <v>20</v>
       </c>
-      <c r="V28">
+      <c r="X28">
         <v>199.99</v>
       </c>
-      <c r="W28">
+      <c r="Y28">
         <v>218</v>
       </c>
-      <c r="X28">
+      <c r="Z28">
         <v>226</v>
       </c>
-      <c r="Y28">
+      <c r="AA28">
         <v>895335</v>
       </c>
-      <c r="Z28">
-        <v>0</v>
-      </c>
-      <c r="AA28" s="7">
+      <c r="AB28">
+        <v>0</v>
+      </c>
+      <c r="AC28" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB28" s="1" t="s">
+      <c r="AD28" s="1" t="s">
         <v>294</v>
       </c>
     </row>
-    <row r="29" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A29">
         <v>1</v>
       </c>
@@ -3712,62 +3914,68 @@
         <v>6</v>
       </c>
       <c r="J29">
+        <v>11</v>
+      </c>
+      <c r="K29" t="s">
+        <v>315</v>
+      </c>
+      <c r="L29">
         <v>4</v>
       </c>
-      <c r="K29" t="s">
+      <c r="M29" t="s">
         <v>268</v>
       </c>
-      <c r="L29" t="s">
+      <c r="N29" t="s">
         <v>186</v>
       </c>
-      <c r="M29">
+      <c r="O29">
         <v>16</v>
       </c>
-      <c r="N29">
+      <c r="P29">
         <v>320</v>
       </c>
-      <c r="O29" t="s">
+      <c r="Q29" t="s">
         <v>278</v>
       </c>
-      <c r="P29" t="s">
+      <c r="R29" t="s">
         <v>289</v>
       </c>
-      <c r="Q29">
+      <c r="S29">
         <v>988.94</v>
       </c>
-      <c r="R29">
+      <c r="T29">
         <v>26.12</v>
       </c>
-      <c r="S29">
+      <c r="U29">
         <v>7961</v>
       </c>
-      <c r="T29">
+      <c r="V29">
         <v>20</v>
       </c>
-      <c r="V29">
+      <c r="X29">
         <v>122</v>
       </c>
-      <c r="W29">
+      <c r="Y29">
         <v>151</v>
       </c>
-      <c r="X29">
+      <c r="Z29">
         <v>156</v>
       </c>
-      <c r="Y29">
+      <c r="AA29">
         <v>890172</v>
       </c>
-      <c r="Z29">
-        <v>0</v>
-      </c>
-      <c r="AA29" s="7">
+      <c r="AB29">
+        <v>0</v>
+      </c>
+      <c r="AC29" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB29" s="1" t="s">
+      <c r="AD29" s="1" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="30" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A30">
         <v>1</v>
       </c>
@@ -3796,62 +4004,68 @@
         <v>6</v>
       </c>
       <c r="J30">
+        <v>11</v>
+      </c>
+      <c r="K30" t="s">
+        <v>315</v>
+      </c>
+      <c r="L30">
         <v>4</v>
       </c>
-      <c r="K30" t="s">
+      <c r="M30" t="s">
         <v>268</v>
       </c>
-      <c r="L30" t="s">
+      <c r="N30" t="s">
         <v>186</v>
       </c>
-      <c r="M30">
+      <c r="O30">
         <v>16</v>
       </c>
-      <c r="N30">
+      <c r="P30">
         <v>320</v>
       </c>
-      <c r="O30" t="s">
+      <c r="Q30" t="s">
         <v>278</v>
       </c>
-      <c r="P30" t="s">
+      <c r="R30" t="s">
         <v>298</v>
       </c>
-      <c r="Q30">
+      <c r="S30">
         <v>2766.4</v>
       </c>
-      <c r="R30">
+      <c r="T30">
         <v>107.69</v>
       </c>
-      <c r="S30">
+      <c r="U30">
         <v>1707</v>
       </c>
-      <c r="T30">
+      <c r="V30">
         <v>47</v>
       </c>
-      <c r="V30">
+      <c r="X30">
         <v>162</v>
       </c>
-      <c r="W30">
+      <c r="Y30">
         <v>174</v>
       </c>
-      <c r="X30">
+      <c r="Z30">
         <v>287</v>
       </c>
-      <c r="Y30">
+      <c r="AA30">
         <v>2499413</v>
       </c>
-      <c r="Z30">
-        <v>0</v>
-      </c>
-      <c r="AA30" s="7">
+      <c r="AB30">
+        <v>0</v>
+      </c>
+      <c r="AC30" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB30" s="1" t="s">
+      <c r="AD30" s="1" t="s">
         <v>299</v>
       </c>
     </row>
-    <row r="31" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A31">
         <v>1</v>
       </c>
@@ -3880,62 +4094,68 @@
         <v>6</v>
       </c>
       <c r="J31">
+        <v>11</v>
+      </c>
+      <c r="K31" t="s">
+        <v>315</v>
+      </c>
+      <c r="L31">
         <v>4</v>
       </c>
-      <c r="K31" t="s">
+      <c r="M31" t="s">
         <v>268</v>
       </c>
-      <c r="L31" t="s">
+      <c r="N31" t="s">
         <v>186</v>
       </c>
-      <c r="M31">
+      <c r="O31">
         <v>16</v>
       </c>
-      <c r="N31">
+      <c r="P31">
         <v>320</v>
       </c>
-      <c r="O31" t="s">
+      <c r="Q31" t="s">
         <v>278</v>
       </c>
-      <c r="P31" t="s">
+      <c r="R31" t="s">
         <v>298</v>
       </c>
-      <c r="Q31">
+      <c r="S31">
         <v>2762.97</v>
       </c>
-      <c r="R31">
+      <c r="T31">
         <v>214.31</v>
       </c>
-      <c r="S31">
+      <c r="U31">
         <v>1301</v>
       </c>
-      <c r="T31">
+      <c r="V31">
         <v>92</v>
       </c>
-      <c r="V31">
+      <c r="X31">
         <v>177.99</v>
       </c>
-      <c r="W31">
+      <c r="Y31">
         <v>194</v>
       </c>
-      <c r="X31">
+      <c r="Z31">
         <v>199</v>
       </c>
-      <c r="Y31">
+      <c r="AA31">
         <v>2514537</v>
       </c>
-      <c r="Z31">
-        <v>0</v>
-      </c>
-      <c r="AA31" s="7">
+      <c r="AB31">
+        <v>0</v>
+      </c>
+      <c r="AC31" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB31" s="1" t="s">
+      <c r="AD31" s="1" t="s">
         <v>300</v>
       </c>
     </row>
-    <row r="32" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:30" hidden="1" x14ac:dyDescent="0.2">
       <c r="A32">
         <v>1</v>
       </c>
@@ -3964,62 +4184,68 @@
         <v>6</v>
       </c>
       <c r="J32">
+        <v>11</v>
+      </c>
+      <c r="K32" t="s">
+        <v>315</v>
+      </c>
+      <c r="L32">
         <v>4</v>
       </c>
-      <c r="K32" t="s">
+      <c r="M32" t="s">
         <v>268</v>
       </c>
-      <c r="L32" t="s">
+      <c r="N32" t="s">
         <v>186</v>
       </c>
-      <c r="M32">
+      <c r="O32">
         <v>16</v>
       </c>
-      <c r="N32">
+      <c r="P32">
         <v>320</v>
       </c>
-      <c r="O32" t="s">
+      <c r="Q32" t="s">
         <v>278</v>
       </c>
-      <c r="P32" t="s">
+      <c r="R32" t="s">
         <v>298</v>
       </c>
-      <c r="Q32">
+      <c r="S32">
         <v>2481.89</v>
       </c>
-      <c r="R32">
+      <c r="T32">
         <v>396.67</v>
       </c>
-      <c r="S32">
+      <c r="U32">
         <v>18637</v>
       </c>
-      <c r="T32">
+      <c r="V32">
         <v>172</v>
       </c>
-      <c r="V32">
+      <c r="X32">
         <v>530</v>
       </c>
-      <c r="W32">
+      <c r="Y32">
         <v>549</v>
       </c>
-      <c r="X32">
+      <c r="Z32">
         <v>560</v>
       </c>
-      <c r="Y32">
+      <c r="AA32">
         <v>2266488</v>
       </c>
-      <c r="Z32">
-        <v>0</v>
-      </c>
-      <c r="AA32" s="7">
+      <c r="AB32">
+        <v>0</v>
+      </c>
+      <c r="AC32" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB32" s="1" t="s">
+      <c r="AD32" s="1" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="33" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A33">
         <v>1</v>
       </c>
@@ -4048,65 +4274,71 @@
         <v>6</v>
       </c>
       <c r="J33">
+        <v>11</v>
+      </c>
+      <c r="K33" t="s">
+        <v>315</v>
+      </c>
+      <c r="L33">
         <v>4</v>
       </c>
-      <c r="K33" t="s">
+      <c r="M33" t="s">
         <v>268</v>
       </c>
-      <c r="L33" t="s">
+      <c r="N33" t="s">
         <v>186</v>
       </c>
-      <c r="M33">
+      <c r="O33">
         <v>16</v>
       </c>
-      <c r="N33">
+      <c r="P33">
         <v>320</v>
       </c>
-      <c r="O33" t="s">
+      <c r="Q33" t="s">
         <v>278</v>
       </c>
-      <c r="P33" t="s">
+      <c r="R33" t="s">
         <v>298</v>
       </c>
-      <c r="Q33">
+      <c r="S33">
         <v>2833.3</v>
       </c>
-      <c r="R33">
+      <c r="T33">
         <v>423.14</v>
       </c>
-      <c r="S33">
+      <c r="U33">
         <v>1495.75</v>
       </c>
-      <c r="T33">
+      <c r="V33">
         <v>416.71</v>
       </c>
-      <c r="V33">
+      <c r="X33">
         <v>535.92999999999995</v>
       </c>
-      <c r="W33">
+      <c r="Y33">
         <v>773.38</v>
       </c>
-      <c r="X33">
+      <c r="Z33">
         <v>850.45</v>
       </c>
-      <c r="Y33">
+      <c r="AA33">
         <v>2549970</v>
       </c>
-      <c r="Z33">
-        <v>0</v>
-      </c>
-      <c r="AA33" s="7">
+      <c r="AB33">
+        <v>0</v>
+      </c>
+      <c r="AC33" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB33" s="1" t="s">
+      <c r="AD33" s="1" t="s">
         <v>305</v>
       </c>
-      <c r="AC33" t="s">
+      <c r="AE33" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="34" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A34">
         <v>1</v>
       </c>
@@ -4135,65 +4367,71 @@
         <v>6</v>
       </c>
       <c r="J34">
+        <v>11</v>
+      </c>
+      <c r="K34" t="s">
+        <v>315</v>
+      </c>
+      <c r="L34">
         <v>4</v>
       </c>
-      <c r="K34" t="s">
+      <c r="M34" t="s">
         <v>268</v>
       </c>
-      <c r="L34" t="s">
+      <c r="N34" t="s">
         <v>186</v>
       </c>
-      <c r="M34">
+      <c r="O34">
         <v>16</v>
       </c>
-      <c r="N34">
+      <c r="P34">
         <v>320</v>
       </c>
-      <c r="O34" t="s">
+      <c r="Q34" t="s">
         <v>278</v>
       </c>
-      <c r="P34" t="s">
+      <c r="R34" t="s">
         <v>298</v>
       </c>
-      <c r="Q34">
+      <c r="S34">
         <v>2758.85</v>
       </c>
-      <c r="R34">
+      <c r="T34">
         <v>868.39</v>
       </c>
-      <c r="S34">
+      <c r="U34">
         <v>10996.44</v>
       </c>
-      <c r="T34">
+      <c r="V34">
         <v>846.49</v>
       </c>
-      <c r="V34">
+      <c r="X34">
         <v>1054.3800000000001</v>
       </c>
-      <c r="W34">
+      <c r="Y34">
         <v>2585.58</v>
       </c>
-      <c r="X34">
+      <c r="Z34">
         <v>10977.49</v>
       </c>
-      <c r="Y34">
+      <c r="AA34">
         <v>2482966</v>
       </c>
-      <c r="Z34">
-        <v>0</v>
-      </c>
-      <c r="AA34" s="7">
+      <c r="AB34">
+        <v>0</v>
+      </c>
+      <c r="AC34" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB34" s="1" t="s">
+      <c r="AD34" s="1" t="s">
         <v>306</v>
       </c>
-      <c r="AC34" t="s">
+      <c r="AE34" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="35" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A35">
         <v>1</v>
       </c>
@@ -4222,65 +4460,71 @@
         <v>6</v>
       </c>
       <c r="J35">
+        <v>11</v>
+      </c>
+      <c r="K35" t="s">
+        <v>315</v>
+      </c>
+      <c r="L35">
         <v>4</v>
       </c>
-      <c r="K35" t="s">
+      <c r="M35" t="s">
         <v>268</v>
       </c>
-      <c r="L35" t="s">
+      <c r="N35" t="s">
         <v>186</v>
       </c>
-      <c r="M35">
+      <c r="O35">
         <v>16</v>
       </c>
-      <c r="N35">
+      <c r="P35">
         <v>320</v>
       </c>
-      <c r="O35" t="s">
+      <c r="Q35" t="s">
         <v>278</v>
       </c>
-      <c r="P35" t="s">
+      <c r="R35" t="s">
         <v>298</v>
       </c>
-      <c r="Q35">
+      <c r="S35">
         <v>2785.19</v>
       </c>
-      <c r="R35">
+      <c r="T35">
         <v>1717.29</v>
       </c>
-      <c r="S35">
+      <c r="U35">
         <v>5277.52</v>
       </c>
-      <c r="T35">
+      <c r="V35">
         <v>1700.94</v>
       </c>
-      <c r="V35">
+      <c r="X35">
         <v>2042.76</v>
       </c>
-      <c r="W35">
+      <c r="Y35">
         <v>2380.39</v>
       </c>
-      <c r="X35">
+      <c r="Z35">
         <v>3535.87</v>
       </c>
-      <c r="Y35">
+      <c r="AA35">
         <v>2506675</v>
       </c>
-      <c r="Z35">
-        <v>0</v>
-      </c>
-      <c r="AA35" s="7">
+      <c r="AB35">
+        <v>0</v>
+      </c>
+      <c r="AC35" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB35" s="1" t="s">
+      <c r="AD35" s="1" t="s">
         <v>307</v>
       </c>
-      <c r="AC35" t="s">
+      <c r="AE35" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="36" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A36">
         <v>1</v>
       </c>
@@ -4309,65 +4553,71 @@
         <v>6</v>
       </c>
       <c r="J36">
+        <v>11</v>
+      </c>
+      <c r="K36" t="s">
+        <v>315</v>
+      </c>
+      <c r="L36">
         <v>4</v>
       </c>
-      <c r="K36" t="s">
+      <c r="M36" t="s">
         <v>268</v>
       </c>
-      <c r="L36" t="s">
+      <c r="N36" t="s">
         <v>186</v>
       </c>
-      <c r="M36">
+      <c r="O36">
         <v>16</v>
       </c>
-      <c r="N36">
+      <c r="P36">
         <v>320</v>
       </c>
-      <c r="O36" t="s">
+      <c r="Q36" t="s">
         <v>278</v>
       </c>
-      <c r="P36" t="s">
+      <c r="R36" t="s">
         <v>298</v>
       </c>
-      <c r="Q36">
+      <c r="S36">
         <v>2777.95</v>
       </c>
-      <c r="R36">
+      <c r="T36">
         <v>3432.6</v>
       </c>
-      <c r="S36">
+      <c r="U36">
         <v>7428.99</v>
       </c>
-      <c r="T36">
+      <c r="V36">
         <v>3402.41</v>
       </c>
-      <c r="V36">
+      <c r="X36">
         <v>3984.68</v>
       </c>
-      <c r="W36">
+      <c r="Y36">
         <v>4255.13</v>
       </c>
-      <c r="X36">
+      <c r="Z36">
         <v>7068.19</v>
       </c>
-      <c r="Y36">
+      <c r="AA36">
         <v>2500154</v>
       </c>
-      <c r="Z36">
-        <v>0</v>
-      </c>
-      <c r="AA36" s="7">
+      <c r="AB36">
+        <v>0</v>
+      </c>
+      <c r="AC36" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB36" s="1" t="s">
+      <c r="AD36" s="1" t="s">
         <v>308</v>
       </c>
-      <c r="AC36" t="s">
+      <c r="AE36" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="37" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A37">
         <v>1</v>
       </c>
@@ -4396,65 +4646,71 @@
         <v>6</v>
       </c>
       <c r="J37">
+        <v>11</v>
+      </c>
+      <c r="K37" t="s">
+        <v>315</v>
+      </c>
+      <c r="L37">
         <v>4</v>
       </c>
-      <c r="K37" t="s">
+      <c r="M37" t="s">
         <v>268</v>
       </c>
-      <c r="L37" t="s">
+      <c r="N37" t="s">
         <v>186</v>
       </c>
-      <c r="M37">
+      <c r="O37">
         <v>16</v>
       </c>
-      <c r="N37">
+      <c r="P37">
         <v>320</v>
       </c>
-      <c r="O37" t="s">
+      <c r="Q37" t="s">
         <v>278</v>
       </c>
-      <c r="P37" t="s">
+      <c r="R37" t="s">
         <v>298</v>
       </c>
-      <c r="Q37">
+      <c r="S37">
         <v>2740.49</v>
       </c>
-      <c r="R37">
+      <c r="T37">
         <v>6907.07</v>
       </c>
-      <c r="S37">
+      <c r="U37">
         <v>20530.78</v>
       </c>
-      <c r="T37">
+      <c r="V37">
         <v>6905.32</v>
       </c>
-      <c r="V37">
+      <c r="X37">
         <v>7718.24</v>
       </c>
-      <c r="W37">
+      <c r="Y37">
         <v>8366.3700000000008</v>
       </c>
-      <c r="X37">
+      <c r="Z37">
         <v>10219.85</v>
       </c>
-      <c r="Y37">
+      <c r="AA37">
         <v>2466438</v>
       </c>
-      <c r="Z37">
-        <v>0</v>
-      </c>
-      <c r="AA37" s="7">
+      <c r="AB37">
+        <v>0</v>
+      </c>
+      <c r="AC37" s="7">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="AB37" s="1" t="s">
+      <c r="AD37" s="1" t="s">
         <v>309</v>
       </c>
-      <c r="AC37" t="s">
+      <c r="AE37" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="38" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A38">
         <v>1</v>
       </c>
@@ -4483,65 +4739,71 @@
         <v>10</v>
       </c>
       <c r="J38">
+        <v>11</v>
+      </c>
+      <c r="K38" t="s">
+        <v>315</v>
+      </c>
+      <c r="L38">
         <v>4</v>
       </c>
-      <c r="K38" t="s">
+      <c r="M38" t="s">
         <v>268</v>
       </c>
-      <c r="L38" t="s">
+      <c r="N38" t="s">
         <v>186</v>
       </c>
-      <c r="M38">
+      <c r="O38">
         <v>16</v>
       </c>
-      <c r="N38">
+      <c r="P38">
         <v>320</v>
       </c>
-      <c r="O38" t="s">
+      <c r="Q38" t="s">
         <v>278</v>
       </c>
-      <c r="P38" t="s">
+      <c r="R38" t="s">
         <v>298</v>
       </c>
-      <c r="Q38">
+      <c r="S38">
         <v>2493.92</v>
       </c>
-      <c r="R38">
+      <c r="T38">
         <v>3822.88</v>
       </c>
-      <c r="S38">
+      <c r="U38">
         <v>7328.76</v>
       </c>
-      <c r="T38">
+      <c r="V38">
         <v>3818.39</v>
       </c>
-      <c r="V38">
+      <c r="X38">
         <v>4271.87</v>
       </c>
-      <c r="W38">
+      <c r="Y38">
         <v>4458.07</v>
       </c>
-      <c r="X38">
+      <c r="Z38">
         <v>5492.43</v>
       </c>
-      <c r="Y38">
+      <c r="AA38">
         <v>2244524</v>
       </c>
-      <c r="Z38">
-        <v>0</v>
-      </c>
-      <c r="AA38" s="7">
-        <f t="shared" ref="AA38:AA40" si="1">Z38/Y38</f>
-        <v>0</v>
-      </c>
-      <c r="AB38" s="1" t="s">
+      <c r="AB38">
+        <v>0</v>
+      </c>
+      <c r="AC38" s="7">
+        <f t="shared" ref="AC38:AC47" si="1">AB38/AA38</f>
+        <v>0</v>
+      </c>
+      <c r="AD38" s="1" t="s">
         <v>304</v>
       </c>
-      <c r="AC38" t="s">
+      <c r="AE38" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="39" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
       <c r="A39">
         <v>1</v>
       </c>
@@ -4570,65 +4832,71 @@
         <v>6</v>
       </c>
       <c r="J39">
+        <v>11</v>
+      </c>
+      <c r="K39" t="s">
+        <v>315</v>
+      </c>
+      <c r="L39">
         <v>4</v>
       </c>
-      <c r="K39" t="s">
+      <c r="M39" t="s">
         <v>268</v>
       </c>
-      <c r="L39" t="s">
+      <c r="N39" t="s">
         <v>186</v>
       </c>
-      <c r="M39">
+      <c r="O39">
         <v>16</v>
       </c>
-      <c r="N39">
+      <c r="P39">
         <v>320</v>
       </c>
-      <c r="O39" t="s">
+      <c r="Q39" t="s">
         <v>278</v>
       </c>
-      <c r="P39" t="s">
+      <c r="R39" t="s">
         <v>298</v>
       </c>
-      <c r="Q39">
+      <c r="S39">
         <v>2748.75</v>
       </c>
-      <c r="R39">
+      <c r="T39">
         <v>3469.27</v>
       </c>
-      <c r="S39">
+      <c r="U39">
         <v>5024.18</v>
       </c>
-      <c r="T39">
+      <c r="V39">
         <v>3469.75</v>
       </c>
-      <c r="V39">
+      <c r="X39">
         <v>3840.38</v>
       </c>
-      <c r="W39">
+      <c r="Y39">
         <v>3913.95</v>
       </c>
-      <c r="X39">
+      <c r="Z39">
         <v>3983.14</v>
       </c>
-      <c r="Y39">
+      <c r="AA39">
         <v>2473874</v>
       </c>
-      <c r="Z39">
-        <v>0</v>
-      </c>
-      <c r="AA39" s="7">
+      <c r="AB39">
+        <v>0</v>
+      </c>
+      <c r="AC39" s="7">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB39" s="1" t="s">
+      <c r="AD39" s="1" t="s">
         <v>310</v>
       </c>
-      <c r="AC39" t="s">
+      <c r="AE39" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="40" spans="1:29" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:31" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40">
         <v>1</v>
       </c>
@@ -4657,99 +4925,710 @@
         <v>6</v>
       </c>
       <c r="J40">
+        <v>11</v>
+      </c>
+      <c r="K40" t="s">
+        <v>315</v>
+      </c>
+      <c r="L40">
         <v>4</v>
       </c>
-      <c r="K40" t="s">
+      <c r="M40" t="s">
         <v>268</v>
       </c>
-      <c r="L40" t="s">
+      <c r="N40" t="s">
         <v>186</v>
       </c>
-      <c r="M40">
+      <c r="O40">
         <v>16</v>
       </c>
-      <c r="N40">
+      <c r="P40">
         <v>320</v>
       </c>
-      <c r="O40" t="s">
+      <c r="Q40" t="s">
         <v>278</v>
       </c>
-      <c r="P40" t="s">
+      <c r="R40" t="s">
         <v>289</v>
       </c>
-      <c r="Q40">
+      <c r="S40">
         <v>987.13</v>
       </c>
-      <c r="R40">
+      <c r="T40">
         <v>433.48</v>
       </c>
-      <c r="S40">
+      <c r="U40">
         <v>12635</v>
       </c>
-      <c r="T40">
+      <c r="V40">
         <v>503</v>
       </c>
-      <c r="V40">
+      <c r="X40">
         <v>2263</v>
       </c>
-      <c r="W40">
+      <c r="Y40">
         <v>3052</v>
       </c>
-      <c r="X40">
+      <c r="Z40">
         <v>3213</v>
       </c>
-      <c r="Y40">
+      <c r="AA40">
         <v>913639</v>
       </c>
-      <c r="Z40">
-        <v>0</v>
-      </c>
-      <c r="AA40" s="9">
+      <c r="AB40">
+        <v>0</v>
+      </c>
+      <c r="AC40" s="9">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="AB40" s="1" t="s">
+      <c r="AD40" s="1" t="s">
         <v>311</v>
       </c>
     </row>
-    <row r="41" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AA41" s="5"/>
-      <c r="AB41" s="1"/>
-    </row>
-    <row r="42" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AA42" s="5"/>
-      <c r="AB42" s="1"/>
-    </row>
-    <row r="43" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AA43" s="5"/>
-      <c r="AB43" s="1"/>
-    </row>
-    <row r="44" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AA44" s="5"/>
-      <c r="AB44" s="1"/>
-    </row>
-    <row r="45" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AA45" s="5"/>
-      <c r="AB45" s="1"/>
-      <c r="AC45" s="6"/>
-    </row>
-    <row r="46" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AA46" s="5"/>
-      <c r="AB46" s="1"/>
-    </row>
-    <row r="47" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AA47" s="5"/>
-      <c r="AB47" s="1"/>
-    </row>
-    <row r="48" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="AA48" s="5"/>
-      <c r="AB48" s="1"/>
-    </row>
-    <row r="49" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="AA49" s="5"/>
-      <c r="AB49" s="1"/>
-    </row>
-    <row r="50" spans="1:28" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A41">
+        <v>1</v>
+      </c>
+      <c r="B41">
+        <v>3</v>
+      </c>
+      <c r="C41" t="s">
+        <v>173</v>
+      </c>
+      <c r="D41">
+        <v>9600</v>
+      </c>
+      <c r="E41">
+        <v>600</v>
+      </c>
+      <c r="F41" t="s">
+        <v>211</v>
+      </c>
+      <c r="G41">
+        <v>1</v>
+      </c>
+      <c r="H41">
+        <v>4</v>
+      </c>
+      <c r="I41">
+        <v>6</v>
+      </c>
+      <c r="J41">
+        <v>11</v>
+      </c>
+      <c r="K41" t="s">
+        <v>317</v>
+      </c>
+      <c r="L41">
+        <v>4</v>
+      </c>
+      <c r="M41" t="s">
+        <v>268</v>
+      </c>
+      <c r="N41" t="s">
+        <v>186</v>
+      </c>
+      <c r="O41">
+        <v>16</v>
+      </c>
+      <c r="P41">
+        <v>320</v>
+      </c>
+      <c r="Q41" t="s">
+        <v>278</v>
+      </c>
+      <c r="R41" t="s">
+        <v>289</v>
+      </c>
+      <c r="S41">
+        <v>988.64</v>
+      </c>
+      <c r="T41">
+        <v>495.05</v>
+      </c>
+      <c r="U41">
+        <v>12512</v>
+      </c>
+      <c r="V41">
+        <v>21</v>
+      </c>
+      <c r="X41">
+        <v>225</v>
+      </c>
+      <c r="Y41">
+        <v>1119.9000000000001</v>
+      </c>
+      <c r="Z41">
+        <v>1211</v>
+      </c>
+      <c r="AA41">
+        <v>914779</v>
+      </c>
+      <c r="AB41">
+        <v>0</v>
+      </c>
+      <c r="AC41" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD41" s="1" t="s">
+        <v>316</v>
+      </c>
+    </row>
+    <row r="42" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A42">
+        <v>1</v>
+      </c>
+      <c r="B42">
+        <v>3</v>
+      </c>
+      <c r="C42" t="s">
+        <v>173</v>
+      </c>
+      <c r="D42">
+        <v>9600</v>
+      </c>
+      <c r="E42">
+        <v>600</v>
+      </c>
+      <c r="F42" t="s">
+        <v>211</v>
+      </c>
+      <c r="G42">
+        <v>1</v>
+      </c>
+      <c r="H42">
+        <v>4</v>
+      </c>
+      <c r="I42">
+        <v>6</v>
+      </c>
+      <c r="J42">
+        <v>17</v>
+      </c>
+      <c r="K42" t="s">
+        <v>317</v>
+      </c>
+      <c r="L42">
+        <v>4</v>
+      </c>
+      <c r="M42" t="s">
+        <v>268</v>
+      </c>
+      <c r="N42" t="s">
+        <v>186</v>
+      </c>
+      <c r="O42">
+        <v>16</v>
+      </c>
+      <c r="P42">
+        <v>320</v>
+      </c>
+      <c r="Q42" t="s">
+        <v>278</v>
+      </c>
+      <c r="R42" t="s">
+        <v>289</v>
+      </c>
+      <c r="S42">
+        <v>993.04</v>
+      </c>
+      <c r="T42">
+        <v>338.57</v>
+      </c>
+      <c r="U42">
+        <v>9423</v>
+      </c>
+      <c r="V42">
+        <v>22</v>
+      </c>
+      <c r="X42">
+        <v>255</v>
+      </c>
+      <c r="Y42">
+        <v>1016</v>
+      </c>
+      <c r="Z42">
+        <v>1144</v>
+      </c>
+      <c r="AA42">
+        <v>912796</v>
+      </c>
+      <c r="AB42">
+        <v>0</v>
+      </c>
+      <c r="AC42" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD42" s="1" t="s">
+        <v>318</v>
+      </c>
+    </row>
+    <row r="43" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A43">
+        <v>1</v>
+      </c>
+      <c r="B43">
+        <v>3</v>
+      </c>
+      <c r="C43" t="s">
+        <v>173</v>
+      </c>
+      <c r="D43">
+        <v>9600</v>
+      </c>
+      <c r="E43">
+        <v>600</v>
+      </c>
+      <c r="F43" t="s">
+        <v>211</v>
+      </c>
+      <c r="G43">
+        <v>1</v>
+      </c>
+      <c r="H43">
+        <v>4</v>
+      </c>
+      <c r="I43">
+        <v>6</v>
+      </c>
+      <c r="J43">
+        <v>17</v>
+      </c>
+      <c r="K43" t="s">
+        <v>317</v>
+      </c>
+      <c r="L43">
+        <v>4</v>
+      </c>
+      <c r="M43" t="s">
+        <v>268</v>
+      </c>
+      <c r="N43" t="s">
+        <v>186</v>
+      </c>
+      <c r="O43">
+        <v>16</v>
+      </c>
+      <c r="P43">
+        <v>320</v>
+      </c>
+      <c r="Q43" t="s">
+        <v>278</v>
+      </c>
+      <c r="R43" t="s">
+        <v>298</v>
+      </c>
+      <c r="S43">
+        <v>2876.35</v>
+      </c>
+      <c r="T43">
+        <v>3315.14</v>
+      </c>
+      <c r="U43">
+        <v>6752.08</v>
+      </c>
+      <c r="V43">
+        <v>3299.83</v>
+      </c>
+      <c r="X43">
+        <v>3666.1</v>
+      </c>
+      <c r="Y43">
+        <v>3813.27</v>
+      </c>
+      <c r="Z43">
+        <v>4729.66</v>
+      </c>
+      <c r="AA43">
+        <v>2588716</v>
+      </c>
+      <c r="AB43">
+        <v>0</v>
+      </c>
+      <c r="AC43" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD43" s="1" t="s">
+        <v>319</v>
+      </c>
+      <c r="AE43" t="s">
+        <v>303</v>
+      </c>
+    </row>
+    <row r="44" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A44">
+        <v>1</v>
+      </c>
+      <c r="B44">
+        <v>3</v>
+      </c>
+      <c r="C44" t="s">
+        <v>173</v>
+      </c>
+      <c r="D44">
+        <v>19200</v>
+      </c>
+      <c r="E44">
+        <v>600</v>
+      </c>
+      <c r="F44" t="s">
+        <v>211</v>
+      </c>
+      <c r="G44">
+        <v>1</v>
+      </c>
+      <c r="H44">
+        <v>4</v>
+      </c>
+      <c r="I44">
+        <v>6</v>
+      </c>
+      <c r="J44">
+        <v>17</v>
+      </c>
+      <c r="K44" t="s">
+        <v>317</v>
+      </c>
+      <c r="L44">
+        <v>4</v>
+      </c>
+      <c r="M44" t="s">
+        <v>268</v>
+      </c>
+      <c r="N44" t="s">
+        <v>186</v>
+      </c>
+      <c r="O44">
+        <v>16</v>
+      </c>
+      <c r="P44">
+        <v>320</v>
+      </c>
+      <c r="Q44" t="s">
+        <v>278</v>
+      </c>
+      <c r="R44" t="s">
+        <v>289</v>
+      </c>
+      <c r="S44">
+        <v>983.14</v>
+      </c>
+      <c r="T44">
+        <v>432.06</v>
+      </c>
+      <c r="U44">
+        <v>10164</v>
+      </c>
+      <c r="V44">
+        <v>49</v>
+      </c>
+      <c r="X44">
+        <v>4113</v>
+      </c>
+      <c r="Y44">
+        <v>4823.99</v>
+      </c>
+      <c r="Z44">
+        <v>5045</v>
+      </c>
+      <c r="AA44">
+        <v>928837</v>
+      </c>
+      <c r="AB44">
+        <v>0</v>
+      </c>
+      <c r="AC44" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD44" s="1" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="45" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A45">
+        <v>1</v>
+      </c>
+      <c r="B45">
+        <v>3</v>
+      </c>
+      <c r="C45" t="s">
+        <v>173</v>
+      </c>
+      <c r="D45">
+        <v>4800</v>
+      </c>
+      <c r="E45">
+        <v>600</v>
+      </c>
+      <c r="F45" t="s">
+        <v>211</v>
+      </c>
+      <c r="G45">
+        <v>1</v>
+      </c>
+      <c r="H45">
+        <v>4</v>
+      </c>
+      <c r="I45">
+        <v>6</v>
+      </c>
+      <c r="J45">
+        <v>17</v>
+      </c>
+      <c r="K45" t="s">
+        <v>317</v>
+      </c>
+      <c r="L45">
+        <v>4</v>
+      </c>
+      <c r="M45" t="s">
+        <v>268</v>
+      </c>
+      <c r="N45" t="s">
+        <v>186</v>
+      </c>
+      <c r="O45">
+        <v>16</v>
+      </c>
+      <c r="P45">
+        <v>320</v>
+      </c>
+      <c r="Q45" t="s">
+        <v>278</v>
+      </c>
+      <c r="R45" t="s">
+        <v>289</v>
+      </c>
+      <c r="S45">
+        <v>985.98</v>
+      </c>
+      <c r="T45">
+        <v>267.79000000000002</v>
+      </c>
+      <c r="U45">
+        <v>13718</v>
+      </c>
+      <c r="V45">
+        <v>23</v>
+      </c>
+      <c r="X45">
+        <v>488</v>
+      </c>
+      <c r="Y45">
+        <v>645</v>
+      </c>
+      <c r="Z45">
+        <v>780</v>
+      </c>
+      <c r="AA45">
+        <v>906905</v>
+      </c>
+      <c r="AB45">
+        <v>0</v>
+      </c>
+      <c r="AC45" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD45" s="1" t="s">
+        <v>321</v>
+      </c>
+      <c r="AE45" s="6"/>
+    </row>
+    <row r="46" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A46">
+        <v>1</v>
+      </c>
+      <c r="B46">
+        <v>3</v>
+      </c>
+      <c r="C46" t="s">
+        <v>173</v>
+      </c>
+      <c r="D46">
+        <v>2400</v>
+      </c>
+      <c r="E46">
+        <v>600</v>
+      </c>
+      <c r="F46" t="s">
+        <v>211</v>
+      </c>
+      <c r="G46">
+        <v>1</v>
+      </c>
+      <c r="H46">
+        <v>4</v>
+      </c>
+      <c r="I46">
+        <v>6</v>
+      </c>
+      <c r="J46">
+        <v>17</v>
+      </c>
+      <c r="K46" t="s">
+        <v>317</v>
+      </c>
+      <c r="L46">
+        <v>4</v>
+      </c>
+      <c r="M46" t="s">
+        <v>268</v>
+      </c>
+      <c r="N46" t="s">
+        <v>186</v>
+      </c>
+      <c r="O46">
+        <v>16</v>
+      </c>
+      <c r="P46">
+        <v>320</v>
+      </c>
+      <c r="Q46" t="s">
+        <v>278</v>
+      </c>
+      <c r="R46" t="s">
+        <v>289</v>
+      </c>
+      <c r="S46">
+        <v>981.63</v>
+      </c>
+      <c r="T46">
+        <v>254.85</v>
+      </c>
+      <c r="U46">
+        <v>17960</v>
+      </c>
+      <c r="V46">
+        <v>29</v>
+      </c>
+      <c r="X46">
+        <v>479</v>
+      </c>
+      <c r="Y46">
+        <v>524</v>
+      </c>
+      <c r="Z46">
+        <v>542</v>
+      </c>
+      <c r="AA46">
+        <v>902282</v>
+      </c>
+      <c r="AB46">
+        <v>0</v>
+      </c>
+      <c r="AC46" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD46" s="1" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="47" spans="1:31" hidden="1" x14ac:dyDescent="0.2">
+      <c r="A47">
+        <v>1</v>
+      </c>
+      <c r="B47">
+        <v>3</v>
+      </c>
+      <c r="C47" t="s">
+        <v>173</v>
+      </c>
+      <c r="D47">
+        <v>1200</v>
+      </c>
+      <c r="E47">
+        <v>600</v>
+      </c>
+      <c r="F47" t="s">
+        <v>211</v>
+      </c>
+      <c r="G47">
+        <v>1</v>
+      </c>
+      <c r="H47">
+        <v>4</v>
+      </c>
+      <c r="I47">
+        <v>6</v>
+      </c>
+      <c r="J47">
+        <v>17</v>
+      </c>
+      <c r="K47" t="s">
+        <v>317</v>
+      </c>
+      <c r="L47">
+        <v>4</v>
+      </c>
+      <c r="M47" t="s">
+        <v>268</v>
+      </c>
+      <c r="N47" t="s">
+        <v>186</v>
+      </c>
+      <c r="O47">
+        <v>16</v>
+      </c>
+      <c r="P47">
+        <v>320</v>
+      </c>
+      <c r="Q47" t="s">
+        <v>278</v>
+      </c>
+      <c r="R47" t="s">
+        <v>289</v>
+      </c>
+      <c r="S47">
+        <v>984.29</v>
+      </c>
+      <c r="T47">
+        <v>125.31</v>
+      </c>
+      <c r="U47">
+        <v>10611</v>
+      </c>
+      <c r="V47">
+        <v>27</v>
+      </c>
+      <c r="X47">
+        <v>452</v>
+      </c>
+      <c r="Y47">
+        <v>490</v>
+      </c>
+      <c r="Z47">
+        <v>493</v>
+      </c>
+      <c r="AA47">
+        <v>898577</v>
+      </c>
+      <c r="AB47">
+        <v>0</v>
+      </c>
+      <c r="AC47" s="9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="AD47" s="1" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="48" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="AC48" s="5"/>
+      <c r="AD48" s="1"/>
+    </row>
+    <row r="49" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AC49" s="5"/>
+      <c r="AD49" s="1"/>
+    </row>
+    <row r="50" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A50" s="3"/>
       <c r="B50" s="3"/>
       <c r="C50" s="3"/>
@@ -4766,16 +5645,18 @@
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
       <c r="P50" s="3"/>
-      <c r="S50" s="3"/>
-      <c r="T50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
       <c r="U50" s="3"/>
       <c r="V50" s="3"/>
       <c r="W50" s="3"/>
       <c r="X50" s="3"/>
-      <c r="AA50" s="5"/>
-      <c r="AB50" s="1"/>
-    </row>
-    <row r="51" spans="1:28" x14ac:dyDescent="0.2">
+      <c r="Y50" s="3"/>
+      <c r="Z50" s="3"/>
+      <c r="AC50" s="5"/>
+      <c r="AD50" s="1"/>
+    </row>
+    <row r="51" spans="1:30" x14ac:dyDescent="0.2">
       <c r="A51" s="3"/>
       <c r="B51" s="3"/>
       <c r="C51" s="3"/>
@@ -4792,58 +5673,71 @@
       <c r="N51" s="3"/>
       <c r="O51" s="3"/>
       <c r="P51" s="3"/>
-      <c r="S51" s="3"/>
-      <c r="T51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
       <c r="U51" s="3"/>
-      <c r="AA51" s="5"/>
-      <c r="AB51" s="1"/>
-    </row>
-    <row r="52" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="T52" s="3"/>
-      <c r="AA52" s="5"/>
-      <c r="AB52" s="1"/>
-    </row>
-    <row r="53" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="AA53" s="5"/>
-      <c r="AB53" s="1"/>
-    </row>
-    <row r="54" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="T54" s="3"/>
-      <c r="AA54" s="5"/>
-      <c r="AB54" s="1"/>
-    </row>
-    <row r="55" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="T55" s="3"/>
-      <c r="AA55" s="5"/>
-      <c r="AB55" s="1"/>
-    </row>
-    <row r="56" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="T56" s="3"/>
-      <c r="AA56" s="5"/>
-      <c r="AB56" s="1"/>
-    </row>
-    <row r="57" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="T57" s="3"/>
-      <c r="AA57" s="5"/>
-      <c r="AB57" s="1"/>
-    </row>
-    <row r="58" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="T58" s="3"/>
-      <c r="AA58" s="5"/>
-      <c r="AB58" s="1"/>
-    </row>
-    <row r="59" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="T59" s="3"/>
-      <c r="AA59" s="5"/>
-      <c r="AB59" s="1"/>
-    </row>
-    <row r="60" spans="1:28" x14ac:dyDescent="0.2">
-      <c r="T60" s="3"/>
-      <c r="AA60" s="5"/>
-      <c r="AB60" s="1"/>
+      <c r="V51" s="3"/>
+      <c r="W51" s="3"/>
+      <c r="AC51" s="5"/>
+      <c r="AD51" s="1"/>
+    </row>
+    <row r="52" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V52" s="3"/>
+      <c r="AC52" s="5"/>
+      <c r="AD52" s="1"/>
+    </row>
+    <row r="53" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="AC53" s="5"/>
+      <c r="AD53" s="1"/>
+    </row>
+    <row r="54" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V54" s="3"/>
+      <c r="AC54" s="5"/>
+      <c r="AD54" s="1"/>
+    </row>
+    <row r="55" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V55" s="3"/>
+      <c r="AC55" s="5"/>
+      <c r="AD55" s="1"/>
+    </row>
+    <row r="56" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V56" s="3"/>
+      <c r="AC56" s="5"/>
+      <c r="AD56" s="1"/>
+    </row>
+    <row r="57" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V57" s="3"/>
+      <c r="AC57" s="5"/>
+      <c r="AD57" s="1"/>
+    </row>
+    <row r="58" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V58" s="3"/>
+      <c r="AC58" s="5"/>
+      <c r="AD58" s="1"/>
+    </row>
+    <row r="59" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V59" s="3"/>
+      <c r="AC59" s="5"/>
+      <c r="AD59" s="1"/>
+    </row>
+    <row r="60" spans="1:30" x14ac:dyDescent="0.2">
+      <c r="V60" s="3"/>
+      <c r="AC60" s="5"/>
+      <c r="AD60" s="1"/>
     </row>
   </sheetData>
-  <autoFilter ref="A2:AC42" xr:uid="{0BCD43CD-D15C-C44C-860E-27B2AEF78201}"/>
+  <autoFilter ref="A2:AE47" xr:uid="{0BCD43CD-D15C-C44C-860E-27B2AEF78201}">
+    <filterColumn colId="3">
+      <filters>
+        <filter val="2400"/>
+      </filters>
+    </filterColumn>
+    <filterColumn colId="17">
+      <filters>
+        <filter val="https 1.1"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <phoneticPr fontId="4" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>